<commit_message>
lagt till halve 014.
</commit_message>
<xml_diff>
--- a/Rawdata/riptransekter helags 2018.xlsx
+++ b/Rawdata/riptransekter helags 2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="460" windowWidth="25600" windowHeight="14120" xr2:uid="{731D7839-4CAB-374B-BEA5-3406519CB6C1}"/>
+    <workbookView xWindow="7420" yWindow="460" windowWidth="25600" windowHeight="14120" xr2:uid="{731D7839-4CAB-374B-BEA5-3406519CB6C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1977" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2038" uniqueCount="417">
   <si>
     <t>vinkel</t>
   </si>
@@ -1257,6 +1257,24 @@
   </si>
   <si>
     <t>ljusbrin, oformlig</t>
+  </si>
+  <si>
+    <t>skare + 1 cm nysnö + 2 cm nysnö under dagen</t>
+  </si>
+  <si>
+    <t>mulet, vind 3 m/s, 0 till -2 grader</t>
+  </si>
+  <si>
+    <t>C till fast, färsk</t>
+  </si>
+  <si>
+    <t>ljusbrun, mjuk</t>
+  </si>
+  <si>
+    <t>blandat färskt och gammalt</t>
+  </si>
+  <si>
+    <t>relatiivt mycket snö och lite barmark på sträcka 1. Få buskar och lite ljung.</t>
   </si>
 </sst>
 </file>
@@ -1614,8 +1632,8 @@
   <dimension ref="A1:Z438"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N166" sqref="N166:N167"/>
+      <pane ySplit="1" topLeftCell="A243" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A250" sqref="A250:F250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9439,7 +9457,15 @@
       <c r="E232" s="2">
         <v>43216.280555555553</v>
       </c>
-      <c r="F232" s="2"/>
+      <c r="F232" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="N232" t="s">
+        <v>412</v>
+      </c>
+      <c r="O232" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="233" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
@@ -9457,97 +9483,163 @@
       <c r="E233" s="2">
         <v>43216.380555555559</v>
       </c>
-      <c r="F233" s="2"/>
+      <c r="F233" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="234" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>121</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>29</v>
+        <v>118</v>
       </c>
       <c r="C234" s="3">
-        <v>6978221351667</v>
+        <v>6978333351234</v>
       </c>
       <c r="D234" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E234" s="2">
-        <v>43216.390972222223</v>
-      </c>
-      <c r="F234" s="2"/>
+        <v>43216.380555555559</v>
+      </c>
+      <c r="F234" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G234">
+        <v>156</v>
+      </c>
+      <c r="H234">
+        <v>102</v>
+      </c>
+      <c r="I234" t="s">
+        <v>156</v>
+      </c>
+      <c r="L234">
+        <v>1</v>
+      </c>
     </row>
     <row r="235" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>121</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="C235" s="3">
-        <v>6977654353487</v>
+        <v>6978333351234</v>
       </c>
       <c r="D235" t="s">
-        <v>260</v>
+        <v>287</v>
       </c>
       <c r="E235" s="2">
-        <v>43216.40625</v>
-      </c>
-      <c r="F235" s="2"/>
+        <v>43216.380555555559</v>
+      </c>
+      <c r="F235" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G235">
+        <v>102</v>
+      </c>
+      <c r="H235">
+        <v>275</v>
+      </c>
+      <c r="I235" t="s">
+        <v>156</v>
+      </c>
+      <c r="L235">
+        <v>1</v>
+      </c>
     </row>
     <row r="236" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>121</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C236" s="3">
-        <v>6977528353996</v>
+        <v>6978221351667</v>
       </c>
       <c r="D236" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E236" s="2">
-        <v>43216.413888888892</v>
-      </c>
-      <c r="F236" s="2"/>
+        <v>43216.390972222223</v>
+      </c>
+      <c r="F236" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G236">
+        <v>167</v>
+      </c>
+      <c r="H236">
+        <v>283</v>
+      </c>
+      <c r="I236" t="s">
+        <v>156</v>
+      </c>
+      <c r="L236">
+        <v>1</v>
+      </c>
     </row>
     <row r="237" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>121</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C237" s="3">
-        <v>6977484354587</v>
+        <v>6977654353487</v>
       </c>
       <c r="D237" t="s">
-        <v>208</v>
+        <v>260</v>
       </c>
       <c r="E237" s="2">
-        <v>43216.42291666667</v>
-      </c>
-      <c r="F237" s="2"/>
+        <v>43216.40625</v>
+      </c>
+      <c r="F237" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J237" t="s">
+        <v>15</v>
+      </c>
+      <c r="L237">
+        <v>1</v>
+      </c>
+      <c r="M237" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="238" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>121</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="C238" s="3">
-        <v>6977493354708</v>
+        <v>6977528353996</v>
       </c>
       <c r="D238" t="s">
-        <v>245</v>
+        <v>290</v>
       </c>
       <c r="E238" s="2">
-        <v>43216.426388888889</v>
-      </c>
-      <c r="F238" s="2"/>
+        <v>43216.413888888892</v>
+      </c>
+      <c r="F238" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J238" t="s">
+        <v>10</v>
+      </c>
+      <c r="L238">
+        <v>1</v>
+      </c>
+      <c r="M238" t="s">
+        <v>414</v>
+      </c>
       <c r="W238" s="3"/>
       <c r="Y238" s="2"/>
       <c r="Z238" s="2"/>
@@ -9557,16 +9649,28 @@
         <v>121</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C239" s="3">
-        <v>6977510354981</v>
+        <v>6977484354587</v>
       </c>
       <c r="D239" t="s">
-        <v>272</v>
+        <v>208</v>
       </c>
       <c r="E239" s="2">
-        <v>43216.430555555555</v>
+        <v>43216.42291666667</v>
+      </c>
+      <c r="F239" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J239" t="s">
+        <v>10</v>
+      </c>
+      <c r="L239">
+        <v>1</v>
+      </c>
+      <c r="M239" t="s">
+        <v>166</v>
       </c>
       <c r="W239" s="3"/>
       <c r="Y239" s="2"/>
@@ -9577,16 +9681,25 @@
         <v>121</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C240" s="3">
-        <v>6977503355128</v>
+        <v>6977493354708</v>
       </c>
       <c r="D240" t="s">
-        <v>291</v>
+        <v>245</v>
       </c>
       <c r="E240" s="2">
-        <v>43216.431944444441</v>
+        <v>43216.426388888889</v>
+      </c>
+      <c r="F240" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J240" t="s">
+        <v>15</v>
+      </c>
+      <c r="L240">
+        <v>1</v>
       </c>
       <c r="W240" s="3"/>
       <c r="Y240" s="2"/>
@@ -9597,18 +9710,35 @@
         <v>121</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="C241" s="3">
-        <v>6977550355108</v>
+        <v>6977510354981</v>
       </c>
       <c r="D241" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="E241" s="2">
-        <v>43216.442361111112</v>
-      </c>
-      <c r="F241" s="2"/>
+        <v>43216.430555555555</v>
+      </c>
+      <c r="F241" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G241">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="H241">
+        <v>270</v>
+      </c>
+      <c r="J241" t="s">
+        <v>15</v>
+      </c>
+      <c r="L241">
+        <v>20</v>
+      </c>
+      <c r="M241" t="s">
+        <v>415</v>
+      </c>
       <c r="W241" s="3"/>
       <c r="Y241" s="2"/>
       <c r="Z241" s="2"/>
@@ -9618,18 +9748,23 @@
         <v>121</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C242" s="3">
-        <v>6977799355071</v>
+        <v>6977503355128</v>
       </c>
       <c r="D242" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E242" s="2">
-        <v>43216.448611111111</v>
-      </c>
-      <c r="F242" s="2"/>
+        <v>43216.431944444441</v>
+      </c>
+      <c r="F242" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M242" t="s">
+        <v>416</v>
+      </c>
       <c r="W242" s="3"/>
       <c r="Y242" s="2"/>
       <c r="Z242" s="2"/>
@@ -9639,18 +9774,32 @@
         <v>121</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C243" s="3">
-        <v>6978993354678</v>
+        <v>6977550355108</v>
       </c>
       <c r="D243" t="s">
-        <v>372</v>
+        <v>292</v>
       </c>
       <c r="E243" s="2">
-        <v>43216.490277777775</v>
-      </c>
-      <c r="F243" s="2"/>
+        <v>43216.442361111112</v>
+      </c>
+      <c r="F243" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G243">
+        <v>230</v>
+      </c>
+      <c r="H243">
+        <v>276</v>
+      </c>
+      <c r="I243" t="s">
+        <v>156</v>
+      </c>
+      <c r="L243">
+        <v>1</v>
+      </c>
       <c r="W243" s="3"/>
       <c r="Y243" s="2"/>
       <c r="Z243" s="2"/>
@@ -9660,18 +9809,32 @@
         <v>121</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="C244" s="3">
-        <v>6980084354118</v>
+        <v>6977550355108</v>
       </c>
       <c r="D244" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
       <c r="E244" s="2">
-        <v>43216.490277777775</v>
-      </c>
-      <c r="F244" s="2"/>
+        <v>43216.442361111112</v>
+      </c>
+      <c r="F244" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G244">
+        <v>247</v>
+      </c>
+      <c r="H244">
+        <v>189</v>
+      </c>
+      <c r="I244" t="s">
+        <v>156</v>
+      </c>
+      <c r="L244">
+        <v>1</v>
+      </c>
       <c r="W244" s="3"/>
       <c r="Y244" s="2"/>
       <c r="Z244" s="2"/>
@@ -9681,18 +9844,35 @@
         <v>121</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C245" s="3">
-        <v>6981270353841</v>
+        <v>6977799355071</v>
       </c>
       <c r="D245" t="s">
-        <v>271</v>
+        <v>292</v>
       </c>
       <c r="E245" s="2">
-        <v>43216.509027777778</v>
-      </c>
-      <c r="F245" s="2"/>
+        <v>43216.448611111111</v>
+      </c>
+      <c r="F245" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G245">
+        <v>164</v>
+      </c>
+      <c r="H245">
+        <v>20</v>
+      </c>
+      <c r="I245" t="s">
+        <v>154</v>
+      </c>
+      <c r="J245" t="s">
+        <v>15</v>
+      </c>
+      <c r="L245">
+        <v>1</v>
+      </c>
       <c r="W245" s="3"/>
       <c r="Y245" s="2"/>
       <c r="Z245" s="2"/>
@@ -9702,18 +9882,35 @@
         <v>121</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C246" s="3">
-        <v>6980911353777</v>
+        <v>6978993354678</v>
       </c>
       <c r="D246" t="s">
-        <v>260</v>
+        <v>372</v>
       </c>
       <c r="E246" s="2">
-        <v>43216.606249999997</v>
-      </c>
-      <c r="F246" s="2"/>
+        <v>43216.490277777775</v>
+      </c>
+      <c r="F246" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G246">
+        <v>63</v>
+      </c>
+      <c r="H246">
+        <v>284</v>
+      </c>
+      <c r="I246" t="s">
+        <v>154</v>
+      </c>
+      <c r="J246" t="s">
+        <v>10</v>
+      </c>
+      <c r="L246">
+        <v>2</v>
+      </c>
       <c r="W246" s="3"/>
       <c r="Y246" s="2"/>
       <c r="Z246" s="2"/>
@@ -9723,18 +9920,32 @@
         <v>121</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="C247" s="3">
-        <v>6980531353694</v>
+        <v>6978993354678</v>
       </c>
       <c r="D247" t="s">
-        <v>218</v>
+        <v>372</v>
       </c>
       <c r="E247" s="2">
-        <v>43216.615277777775</v>
-      </c>
-      <c r="F247" s="2"/>
+        <v>43216.490277777775</v>
+      </c>
+      <c r="F247" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G247">
+        <v>134</v>
+      </c>
+      <c r="H247">
+        <v>195</v>
+      </c>
+      <c r="I247" t="s">
+        <v>156</v>
+      </c>
+      <c r="L247">
+        <v>1</v>
+      </c>
       <c r="W247" s="3"/>
       <c r="Y247" s="2"/>
       <c r="Z247" s="2"/>
@@ -9744,18 +9955,35 @@
         <v>121</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="C248" s="3">
-        <v>6980411353676</v>
+        <v>6980084354118</v>
       </c>
       <c r="D248" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="E248" s="2">
-        <v>43216.620138888888</v>
-      </c>
-      <c r="F248" s="2"/>
+        <v>43216.490277777775</v>
+      </c>
+      <c r="F248" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G248">
+        <v>112</v>
+      </c>
+      <c r="H248">
+        <v>18</v>
+      </c>
+      <c r="I248" t="s">
+        <v>153</v>
+      </c>
+      <c r="J248" t="s">
+        <v>10</v>
+      </c>
+      <c r="L248">
+        <v>1</v>
+      </c>
       <c r="W248" s="3"/>
       <c r="Y248" s="2"/>
       <c r="Z248" s="2"/>
@@ -9765,18 +9993,20 @@
         <v>121</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="C249" s="3">
-        <v>6980373353646</v>
+        <v>6980084354118</v>
       </c>
       <c r="D249" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="E249" s="2">
-        <v>43216.622916666667</v>
-      </c>
-      <c r="F249" s="2"/>
+        <v>43216.490277777775</v>
+      </c>
+      <c r="F249" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="W249" s="3"/>
       <c r="Y249" s="2"/>
       <c r="Z249" s="2"/>
@@ -9786,18 +10016,20 @@
         <v>121</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C250" s="3">
-        <v>6980103353507</v>
+        <v>6980084354118</v>
       </c>
       <c r="D250" t="s">
-        <v>182</v>
+        <v>281</v>
       </c>
       <c r="E250" s="2">
-        <v>43216.62777777778</v>
-      </c>
-      <c r="F250" s="2"/>
+        <v>43216.490277777775</v>
+      </c>
+      <c r="F250" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="W250" s="3"/>
       <c r="Y250" s="2"/>
       <c r="Z250" s="2"/>
@@ -9807,16 +10039,16 @@
         <v>121</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C251" s="3">
-        <v>6979753353371</v>
+        <v>6981270353841</v>
       </c>
       <c r="D251" t="s">
-        <v>294</v>
+        <v>271</v>
       </c>
       <c r="E251" s="2">
-        <v>43216.634722222225</v>
+        <v>43216.509027777778</v>
       </c>
       <c r="F251" s="2"/>
       <c r="W251" s="3"/>
@@ -9828,16 +10060,16 @@
         <v>121</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="C252" s="3">
-        <v>6979459353143</v>
+        <v>6980911353777</v>
       </c>
       <c r="D252" t="s">
-        <v>295</v>
+        <v>260</v>
       </c>
       <c r="E252" s="2">
-        <v>43216.640972222223</v>
+        <v>43216.606249999997</v>
       </c>
       <c r="F252" s="2"/>
       <c r="W252" s="3"/>
@@ -9849,16 +10081,16 @@
         <v>121</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="C253" s="3">
-        <v>6979305353040</v>
+        <v>6980531353694</v>
       </c>
       <c r="D253" t="s">
-        <v>296</v>
+        <v>218</v>
       </c>
       <c r="E253" s="2">
-        <v>43216.645138888889</v>
+        <v>43216.615277777775</v>
       </c>
       <c r="F253" s="2"/>
       <c r="W253" s="3"/>
@@ -9870,16 +10102,16 @@
         <v>121</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>120</v>
+        <v>51</v>
       </c>
       <c r="C254" s="3">
-        <v>6979202352873</v>
+        <v>6980411353676</v>
       </c>
       <c r="D254" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E254" s="2">
-        <v>43216.650694444441</v>
+        <v>43216.620138888888</v>
       </c>
       <c r="F254" s="2"/>
       <c r="W254" s="3"/>
@@ -9891,16 +10123,16 @@
         <v>121</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C255" s="3">
-        <v>6978426351327</v>
+        <v>6980373353646</v>
       </c>
       <c r="D255" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="E255" s="2">
-        <v>43216.677083333336</v>
+        <v>43216.622916666667</v>
       </c>
       <c r="F255" s="2"/>
       <c r="W255" s="3"/>
@@ -9909,19 +10141,19 @@
     </row>
     <row r="256" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="C256" s="3">
-        <v>6982302355715</v>
+        <v>6980103353507</v>
       </c>
       <c r="D256" t="s">
-        <v>299</v>
+        <v>182</v>
       </c>
       <c r="E256" s="2">
-        <v>43217.268750000003</v>
+        <v>43216.62777777778</v>
       </c>
       <c r="F256" s="2"/>
       <c r="W256" s="3"/>
@@ -9930,19 +10162,19 @@
     </row>
     <row r="257" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="C257" s="3">
-        <v>6983090356519</v>
+        <v>6979753353371</v>
       </c>
       <c r="D257" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="E257" s="2">
-        <v>43217.288194444445</v>
+        <v>43216.634722222225</v>
       </c>
       <c r="F257" s="2"/>
       <c r="W257" s="3"/>
@@ -9951,19 +10183,19 @@
     </row>
     <row r="258" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="C258" s="3">
-        <v>6983032356674</v>
+        <v>6979459353143</v>
       </c>
       <c r="D258" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="E258" s="2">
-        <v>43217.292361111111</v>
+        <v>43216.640972222223</v>
       </c>
       <c r="F258" s="2"/>
       <c r="W258" s="3"/>
@@ -9972,19 +10204,19 @@
     </row>
     <row r="259" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>116</v>
+        <v>51</v>
       </c>
       <c r="C259" s="3">
-        <v>6982991356782</v>
+        <v>6979305353040</v>
       </c>
       <c r="D259" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E259" s="2">
-        <v>43217.294444444444</v>
+        <v>43216.645138888889</v>
       </c>
       <c r="F259" s="2"/>
       <c r="W259" s="3"/>
@@ -9993,19 +10225,19 @@
     </row>
     <row r="260" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="C260" s="3">
-        <v>6982916356948</v>
+        <v>6979202352873</v>
       </c>
       <c r="D260" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="E260" s="2">
-        <v>43217.296527777777</v>
+        <v>43216.650694444441</v>
       </c>
       <c r="F260" s="2"/>
       <c r="W260" s="3"/>
@@ -10014,19 +10246,19 @@
     </row>
     <row r="261" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C261" s="3">
-        <v>6982928357079</v>
+        <v>6978426351327</v>
       </c>
       <c r="D261" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="E261" s="2">
-        <v>43217.298611111109</v>
+        <v>43216.677083333336</v>
       </c>
       <c r="F261" s="2"/>
       <c r="W261" s="3"/>
@@ -10038,16 +10270,16 @@
         <v>125</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="C262" s="3">
-        <v>6982958357172</v>
+        <v>6982302355715</v>
       </c>
       <c r="D262" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E262" s="2">
-        <v>43217.3</v>
+        <v>43217.268750000003</v>
       </c>
       <c r="F262" s="2"/>
       <c r="W262" s="3"/>
@@ -10059,16 +10291,16 @@
         <v>125</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>51</v>
+        <v>122</v>
       </c>
       <c r="C263" s="3">
-        <v>6982732357448</v>
+        <v>6983090356519</v>
       </c>
       <c r="D263" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E263" s="2">
-        <v>43217.305555555555</v>
+        <v>43217.288194444445</v>
       </c>
       <c r="F263" s="2"/>
       <c r="W263" s="3"/>
@@ -10080,16 +10312,16 @@
         <v>125</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="C264" s="3">
-        <v>6982630357699</v>
+        <v>6983032356674</v>
       </c>
       <c r="D264" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="E264" s="2">
-        <v>43217.30972222222</v>
+        <v>43217.292361111111</v>
       </c>
     </row>
     <row r="265" spans="1:26" x14ac:dyDescent="0.2">
@@ -10097,16 +10329,16 @@
         <v>125</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
       <c r="C265" s="3">
-        <v>6982183358919</v>
+        <v>6982991356782</v>
       </c>
       <c r="D265" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E265" s="2">
-        <v>43217.379861111112</v>
+        <v>43217.294444444444</v>
       </c>
     </row>
     <row r="266" spans="1:26" x14ac:dyDescent="0.2">
@@ -10114,16 +10346,16 @@
         <v>125</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C266" s="3">
-        <v>6982114359058</v>
+        <v>6982916356948</v>
       </c>
       <c r="D266" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="E266" s="2">
-        <v>43217.384027777778</v>
+        <v>43217.296527777777</v>
       </c>
       <c r="F266" s="2"/>
     </row>
@@ -10132,16 +10364,16 @@
         <v>125</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="C267" s="3">
-        <v>6982006359291</v>
+        <v>6982928357079</v>
       </c>
       <c r="D267" t="s">
-        <v>240</v>
+        <v>303</v>
       </c>
       <c r="E267" s="2">
-        <v>43217.388888888891</v>
+        <v>43217.298611111109</v>
       </c>
       <c r="F267" s="2"/>
     </row>
@@ -10150,16 +10382,16 @@
         <v>125</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="C268" s="3">
-        <v>6981940359461</v>
+        <v>6982958357172</v>
       </c>
       <c r="D268" t="s">
-        <v>239</v>
+        <v>304</v>
       </c>
       <c r="E268" s="2">
-        <v>43217.392361111109</v>
+        <v>43217.3</v>
       </c>
       <c r="F268" s="2"/>
     </row>
@@ -10171,13 +10403,13 @@
         <v>51</v>
       </c>
       <c r="C269" s="3">
-        <v>6981870359749</v>
+        <v>6982732357448</v>
       </c>
       <c r="D269" t="s">
-        <v>255</v>
+        <v>305</v>
       </c>
       <c r="E269" s="2">
-        <v>43217.4</v>
+        <v>43217.305555555555</v>
       </c>
       <c r="F269" s="2"/>
     </row>
@@ -10186,16 +10418,16 @@
         <v>125</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="C270" s="3">
-        <v>6981921360308</v>
+        <v>6982630357699</v>
       </c>
       <c r="D270" t="s">
-        <v>214</v>
+        <v>292</v>
       </c>
       <c r="E270" s="2">
-        <v>43217.407638888886</v>
+        <v>43217.30972222222</v>
       </c>
       <c r="F270" s="2"/>
     </row>
@@ -10204,16 +10436,16 @@
         <v>125</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C271" s="3">
-        <v>6983945359739</v>
+        <v>6982183358919</v>
       </c>
       <c r="D271" t="s">
-        <v>221</v>
+        <v>306</v>
       </c>
       <c r="E271" s="2">
-        <v>43217.45208333333</v>
+        <v>43217.379861111112</v>
       </c>
       <c r="F271" s="2"/>
     </row>
@@ -10222,16 +10454,16 @@
         <v>125</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>94</v>
+        <v>35</v>
       </c>
       <c r="C272" s="3">
-        <v>6984478359678</v>
+        <v>6982114359058</v>
       </c>
       <c r="D272" t="s">
-        <v>199</v>
+        <v>307</v>
       </c>
       <c r="E272" s="2">
-        <v>43217.461805555555</v>
+        <v>43217.384027777778</v>
       </c>
       <c r="F272" s="2"/>
     </row>
@@ -10240,16 +10472,16 @@
         <v>125</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C273" s="3">
-        <v>6984553359647</v>
+        <v>6982006359291</v>
       </c>
       <c r="D273" t="s">
-        <v>199</v>
+        <v>240</v>
       </c>
       <c r="E273" s="2">
-        <v>43217.465277777781</v>
+        <v>43217.388888888891</v>
       </c>
       <c r="F273" s="2"/>
     </row>
@@ -10258,16 +10490,16 @@
         <v>125</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="C274" s="3">
-        <v>6985096359518</v>
+        <v>6981940359461</v>
       </c>
       <c r="D274" t="s">
-        <v>308</v>
+        <v>239</v>
       </c>
       <c r="E274" s="2">
-        <v>43217.475694444445</v>
+        <v>43217.392361111109</v>
       </c>
       <c r="F274" s="2"/>
       <c r="O274" s="2"/>
@@ -10277,16 +10509,16 @@
         <v>125</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="C275" s="3">
-        <v>6985863359293</v>
+        <v>6981870359749</v>
       </c>
       <c r="D275" t="s">
-        <v>309</v>
+        <v>255</v>
       </c>
       <c r="E275" s="2">
-        <v>43217.490972222222</v>
+        <v>43217.4</v>
       </c>
       <c r="F275" s="2"/>
       <c r="O275" s="2"/>
@@ -10296,16 +10528,16 @@
         <v>125</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>124</v>
+        <v>68</v>
       </c>
       <c r="C276" s="3">
-        <v>6985409358759</v>
+        <v>6981921360308</v>
       </c>
       <c r="D276" t="s">
-        <v>266</v>
+        <v>214</v>
       </c>
       <c r="E276" s="2">
-        <v>43217.513194444444</v>
+        <v>43217.407638888886</v>
       </c>
       <c r="F276" s="2"/>
       <c r="O276" s="2"/>
@@ -10315,16 +10547,16 @@
         <v>125</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="C277" s="3">
-        <v>6985041358323</v>
+        <v>6983945359739</v>
       </c>
       <c r="D277" t="s">
-        <v>278</v>
+        <v>221</v>
       </c>
       <c r="E277" s="2">
-        <v>43217.520138888889</v>
+        <v>43217.45208333333</v>
       </c>
       <c r="F277" s="2"/>
       <c r="O277" s="2"/>
@@ -10334,16 +10566,16 @@
         <v>125</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="C278" s="3">
-        <v>6983184356513</v>
+        <v>6984478359678</v>
       </c>
       <c r="D278" t="s">
-        <v>310</v>
+        <v>199</v>
       </c>
       <c r="E278" s="2">
-        <v>43217.554166666669</v>
+        <v>43217.461805555555</v>
       </c>
       <c r="F278" s="2"/>
       <c r="N278" s="2"/>
@@ -10351,19 +10583,19 @@
     </row>
     <row r="279" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="C279" s="3">
-        <v>7005963362616</v>
+        <v>6984553359647</v>
       </c>
       <c r="D279" t="s">
-        <v>323</v>
+        <v>199</v>
       </c>
       <c r="E279" s="2">
-        <v>43220.375</v>
+        <v>43217.465277777781</v>
       </c>
       <c r="F279" s="2"/>
       <c r="N279" s="2"/>
@@ -10371,19 +10603,19 @@
     </row>
     <row r="280" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>67</v>
+        <v>120</v>
       </c>
       <c r="C280" s="3">
-        <v>7005930362243</v>
+        <v>6985096359518</v>
       </c>
       <c r="D280" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E280" s="2">
-        <v>43220.384027777778</v>
+        <v>43217.475694444445</v>
       </c>
       <c r="F280" s="2"/>
       <c r="N280" s="2"/>
@@ -10391,19 +10623,19 @@
     </row>
     <row r="281" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="C281" s="3">
-        <v>7005887361616</v>
+        <v>6985863359293</v>
       </c>
       <c r="D281" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E281" s="2">
-        <v>43220.38958333333</v>
+        <v>43217.490972222222</v>
       </c>
       <c r="F281" s="2"/>
       <c r="N281" s="2"/>
@@ -10411,19 +10643,19 @@
     </row>
     <row r="282" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
       <c r="C282" s="3">
-        <v>7005948361408</v>
+        <v>6985409358759</v>
       </c>
       <c r="D282" t="s">
-        <v>313</v>
+        <v>266</v>
       </c>
       <c r="E282" s="2">
-        <v>43220.393055555556</v>
+        <v>43217.513194444444</v>
       </c>
       <c r="F282" s="2"/>
       <c r="N282" s="2"/>
@@ -10431,19 +10663,19 @@
     </row>
     <row r="283" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C283" s="3">
-        <v>7006091360439</v>
+        <v>6985041358323</v>
       </c>
       <c r="D283" t="s">
-        <v>219</v>
+        <v>278</v>
       </c>
       <c r="E283" s="2">
-        <v>43220.415277777778</v>
+        <v>43217.520138888889</v>
       </c>
       <c r="F283" s="2"/>
       <c r="N283" s="2"/>
@@ -10451,19 +10683,19 @@
     </row>
     <row r="284" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="C284" s="3">
-        <v>7006105360299</v>
+        <v>6983184356513</v>
       </c>
       <c r="D284" t="s">
-        <v>247</v>
+        <v>310</v>
       </c>
       <c r="E284" s="2">
-        <v>43220.418055555558</v>
+        <v>43217.554166666669</v>
       </c>
       <c r="F284" s="2"/>
       <c r="N284" s="2"/>
@@ -10474,16 +10706,16 @@
         <v>145</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>72</v>
+        <v>126</v>
       </c>
       <c r="C285" s="3">
-        <v>7006130360148</v>
+        <v>7005963362616</v>
       </c>
       <c r="D285" t="s">
-        <v>253</v>
+        <v>323</v>
       </c>
       <c r="E285" s="2">
-        <v>43220.422222222223</v>
+        <v>43220.375</v>
       </c>
       <c r="F285" s="2"/>
       <c r="N285" s="2"/>
@@ -10494,16 +10726,16 @@
         <v>145</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C286" s="3">
-        <v>7006133360128</v>
+        <v>7005930362243</v>
       </c>
       <c r="D286" t="s">
-        <v>253</v>
+        <v>311</v>
       </c>
       <c r="E286" s="2">
-        <v>43220.424305555556</v>
+        <v>43220.384027777778</v>
       </c>
       <c r="F286" s="2"/>
       <c r="N286" s="2"/>
@@ -10514,16 +10746,16 @@
         <v>145</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>74</v>
+        <v>116</v>
       </c>
       <c r="C287" s="3">
-        <v>7006146360075</v>
+        <v>7005887361616</v>
       </c>
       <c r="D287" t="s">
-        <v>225</v>
+        <v>312</v>
       </c>
       <c r="E287" s="2">
-        <v>43220.425694444442</v>
+        <v>43220.38958333333</v>
       </c>
       <c r="F287" s="2"/>
       <c r="N287" s="2"/>
@@ -10534,16 +10766,16 @@
         <v>145</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="C288" s="3">
-        <v>7006171360032</v>
+        <v>7005948361408</v>
       </c>
       <c r="D288" t="s">
-        <v>294</v>
+        <v>313</v>
       </c>
       <c r="E288" s="2">
-        <v>43220.427777777775</v>
+        <v>43220.393055555556</v>
       </c>
       <c r="F288" s="2"/>
       <c r="N288" s="2"/>
@@ -10554,16 +10786,16 @@
         <v>145</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="C289" s="3">
-        <v>7006203359711</v>
+        <v>7006091360439</v>
       </c>
       <c r="D289" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="E289" s="2">
-        <v>43220.432638888888</v>
+        <v>43220.415277777778</v>
       </c>
       <c r="F289" s="2"/>
       <c r="N289" s="2"/>
@@ -10574,16 +10806,16 @@
         <v>145</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="C290" s="3">
-        <v>7006211359605</v>
+        <v>7006105360299</v>
       </c>
       <c r="D290" t="s">
-        <v>217</v>
+        <v>247</v>
       </c>
       <c r="E290" s="2">
-        <v>43220.43472222222</v>
+        <v>43220.418055555558</v>
       </c>
       <c r="F290" s="2"/>
       <c r="N290" s="2"/>
@@ -10594,16 +10826,16 @@
         <v>145</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C291" s="3">
-        <v>7006143359330</v>
+        <v>7006130360148</v>
       </c>
       <c r="D291" t="s">
-        <v>314</v>
+        <v>253</v>
       </c>
       <c r="E291" s="2">
-        <v>43220.4375</v>
+        <v>43220.422222222223</v>
       </c>
       <c r="F291" s="2"/>
       <c r="N291" s="2"/>
@@ -10614,16 +10846,16 @@
         <v>145</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="C292" s="3">
-        <v>7006114359146</v>
+        <v>7006133360128</v>
       </c>
       <c r="D292" t="s">
-        <v>315</v>
+        <v>253</v>
       </c>
       <c r="E292" s="2">
-        <v>43220.441666666666</v>
+        <v>43220.424305555556</v>
       </c>
       <c r="F292" s="2"/>
       <c r="N292" s="2"/>
@@ -10634,16 +10866,16 @@
         <v>145</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C293" s="3">
-        <v>7006105359105</v>
+        <v>7006146360075</v>
       </c>
       <c r="D293" t="s">
-        <v>307</v>
+        <v>225</v>
       </c>
       <c r="E293" s="2">
-        <v>43220.443055555559</v>
+        <v>43220.425694444442</v>
       </c>
       <c r="F293" s="2"/>
       <c r="N293" s="2"/>
@@ -10654,16 +10886,16 @@
         <v>145</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="C294" s="3">
-        <v>7006097359055</v>
+        <v>7006171360032</v>
       </c>
       <c r="D294" t="s">
-        <v>273</v>
+        <v>294</v>
       </c>
       <c r="E294" s="2">
-        <v>43220.445138888892</v>
+        <v>43220.427777777775</v>
       </c>
       <c r="F294" s="2"/>
       <c r="N294" s="2"/>
@@ -10674,16 +10906,16 @@
         <v>145</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="C295" s="3">
-        <v>7006092358975</v>
+        <v>7006203359711</v>
       </c>
       <c r="D295" t="s">
-        <v>307</v>
+        <v>233</v>
       </c>
       <c r="E295" s="2">
-        <v>43220.448611111111</v>
+        <v>43220.432638888888</v>
       </c>
       <c r="F295" s="2"/>
       <c r="N295" s="2"/>
@@ -10694,16 +10926,16 @@
         <v>145</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C296" s="3">
-        <v>7006069358719</v>
+        <v>7006211359605</v>
       </c>
       <c r="D296" t="s">
-        <v>315</v>
+        <v>217</v>
       </c>
       <c r="E296" s="2">
-        <v>43220.45208333333</v>
+        <v>43220.43472222222</v>
       </c>
       <c r="F296" s="2"/>
       <c r="N296" s="2"/>
@@ -10714,16 +10946,16 @@
         <v>145</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C297" s="3">
-        <v>7006070358639</v>
+        <v>7006143359330</v>
       </c>
       <c r="D297" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="E297" s="2">
-        <v>43220.45416666667</v>
+        <v>43220.4375</v>
       </c>
       <c r="F297" s="2"/>
       <c r="N297" s="2"/>
@@ -10733,16 +10965,16 @@
         <v>145</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="C298" s="3">
-        <v>7006048358564</v>
+        <v>7006114359146</v>
       </c>
       <c r="D298" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="E298" s="2">
-        <v>43220.455555555556</v>
+        <v>43220.441666666666</v>
       </c>
       <c r="F298" s="2"/>
       <c r="N298" s="2"/>
@@ -10752,16 +10984,16 @@
         <v>145</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>128</v>
+        <v>80</v>
       </c>
       <c r="C299" s="3">
-        <v>7005966358599</v>
+        <v>7006105359105</v>
       </c>
       <c r="D299" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E299" s="2">
-        <v>43220.482638888891</v>
+        <v>43220.443055555559</v>
       </c>
       <c r="F299" s="2"/>
       <c r="N299" s="2"/>
@@ -10771,16 +11003,16 @@
         <v>145</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="C300" s="3">
-        <v>7005754358715</v>
+        <v>7006097359055</v>
       </c>
       <c r="D300" t="s">
-        <v>317</v>
+        <v>273</v>
       </c>
       <c r="E300" s="2">
-        <v>43220.486805555556</v>
+        <v>43220.445138888892</v>
       </c>
       <c r="F300" s="2"/>
       <c r="N300" s="2"/>
@@ -10790,16 +11022,16 @@
         <v>145</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="C301" s="3">
-        <v>7005614358794</v>
+        <v>7006092358975</v>
       </c>
       <c r="D301" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="E301" s="2">
-        <v>43220.488888888889</v>
+        <v>43220.448611111111</v>
       </c>
       <c r="F301" s="2"/>
       <c r="P301" s="2"/>
@@ -10809,16 +11041,16 @@
         <v>145</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C302" s="3">
-        <v>7005555358825</v>
+        <v>7006069358719</v>
       </c>
       <c r="D302" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E302" s="2">
-        <v>43220.490277777775</v>
+        <v>43220.45208333333</v>
       </c>
       <c r="F302" s="2"/>
       <c r="P302" s="2"/>
@@ -10828,16 +11060,16 @@
         <v>145</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C303" s="3">
-        <v>7005172359049</v>
+        <v>7006070358639</v>
       </c>
       <c r="D303" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="E303" s="2">
-        <v>43220.493055555555</v>
+        <v>43220.45416666667</v>
       </c>
       <c r="F303" s="2"/>
       <c r="P303" s="2"/>
@@ -10847,16 +11079,16 @@
         <v>145</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="C304" s="3">
-        <v>7004845359228</v>
+        <v>7006048358564</v>
       </c>
       <c r="D304" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="E304" s="2">
-        <v>43220.49722222222</v>
+        <v>43220.455555555556</v>
       </c>
       <c r="F304" s="2"/>
       <c r="O304" s="2"/>
@@ -10867,16 +11099,16 @@
         <v>145</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="C305" s="3">
-        <v>7004594359342</v>
+        <v>7005966358599</v>
       </c>
       <c r="D305" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E305" s="2">
-        <v>43220.503472222219</v>
+        <v>43220.482638888891</v>
       </c>
       <c r="F305" s="2"/>
       <c r="O305" s="2"/>
@@ -10887,16 +11119,16 @@
         <v>145</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="C306" s="3">
-        <v>7004462359409</v>
+        <v>7005754358715</v>
       </c>
       <c r="D306" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="E306" s="2">
-        <v>43220.506249999999</v>
+        <v>43220.486805555556</v>
       </c>
       <c r="F306" s="2"/>
       <c r="O306" s="2"/>
@@ -10907,16 +11139,16 @@
         <v>145</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>51</v>
+        <v>130</v>
       </c>
       <c r="C307" s="3">
-        <v>7004326359594</v>
+        <v>7005614358794</v>
       </c>
       <c r="D307" t="s">
-        <v>323</v>
+        <v>302</v>
       </c>
       <c r="E307" s="2">
-        <v>43220.508333333331</v>
+        <v>43220.488888888889</v>
       </c>
       <c r="F307" s="2"/>
       <c r="O307" s="2"/>
@@ -10927,16 +11159,16 @@
         <v>145</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="C308" s="3">
-        <v>7004265359557</v>
+        <v>7005555358825</v>
       </c>
       <c r="D308" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="E308" s="2">
-        <v>43220.509722222225</v>
+        <v>43220.490277777775</v>
       </c>
       <c r="F308" s="2"/>
       <c r="M308" s="3"/>
@@ -10948,16 +11180,16 @@
         <v>145</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="C309" s="3">
-        <v>7004067359659</v>
+        <v>7005172359049</v>
       </c>
       <c r="D309" t="s">
-        <v>288</v>
+        <v>319</v>
       </c>
       <c r="E309" s="2">
-        <v>43220.513194444444</v>
+        <v>43220.493055555555</v>
       </c>
       <c r="F309" s="2"/>
       <c r="M309" s="3"/>
@@ -10969,16 +11201,16 @@
         <v>145</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>133</v>
+        <v>86</v>
       </c>
       <c r="C310" s="3">
-        <v>7004008359687</v>
+        <v>7004845359228</v>
       </c>
       <c r="D310" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E310" s="2">
-        <v>43220.515277777777</v>
+        <v>43220.49722222222</v>
       </c>
       <c r="F310" s="2"/>
       <c r="M310" s="3"/>
@@ -10990,16 +11222,16 @@
         <v>145</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>134</v>
+        <v>100</v>
       </c>
       <c r="C311" s="3">
-        <v>7003441360041</v>
+        <v>7004594359342</v>
       </c>
       <c r="D311" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E311" s="2">
-        <v>43220.525694444441</v>
+        <v>43220.503472222219</v>
       </c>
       <c r="F311" s="2"/>
       <c r="M311" s="3"/>
@@ -11011,16 +11243,16 @@
         <v>145</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C312" s="3">
-        <v>7003437360048</v>
+        <v>7004462359409</v>
       </c>
       <c r="D312" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E312" s="2">
-        <v>43220.52847222222</v>
+        <v>43220.506249999999</v>
       </c>
       <c r="F312" s="2"/>
       <c r="M312" s="3"/>
@@ -11032,16 +11264,16 @@
         <v>145</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>135</v>
+        <v>51</v>
       </c>
       <c r="C313" s="3">
-        <v>7003383360066</v>
+        <v>7004326359594</v>
       </c>
       <c r="D313" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="E313" s="2">
-        <v>43220.53125</v>
+        <v>43220.508333333331</v>
       </c>
       <c r="F313" s="2"/>
       <c r="M313" s="3"/>
@@ -11053,16 +11285,16 @@
         <v>145</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>136</v>
+        <v>51</v>
       </c>
       <c r="C314" s="3">
-        <v>7003064360213</v>
+        <v>7004265359557</v>
       </c>
       <c r="D314" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E314" s="2">
-        <v>43220.536111111112</v>
+        <v>43220.509722222225</v>
       </c>
       <c r="F314" s="2"/>
       <c r="M314" s="3"/>
@@ -11074,16 +11306,16 @@
         <v>145</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="C315" s="3">
-        <v>7002924360280</v>
+        <v>7004067359659</v>
       </c>
       <c r="D315" t="s">
-        <v>328</v>
+        <v>288</v>
       </c>
       <c r="E315" s="2">
-        <v>43220.539583333331</v>
+        <v>43220.513194444444</v>
       </c>
       <c r="F315" s="2"/>
       <c r="M315" s="3"/>
@@ -11095,16 +11327,16 @@
         <v>145</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>31</v>
+        <v>133</v>
       </c>
       <c r="C316" s="3">
-        <v>7002846360330</v>
+        <v>7004008359687</v>
       </c>
       <c r="D316" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E316" s="2">
-        <v>43220.542361111111</v>
+        <v>43220.515277777777</v>
       </c>
       <c r="F316" s="2"/>
       <c r="M316" s="3"/>
@@ -11116,16 +11348,16 @@
         <v>145</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="C317" s="3">
-        <v>7002828360337</v>
+        <v>7003441360041</v>
       </c>
       <c r="D317" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E317" s="2">
-        <v>43220.544444444444</v>
+        <v>43220.525694444441</v>
       </c>
       <c r="F317" s="2"/>
       <c r="M317" s="3"/>
@@ -11137,16 +11369,16 @@
         <v>145</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>138</v>
+        <v>49</v>
       </c>
       <c r="C318" s="3">
-        <v>7002573360565</v>
+        <v>7003437360048</v>
       </c>
       <c r="D318" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E318" s="2">
-        <v>43220.55</v>
+        <v>43220.52847222222</v>
       </c>
       <c r="F318" s="2"/>
       <c r="M318" s="3"/>
@@ -11158,16 +11390,16 @@
         <v>145</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="C319" s="3">
-        <v>7002551360604</v>
+        <v>7003383360066</v>
       </c>
       <c r="D319" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="E319" s="2">
-        <v>43220.552777777775</v>
+        <v>43220.53125</v>
       </c>
       <c r="F319" s="2"/>
       <c r="M319" s="3"/>
@@ -11179,16 +11411,16 @@
         <v>145</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C320" s="3">
-        <v>7002731360751</v>
+        <v>7003064360213</v>
       </c>
       <c r="D320" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E320" s="2">
-        <v>43220.55972222222</v>
+        <v>43220.536111111112</v>
       </c>
       <c r="F320" s="2"/>
       <c r="M320" s="3"/>
@@ -11200,16 +11432,16 @@
         <v>145</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>84</v>
+        <v>137</v>
       </c>
       <c r="C321" s="3">
-        <v>7003942361654</v>
+        <v>7002924360280</v>
       </c>
       <c r="D321" t="s">
-        <v>300</v>
+        <v>328</v>
       </c>
       <c r="E321" s="2">
-        <v>43220.577777777777</v>
+        <v>43220.539583333331</v>
       </c>
       <c r="F321" s="2"/>
       <c r="M321" s="3"/>
@@ -11221,16 +11453,16 @@
         <v>145</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="C322" s="3">
-        <v>7004010361690</v>
+        <v>7002846360330</v>
       </c>
       <c r="D322" t="s">
-        <v>300</v>
+        <v>328</v>
       </c>
       <c r="E322" s="2">
-        <v>43220.580555555556</v>
+        <v>43220.542361111111</v>
       </c>
       <c r="F322" s="2"/>
       <c r="M322" s="3"/>
@@ -11242,16 +11474,16 @@
         <v>145</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="C323" s="3">
-        <v>7004478361995</v>
+        <v>7002828360337</v>
       </c>
       <c r="D323" t="s">
-        <v>300</v>
+        <v>328</v>
       </c>
       <c r="E323" s="2">
-        <v>43220.63958333333</v>
+        <v>43220.544444444444</v>
       </c>
       <c r="F323" s="2"/>
       <c r="M323" s="3"/>
@@ -11263,16 +11495,16 @@
         <v>145</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C324" s="3">
-        <v>7004518362018</v>
+        <v>7002573360565</v>
       </c>
       <c r="D324" t="s">
-        <v>300</v>
+        <v>329</v>
       </c>
       <c r="E324" s="2">
-        <v>43220.64166666667</v>
+        <v>43220.55</v>
       </c>
       <c r="F324" s="2"/>
       <c r="M324" s="3"/>
@@ -11284,16 +11516,16 @@
         <v>145</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>141</v>
+        <v>75</v>
       </c>
       <c r="C325" s="3">
-        <v>7004641362075</v>
+        <v>7002551360604</v>
       </c>
       <c r="D325" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="E325" s="2">
-        <v>43220.643750000003</v>
+        <v>43220.552777777775</v>
       </c>
       <c r="F325" s="2"/>
       <c r="M325" s="3"/>
@@ -11305,16 +11537,16 @@
         <v>145</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C326" s="3">
-        <v>7004976362244</v>
+        <v>7002731360751</v>
       </c>
       <c r="D326" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E326" s="2">
-        <v>43220.648611111108</v>
+        <v>43220.55972222222</v>
       </c>
       <c r="M326" s="3"/>
       <c r="O326" s="2"/>
@@ -11325,16 +11557,16 @@
         <v>145</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>143</v>
+        <v>84</v>
       </c>
       <c r="C327" s="3">
-        <v>7005036362271</v>
+        <v>7003942361654</v>
       </c>
       <c r="D327" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E327" s="2">
-        <v>43220.650694444441</v>
+        <v>43220.577777777777</v>
       </c>
       <c r="M327" s="3"/>
       <c r="O327" s="2"/>
@@ -11345,16 +11577,16 @@
         <v>145</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
       <c r="C328" s="3">
-        <v>7005401362460</v>
+        <v>7004010361690</v>
       </c>
       <c r="D328" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="E328" s="2">
-        <v>43220.654861111114</v>
+        <v>43220.580555555556</v>
       </c>
       <c r="M328" s="3"/>
       <c r="O328" s="2"/>
@@ -11362,19 +11594,19 @@
     </row>
     <row r="329" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="C329" s="3">
-        <v>7004400359209</v>
+        <v>7004478361995</v>
       </c>
       <c r="D329" t="s">
-        <v>333</v>
+        <v>300</v>
       </c>
       <c r="E329" s="2">
-        <v>43221.29583333333</v>
+        <v>43220.63958333333</v>
       </c>
       <c r="M329" s="3"/>
       <c r="O329" s="2"/>
@@ -11382,19 +11614,19 @@
     </row>
     <row r="330" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="C330" s="3">
-        <v>7003918358291</v>
+        <v>7004518362018</v>
       </c>
       <c r="D330" t="s">
-        <v>321</v>
+        <v>300</v>
       </c>
       <c r="E330" s="2">
-        <v>43221.315972222219</v>
+        <v>43220.64166666667</v>
       </c>
       <c r="M330" s="3"/>
       <c r="O330" s="2"/>
@@ -11402,76 +11634,76 @@
     </row>
     <row r="331" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="C331" s="3">
-        <v>7003782358005</v>
+        <v>7004641362075</v>
       </c>
       <c r="D331" t="s">
-        <v>325</v>
+        <v>292</v>
       </c>
       <c r="E331" s="2">
-        <v>43221.322222222225</v>
+        <v>43220.643750000003</v>
       </c>
       <c r="M331" s="3"/>
       <c r="O331" s="2"/>
     </row>
     <row r="332" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>67</v>
+        <v>142</v>
       </c>
       <c r="C332" s="3">
-        <v>7003733357829</v>
+        <v>7004976362244</v>
       </c>
       <c r="D332" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E332" s="2">
-        <v>43221.325694444444</v>
+        <v>43220.648611111108</v>
       </c>
       <c r="M332" s="3"/>
       <c r="O332" s="2"/>
     </row>
     <row r="333" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>33</v>
+        <v>143</v>
       </c>
       <c r="C333" s="3">
-        <v>7003632357578</v>
+        <v>7005036362271</v>
       </c>
       <c r="D333" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="E333" s="2">
-        <v>43221.329861111109</v>
+        <v>43220.650694444441</v>
       </c>
       <c r="M333" s="3"/>
       <c r="O333" s="2"/>
     </row>
     <row r="334" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>69</v>
+        <v>144</v>
       </c>
       <c r="C334" s="3">
-        <v>7002949356265</v>
+        <v>7005401362460</v>
       </c>
       <c r="D334" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E334" s="2">
-        <v>43221.34375</v>
+        <v>43220.654861111114</v>
       </c>
       <c r="M334" s="3"/>
     </row>
@@ -11480,16 +11712,16 @@
         <v>149</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>36</v>
+        <v>146</v>
       </c>
       <c r="C335" s="3">
-        <v>7002812355949</v>
+        <v>7004400359209</v>
       </c>
       <c r="D335" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E335" s="2">
-        <v>43221.348611111112</v>
+        <v>43221.29583333333</v>
       </c>
       <c r="M335" s="3"/>
     </row>
@@ -11498,16 +11730,16 @@
         <v>149</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="C336" s="3">
-        <v>7002785355789</v>
+        <v>7003918358291</v>
       </c>
       <c r="D336" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="E336" s="2">
-        <v>43221.351388888892</v>
+        <v>43221.315972222219</v>
       </c>
       <c r="M336" s="3"/>
     </row>
@@ -11516,16 +11748,16 @@
         <v>149</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="C337" s="3">
-        <v>7002775355736</v>
+        <v>7003782358005</v>
       </c>
       <c r="D337" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="E337" s="2">
-        <v>43221.354166666664</v>
+        <v>43221.322222222225</v>
       </c>
       <c r="M337" s="3"/>
     </row>
@@ -11534,16 +11766,16 @@
         <v>149</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C338" s="3">
-        <v>7002767355630</v>
+        <v>7003733357829</v>
       </c>
       <c r="D338" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="E338" s="2">
-        <v>43221.375694444447</v>
+        <v>43221.325694444444</v>
       </c>
     </row>
     <row r="339" spans="1:15" x14ac:dyDescent="0.2">
@@ -11551,16 +11783,16 @@
         <v>149</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C339" s="3">
-        <v>7003185355743</v>
+        <v>7003632357578</v>
       </c>
       <c r="D339" t="s">
-        <v>340</v>
+        <v>313</v>
       </c>
       <c r="E339" s="2">
-        <v>43221.38958333333</v>
+        <v>43221.329861111109</v>
       </c>
     </row>
     <row r="340" spans="1:15" x14ac:dyDescent="0.2">
@@ -11568,16 +11800,16 @@
         <v>149</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C340" s="3">
-        <v>7003537355760</v>
+        <v>7002949356265</v>
       </c>
       <c r="D340" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="E340" s="2">
-        <v>43221.397916666669</v>
+        <v>43221.34375</v>
       </c>
       <c r="O340" s="2"/>
     </row>
@@ -11586,16 +11818,16 @@
         <v>149</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C341" s="3">
-        <v>7003563355747</v>
+        <v>7002812355949</v>
       </c>
       <c r="D341" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="E341" s="2">
-        <v>43221.4</v>
+        <v>43221.348611111112</v>
       </c>
       <c r="O341" s="2"/>
     </row>
@@ -11604,16 +11836,16 @@
         <v>149</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="C342" s="3">
-        <v>7003632355750</v>
+        <v>7002785355789</v>
       </c>
       <c r="D342" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="E342" s="2">
-        <v>43221.404166666667</v>
+        <v>43221.351388888892</v>
       </c>
       <c r="O342" s="2"/>
     </row>
@@ -11622,16 +11854,16 @@
         <v>149</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C343" s="3">
-        <v>7005429356236</v>
+        <v>7002775355736</v>
       </c>
       <c r="D343" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="E343" s="2">
-        <v>43221.426388888889</v>
+        <v>43221.354166666664</v>
       </c>
       <c r="O343" s="2"/>
     </row>
@@ -11640,16 +11872,16 @@
         <v>149</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="C344" s="3">
-        <v>7005578356227</v>
+        <v>7002767355630</v>
       </c>
       <c r="D344" t="s">
-        <v>322</v>
+        <v>339</v>
       </c>
       <c r="E344" s="2">
-        <v>43221.431944444441</v>
+        <v>43221.375694444447</v>
       </c>
       <c r="L344" s="3"/>
       <c r="N344" s="2"/>
@@ -11660,16 +11892,16 @@
         <v>149</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C345" s="3">
-        <v>7005615356234</v>
+        <v>7003185355743</v>
       </c>
       <c r="D345" t="s">
-        <v>321</v>
+        <v>340</v>
       </c>
       <c r="E345" s="2">
-        <v>43221.433333333334</v>
+        <v>43221.38958333333</v>
       </c>
       <c r="L345" s="3"/>
       <c r="N345" s="2"/>
@@ -11680,16 +11912,16 @@
         <v>149</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C346" s="3">
-        <v>7005818356285</v>
+        <v>7003537355760</v>
       </c>
       <c r="D346" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E346" s="2">
-        <v>43221.438888888886</v>
+        <v>43221.397916666669</v>
       </c>
       <c r="L346" s="3"/>
       <c r="N346" s="2"/>
@@ -11700,16 +11932,16 @@
         <v>149</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>147</v>
+        <v>42</v>
       </c>
       <c r="C347" s="3">
-        <v>7005889356297</v>
+        <v>7003563355747</v>
       </c>
       <c r="D347" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E347" s="2">
-        <v>43221.440972222219</v>
+        <v>43221.4</v>
       </c>
       <c r="L347" s="3"/>
       <c r="N347" s="2"/>
@@ -11720,16 +11952,16 @@
         <v>149</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="C348" s="3">
-        <v>7005982356291</v>
+        <v>7003632355750</v>
       </c>
       <c r="D348" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E348" s="2">
-        <v>43221.445833333331</v>
+        <v>43221.404166666667</v>
       </c>
       <c r="L348" s="3"/>
       <c r="N348" s="2"/>
@@ -11740,16 +11972,16 @@
         <v>149</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="C349" s="3">
-        <v>7006067356287</v>
+        <v>7005429356236</v>
       </c>
       <c r="D349" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="E349" s="2">
-        <v>43221.448611111111</v>
+        <v>43221.426388888889</v>
       </c>
       <c r="L349" s="3"/>
       <c r="N349" s="2"/>
@@ -11760,16 +11992,16 @@
         <v>149</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="C350" s="3">
-        <v>7006110356278</v>
+        <v>7005578356227</v>
       </c>
       <c r="D350" t="s">
-        <v>348</v>
+        <v>322</v>
       </c>
       <c r="E350" s="2">
-        <v>43221.45208333333</v>
+        <v>43221.431944444441</v>
       </c>
       <c r="L350" s="3"/>
       <c r="N350" s="2"/>
@@ -11780,16 +12012,16 @@
         <v>149</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C351" s="3">
-        <v>7006178356268</v>
+        <v>7005615356234</v>
       </c>
       <c r="D351" t="s">
-        <v>241</v>
+        <v>321</v>
       </c>
       <c r="E351" s="2">
-        <v>43221.455555555556</v>
+        <v>43221.433333333334</v>
       </c>
       <c r="L351" s="3"/>
       <c r="N351" s="2"/>
@@ -11800,16 +12032,16 @@
         <v>149</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="C352" s="3">
-        <v>7006451356272</v>
+        <v>7005818356285</v>
       </c>
       <c r="D352" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E352" s="2">
-        <v>43221.461111111108</v>
+        <v>43221.438888888886</v>
       </c>
       <c r="L352" s="3"/>
       <c r="N352" s="2"/>
@@ -11820,16 +12052,16 @@
         <v>149</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>75</v>
+        <v>147</v>
       </c>
       <c r="C353" s="3">
-        <v>7006803356301</v>
+        <v>7005889356297</v>
       </c>
       <c r="D353" t="s">
-        <v>245</v>
+        <v>346</v>
       </c>
       <c r="E353" s="2">
-        <v>43221.468055555553</v>
+        <v>43221.440972222219</v>
       </c>
       <c r="L353" s="3"/>
       <c r="N353" s="2"/>
@@ -11840,16 +12072,16 @@
         <v>149</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="C354" s="3">
-        <v>7006600356476</v>
+        <v>7005982356291</v>
       </c>
       <c r="D354" t="s">
-        <v>290</v>
+        <v>346</v>
       </c>
       <c r="E354" s="2">
-        <v>43221.475694444445</v>
+        <v>43221.445833333331</v>
       </c>
       <c r="L354" s="3"/>
       <c r="N354" s="2"/>
@@ -11860,16 +12092,16 @@
         <v>149</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="C355" s="3">
-        <v>7005428357911</v>
+        <v>7006067356287</v>
       </c>
       <c r="D355" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="E355" s="2">
-        <v>43221.529166666667</v>
+        <v>43221.448611111111</v>
       </c>
       <c r="L355" s="3"/>
       <c r="N355" s="2"/>
@@ -11880,16 +12112,16 @@
         <v>149</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="C356" s="3">
-        <v>7005274358127</v>
+        <v>7006110356278</v>
       </c>
       <c r="D356" t="s">
-        <v>291</v>
+        <v>348</v>
       </c>
       <c r="E356" s="2">
-        <v>43221.532638888886</v>
+        <v>43221.45208333333</v>
       </c>
       <c r="L356" s="3"/>
       <c r="N356" s="2"/>
@@ -11900,16 +12132,16 @@
         <v>149</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C357" s="3">
-        <v>7005214358195</v>
+        <v>7006178356268</v>
       </c>
       <c r="D357" t="s">
-        <v>351</v>
+        <v>241</v>
       </c>
       <c r="E357" s="2">
-        <v>43221.535416666666</v>
+        <v>43221.455555555556</v>
       </c>
       <c r="L357" s="3"/>
       <c r="N357" s="2"/>
@@ -11920,16 +12152,16 @@
         <v>149</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>148</v>
+        <v>29</v>
       </c>
       <c r="C358" s="3">
-        <v>7004453359147</v>
+        <v>7006451356272</v>
       </c>
       <c r="D358" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E358" s="2">
-        <v>43221.547222222223</v>
+        <v>43221.461111111108</v>
       </c>
       <c r="L358" s="3"/>
       <c r="N358" s="2"/>
@@ -11937,19 +12169,19 @@
     </row>
     <row r="359" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="C359" s="3">
-        <v>7008546366649</v>
+        <v>7006803356301</v>
       </c>
       <c r="D359" t="s">
-        <v>208</v>
+        <v>245</v>
       </c>
       <c r="E359" s="2">
-        <v>43222.325694444444</v>
+        <v>43221.468055555553</v>
       </c>
       <c r="L359" s="3"/>
       <c r="N359" s="2"/>
@@ -11957,19 +12189,19 @@
     </row>
     <row r="360" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C360" s="3">
-        <v>7008527366619</v>
+        <v>7006600356476</v>
       </c>
       <c r="D360" t="s">
-        <v>235</v>
+        <v>290</v>
       </c>
       <c r="E360" s="2">
-        <v>43222.329861111109</v>
+        <v>43221.475694444445</v>
       </c>
       <c r="L360" s="3"/>
       <c r="N360" s="2"/>
@@ -11977,19 +12209,19 @@
     </row>
     <row r="361" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="C361" s="3">
-        <v>7008489366555</v>
+        <v>7005428357911</v>
       </c>
       <c r="D361" t="s">
-        <v>196</v>
+        <v>350</v>
       </c>
       <c r="E361" s="2">
-        <v>43222.334027777775</v>
+        <v>43221.529166666667</v>
       </c>
       <c r="L361" s="3"/>
       <c r="N361" s="2"/>
@@ -11997,19 +12229,19 @@
     </row>
     <row r="362" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="C362" s="3">
-        <v>7008481366542</v>
+        <v>7005274358127</v>
       </c>
       <c r="D362" t="s">
-        <v>223</v>
+        <v>291</v>
       </c>
       <c r="E362" s="2">
-        <v>43222.335416666669</v>
+        <v>43221.532638888886</v>
       </c>
       <c r="L362" s="3"/>
       <c r="N362" s="2"/>
@@ -12017,19 +12249,19 @@
     </row>
     <row r="363" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C363" s="3">
-        <v>7008469366500</v>
+        <v>7005214358195</v>
       </c>
       <c r="D363" t="s">
-        <v>213</v>
+        <v>351</v>
       </c>
       <c r="E363" s="2">
-        <v>43222.336805555555</v>
+        <v>43221.535416666666</v>
       </c>
       <c r="L363" s="3"/>
       <c r="N363" s="2"/>
@@ -12037,19 +12269,19 @@
     </row>
     <row r="364" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>41</v>
+        <v>148</v>
       </c>
       <c r="C364" s="3">
-        <v>7008230366123</v>
+        <v>7004453359147</v>
       </c>
       <c r="D364" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E364" s="2">
-        <v>43222.348611111112</v>
+        <v>43221.547222222223</v>
       </c>
       <c r="L364" s="3"/>
       <c r="N364" s="2"/>
@@ -12060,16 +12292,16 @@
         <v>152</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>42</v>
+        <v>150</v>
       </c>
       <c r="C365" s="3">
-        <v>7008184366055</v>
+        <v>7008546366649</v>
       </c>
       <c r="D365" t="s">
-        <v>354</v>
+        <v>208</v>
       </c>
       <c r="E365" s="2">
-        <v>43222.351388888892</v>
+        <v>43222.325694444444</v>
       </c>
       <c r="L365" s="3"/>
       <c r="N365" s="2"/>
@@ -12080,16 +12312,16 @@
         <v>152</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C366" s="3">
-        <v>7007756365256</v>
+        <v>7008527366619</v>
       </c>
       <c r="D366" t="s">
-        <v>355</v>
+        <v>235</v>
       </c>
       <c r="E366" s="2">
-        <v>43222.363888888889</v>
+        <v>43222.329861111109</v>
       </c>
       <c r="L366" s="3"/>
       <c r="N366" s="2"/>
@@ -12100,16 +12332,16 @@
         <v>152</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C367" s="3">
-        <v>7007701365129</v>
+        <v>7008489366555</v>
       </c>
       <c r="D367" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="E367" s="2">
-        <v>43222.366666666669</v>
+        <v>43222.334027777775</v>
       </c>
       <c r="L367" s="3"/>
       <c r="N367" s="2"/>
@@ -12120,16 +12352,16 @@
         <v>152</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="C368" s="3">
-        <v>7007599364865</v>
+        <v>7008481366542</v>
       </c>
       <c r="D368" t="s">
-        <v>356</v>
+        <v>223</v>
       </c>
       <c r="E368" s="2">
-        <v>43222.37222222222</v>
+        <v>43222.335416666669</v>
       </c>
       <c r="L368" s="3"/>
       <c r="N368" s="2"/>
@@ -12140,16 +12372,16 @@
         <v>152</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C369" s="3">
-        <v>7007353364176</v>
+        <v>7008469366500</v>
       </c>
       <c r="D369" t="s">
-        <v>273</v>
+        <v>213</v>
       </c>
       <c r="E369" s="2">
-        <v>43222.379166666666</v>
+        <v>43222.336805555555</v>
       </c>
       <c r="L369" s="3"/>
       <c r="N369" s="2"/>
@@ -12160,16 +12392,16 @@
         <v>152</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C370" s="3">
-        <v>7007224363897</v>
+        <v>7008230366123</v>
       </c>
       <c r="D370" t="s">
-        <v>303</v>
+        <v>353</v>
       </c>
       <c r="E370" s="2">
-        <v>43222.383333333331</v>
+        <v>43222.348611111112</v>
       </c>
       <c r="L370" s="3"/>
       <c r="N370" s="2"/>
@@ -12180,16 +12412,16 @@
         <v>152</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C371" s="3">
-        <v>7006864363345</v>
+        <v>7008184366055</v>
       </c>
       <c r="D371" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="E371" s="2">
-        <v>43222.400000000001</v>
+        <v>43222.351388888892</v>
       </c>
       <c r="L371" s="3"/>
       <c r="N371" s="2"/>
@@ -12200,16 +12432,16 @@
         <v>152</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C372" s="3">
-        <v>7006855363327</v>
+        <v>7007756365256</v>
       </c>
       <c r="D372" t="s">
-        <v>319</v>
+        <v>355</v>
       </c>
       <c r="E372" s="2">
-        <v>43222.402083333334</v>
+        <v>43222.363888888889</v>
       </c>
       <c r="L372" s="3"/>
       <c r="N372" s="2"/>
@@ -12220,16 +12452,16 @@
         <v>152</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="C373" s="3">
-        <v>7006741363193</v>
+        <v>7007701365129</v>
       </c>
       <c r="D373" t="s">
-        <v>358</v>
+        <v>188</v>
       </c>
       <c r="E373" s="2">
-        <v>43222.40625</v>
+        <v>43222.366666666669</v>
       </c>
       <c r="L373" s="3"/>
       <c r="N373" s="2"/>
@@ -12240,16 +12472,16 @@
         <v>152</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C374" s="3">
-        <v>7006705363181</v>
+        <v>7007599364865</v>
       </c>
       <c r="D374" t="s">
-        <v>312</v>
+        <v>356</v>
       </c>
       <c r="E374" s="2">
-        <v>43222.408333333333</v>
+        <v>43222.37222222222</v>
       </c>
       <c r="L374" s="3"/>
       <c r="N374" s="2"/>
@@ -12260,16 +12492,16 @@
         <v>152</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="C375" s="3">
-        <v>7006635363106</v>
+        <v>7007353364176</v>
       </c>
       <c r="D375" t="s">
-        <v>358</v>
+        <v>273</v>
       </c>
       <c r="E375" s="2">
-        <v>43222.410416666666</v>
+        <v>43222.379166666666</v>
       </c>
       <c r="L375" s="3"/>
       <c r="N375" s="2"/>
@@ -12280,16 +12512,16 @@
         <v>152</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="C376" s="3">
-        <v>7006632363092</v>
+        <v>7007224363897</v>
       </c>
       <c r="D376" t="s">
-        <v>358</v>
+        <v>303</v>
       </c>
       <c r="E376" s="2">
-        <v>43222.412499999999</v>
+        <v>43222.383333333331</v>
       </c>
       <c r="L376" s="3"/>
       <c r="N376" s="2"/>
@@ -12300,16 +12532,16 @@
         <v>152</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C377" s="3">
-        <v>7006656363084</v>
+        <v>7006864363345</v>
       </c>
       <c r="D377" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E377" s="2">
-        <v>43222.425000000003</v>
+        <v>43222.400000000001</v>
       </c>
       <c r="L377" s="3"/>
       <c r="N377" s="2"/>
@@ -12319,16 +12551,16 @@
         <v>152</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="C378" s="3">
-        <v>7006704363076</v>
+        <v>7006855363327</v>
       </c>
       <c r="D378" t="s">
-        <v>359</v>
+        <v>319</v>
       </c>
       <c r="E378" s="2">
-        <v>43222.431944444441</v>
+        <v>43222.402083333334</v>
       </c>
       <c r="L378" s="3"/>
       <c r="N378" s="2"/>
@@ -12338,16 +12570,16 @@
         <v>152</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C379" s="3">
-        <v>7006759363054</v>
+        <v>7006741363193</v>
       </c>
       <c r="D379" t="s">
-        <v>288</v>
+        <v>358</v>
       </c>
       <c r="E379" s="2">
-        <v>43222.435416666667</v>
+        <v>43222.40625</v>
       </c>
       <c r="L379" s="3"/>
       <c r="N379" s="2"/>
@@ -12357,16 +12589,16 @@
         <v>152</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C380" s="3">
-        <v>7006796363052</v>
+        <v>7006705363181</v>
       </c>
       <c r="D380" t="s">
-        <v>360</v>
+        <v>312</v>
       </c>
       <c r="E380" s="2">
-        <v>43222.436805555553</v>
+        <v>43222.408333333333</v>
       </c>
       <c r="L380" s="3"/>
       <c r="N380" s="2"/>
@@ -12376,16 +12608,16 @@
         <v>152</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="C381" s="3">
-        <v>7006864363034</v>
+        <v>7006635363106</v>
       </c>
       <c r="D381" t="s">
-        <v>313</v>
+        <v>358</v>
       </c>
       <c r="E381" s="2">
-        <v>43222.439583333333</v>
+        <v>43222.410416666666</v>
       </c>
     </row>
     <row r="382" spans="1:15" x14ac:dyDescent="0.2">
@@ -12393,16 +12625,16 @@
         <v>152</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="C382" s="3">
-        <v>7006882363032</v>
+        <v>7006632363092</v>
       </c>
       <c r="D382" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E382" s="2">
-        <v>43222.44027777778</v>
+        <v>43222.412499999999</v>
       </c>
     </row>
     <row r="383" spans="1:15" x14ac:dyDescent="0.2">
@@ -12410,16 +12642,16 @@
         <v>152</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C383" s="3">
-        <v>7007268362982</v>
+        <v>7006656363084</v>
       </c>
       <c r="D383" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="E383" s="2">
-        <v>43222.448611111111</v>
+        <v>43222.425000000003</v>
       </c>
     </row>
     <row r="384" spans="1:15" x14ac:dyDescent="0.2">
@@ -12427,16 +12659,16 @@
         <v>152</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C384" s="3">
-        <v>7007286362985</v>
+        <v>7006704363076</v>
       </c>
       <c r="D384" t="s">
-        <v>282</v>
+        <v>359</v>
       </c>
       <c r="E384" s="2">
-        <v>43222.450694444444</v>
+        <v>43222.431944444441</v>
       </c>
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.2">
@@ -12444,16 +12676,16 @@
         <v>152</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C385" s="3">
-        <v>7007299362986</v>
+        <v>7006759363054</v>
       </c>
       <c r="D385" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="E385" s="2">
-        <v>43222.45208333333</v>
+        <v>43222.435416666667</v>
       </c>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.2">
@@ -12461,16 +12693,16 @@
         <v>152</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C386" s="3">
-        <v>7007413362958</v>
+        <v>7006796363052</v>
       </c>
       <c r="D386" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="E386" s="2">
-        <v>43222.455555555556</v>
+        <v>43222.436805555553</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.2">
@@ -12478,16 +12710,16 @@
         <v>152</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="C387" s="3">
-        <v>7009681362779</v>
+        <v>7006864363034</v>
       </c>
       <c r="D387" t="s">
-        <v>243</v>
+        <v>313</v>
       </c>
       <c r="E387" s="2">
-        <v>43222.494444444441</v>
+        <v>43222.439583333333</v>
       </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.2">
@@ -12495,16 +12727,16 @@
         <v>152</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C388" s="3">
-        <v>7010638362876</v>
+        <v>7006882363032</v>
       </c>
       <c r="D388" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="E388" s="2">
-        <v>43222.50277777778</v>
+        <v>43222.44027777778</v>
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.2">
@@ -12512,16 +12744,16 @@
         <v>152</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C389" s="3">
-        <v>7010614362913</v>
+        <v>7007268362982</v>
       </c>
       <c r="D389" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E389" s="2">
-        <v>43222.522222222222</v>
+        <v>43222.448611111111</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.2">
@@ -12529,16 +12761,16 @@
         <v>152</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C390" s="3">
-        <v>7010584362972</v>
+        <v>7007286362985</v>
       </c>
       <c r="D390" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="E390" s="2">
-        <v>43222.524305555555</v>
+        <v>43222.450694444444</v>
       </c>
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.2">
@@ -12546,16 +12778,16 @@
         <v>152</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>151</v>
+        <v>77</v>
       </c>
       <c r="C391" s="3">
-        <v>7009698364284</v>
+        <v>7007299362986</v>
       </c>
       <c r="D391" t="s">
-        <v>365</v>
+        <v>281</v>
       </c>
       <c r="E391" s="2">
-        <v>43222.599305555559</v>
+        <v>43222.45208333333</v>
       </c>
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.2">
@@ -12563,16 +12795,16 @@
         <v>152</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C392" s="3">
-        <v>7009212365539</v>
+        <v>7007413362958</v>
       </c>
       <c r="D392" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="E392" s="2">
-        <v>43222.618055555555</v>
+        <v>43222.455555555556</v>
       </c>
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.2">
@@ -12580,16 +12812,16 @@
         <v>152</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C393" s="3">
-        <v>7009208365577</v>
+        <v>7009681362779</v>
       </c>
       <c r="D393" t="s">
-        <v>366</v>
+        <v>243</v>
       </c>
       <c r="E393" s="2">
-        <v>43222.620138888888</v>
+        <v>43222.494444444441</v>
       </c>
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.2">
@@ -12597,16 +12829,16 @@
         <v>152</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C394" s="3">
-        <v>7009208365588</v>
+        <v>7010638362876</v>
       </c>
       <c r="D394" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="E394" s="2">
-        <v>43222.621527777781</v>
+        <v>43222.50277777778</v>
       </c>
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.2">
@@ -12614,16 +12846,16 @@
         <v>152</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="C395" s="3">
-        <v>7009199365638</v>
+        <v>7010614362913</v>
       </c>
       <c r="D395" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E395" s="2">
-        <v>43222.623611111114</v>
+        <v>43222.522222222222</v>
       </c>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.2">
@@ -12631,16 +12863,16 @@
         <v>152</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C396" s="3">
-        <v>7009186365662</v>
+        <v>7010584362972</v>
       </c>
       <c r="D396" t="s">
-        <v>369</v>
+        <v>278</v>
       </c>
       <c r="E396" s="2">
-        <v>43222.625694444447</v>
+        <v>43222.524305555555</v>
       </c>
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.2">
@@ -12648,16 +12880,16 @@
         <v>152</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>51</v>
+        <v>151</v>
       </c>
       <c r="C397" s="3">
-        <v>7008623366228</v>
+        <v>7009698364284</v>
       </c>
       <c r="D397" t="s">
-        <v>184</v>
+        <v>365</v>
       </c>
       <c r="E397" s="2">
-        <v>43222.638888888891</v>
+        <v>43222.599305555559</v>
       </c>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.2">
@@ -12665,13 +12897,16 @@
         <v>152</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="C398" s="3">
-        <v>7009183365670</v>
+        <v>7009212365539</v>
+      </c>
+      <c r="D398" t="s">
+        <v>354</v>
       </c>
       <c r="E398" s="2">
-        <v>43222.640277777777</v>
+        <v>43222.618055555555</v>
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.2">
@@ -12679,15 +12914,114 @@
         <v>152</v>
       </c>
       <c r="B399" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C399" s="3">
+        <v>7009208365577</v>
+      </c>
+      <c r="D399" t="s">
+        <v>366</v>
+      </c>
+      <c r="E399" s="2">
+        <v>43222.620138888888</v>
+      </c>
+    </row>
+    <row r="400" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A400" t="s">
+        <v>152</v>
+      </c>
+      <c r="B400" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C400" s="3">
+        <v>7009208365588</v>
+      </c>
+      <c r="D400" t="s">
+        <v>367</v>
+      </c>
+      <c r="E400" s="2">
+        <v>43222.621527777781</v>
+      </c>
+    </row>
+    <row r="401" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A401" t="s">
+        <v>152</v>
+      </c>
+      <c r="B401" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C401" s="3">
+        <v>7009199365638</v>
+      </c>
+      <c r="D401" t="s">
+        <v>368</v>
+      </c>
+      <c r="E401" s="2">
+        <v>43222.623611111114</v>
+      </c>
+    </row>
+    <row r="402" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A402" t="s">
+        <v>152</v>
+      </c>
+      <c r="B402" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C402" s="3">
+        <v>7009186365662</v>
+      </c>
+      <c r="D402" t="s">
+        <v>369</v>
+      </c>
+      <c r="E402" s="2">
+        <v>43222.625694444447</v>
+      </c>
+    </row>
+    <row r="403" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A403" t="s">
+        <v>152</v>
+      </c>
+      <c r="B403" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C403" s="3">
+        <v>7008623366228</v>
+      </c>
+      <c r="D403" t="s">
+        <v>184</v>
+      </c>
+      <c r="E403" s="2">
+        <v>43222.638888888891</v>
+      </c>
+    </row>
+    <row r="404" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A404" t="s">
+        <v>152</v>
+      </c>
+      <c r="B404" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C404" s="3">
+        <v>7009183365670</v>
+      </c>
+      <c r="E404" s="2">
+        <v>43222.640277777777</v>
+      </c>
+    </row>
+    <row r="405" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A405" t="s">
+        <v>152</v>
+      </c>
+      <c r="B405" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C399" s="3">
+      <c r="C405" s="3">
         <v>7008631366281</v>
       </c>
-      <c r="D399" t="s">
+      <c r="D405" t="s">
         <v>370</v>
       </c>
-      <c r="E399" s="2">
+      <c r="E405" s="2">
         <v>43222.640972222223</v>
       </c>
     </row>

</xml_diff>

<commit_message>
096 klar. 1 hög tillagd på varje RS som bara var 1 hög.
</commit_message>
<xml_diff>
--- a/Rawdata/riptransekter helags 2018.xlsx
+++ b/Rawdata/riptransekter helags 2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11120" yWindow="460" windowWidth="25600" windowHeight="14120" xr2:uid="{731D7839-4CAB-374B-BEA5-3406519CB6C1}"/>
+    <workbookView xWindow="5320" yWindow="460" windowWidth="25600" windowHeight="14120" xr2:uid="{731D7839-4CAB-374B-BEA5-3406519CB6C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2155" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2254" uniqueCount="436">
   <si>
     <t>vinkel</t>
   </si>
@@ -1290,6 +1290,48 @@
   </si>
   <si>
     <t>snö</t>
+  </si>
+  <si>
+    <t>växlande molnighet, 0 till -1</t>
+  </si>
+  <si>
+    <t>skare + 2 mm nysnö</t>
+  </si>
+  <si>
+    <t>snö, lätt vind</t>
+  </si>
+  <si>
+    <t>saknar</t>
+  </si>
+  <si>
+    <t>sol, lite snöfall</t>
+  </si>
+  <si>
+    <t>sol, varmt, 15 grader</t>
+  </si>
+  <si>
+    <t>kan vara dubbelrknad. De jag såg innan flög dock åt andra hållet</t>
+  </si>
+  <si>
+    <t>mycket snö och få barfläckar på transekt</t>
+  </si>
+  <si>
+    <t>molningt, lätt snöfall, kallare</t>
+  </si>
+  <si>
+    <t>kraftigt snöfall</t>
+  </si>
+  <si>
+    <t>någon ljusbrun, någon gammal</t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>930 m</t>
+  </si>
+  <si>
+    <t>gps saknades. Lade till i efterhand. Höjd är en gissning.</t>
   </si>
 </sst>
 </file>
@@ -1646,9 +1688,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B9831C9-A413-654D-876F-A809696709AE}">
   <dimension ref="A1:Z438"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O232" sqref="O232:O265"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A296" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F315" sqref="F315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1795,6 +1837,9 @@
       <c r="J4" t="s">
         <v>10</v>
       </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
       <c r="L4">
         <v>7</v>
       </c>
@@ -1865,6 +1910,9 @@
       <c r="F6" t="s">
         <v>11</v>
       </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
       <c r="L6">
         <v>1</v>
       </c>
@@ -1929,6 +1977,9 @@
       <c r="J8" t="s">
         <v>10</v>
       </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
       <c r="L8">
         <v>15</v>
       </c>
@@ -2037,6 +2088,9 @@
       <c r="J11" t="s">
         <v>16</v>
       </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
       <c r="L11">
         <v>1</v>
       </c>
@@ -2323,6 +2377,9 @@
       <c r="J19" t="s">
         <v>10</v>
       </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
       <c r="L19">
         <v>3</v>
       </c>
@@ -2358,6 +2415,9 @@
       <c r="J20" t="s">
         <v>10</v>
       </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
       <c r="L20">
         <v>1</v>
       </c>
@@ -2425,6 +2485,9 @@
       <c r="J22" t="s">
         <v>16</v>
       </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
       <c r="L22">
         <v>25</v>
       </c>
@@ -2460,6 +2523,9 @@
       <c r="J23" t="s">
         <v>10</v>
       </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
       <c r="L23">
         <v>5</v>
       </c>
@@ -2498,6 +2564,9 @@
       <c r="J24" t="s">
         <v>10</v>
       </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
       <c r="L24">
         <v>1</v>
       </c>
@@ -2536,6 +2605,9 @@
       <c r="J25" t="s">
         <v>15</v>
       </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
       <c r="L25">
         <v>20</v>
       </c>
@@ -2638,6 +2710,9 @@
       <c r="F28" t="s">
         <v>11</v>
       </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
       <c r="L28">
         <v>12</v>
       </c>
@@ -2756,6 +2831,9 @@
       </c>
       <c r="F32" t="s">
         <v>11</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
       </c>
       <c r="L32">
         <v>1</v>
@@ -2961,6 +3039,9 @@
       <c r="J42" t="s">
         <v>16</v>
       </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
       <c r="L42">
         <v>22</v>
       </c>
@@ -2996,6 +3077,9 @@
       <c r="J43" t="s">
         <v>10</v>
       </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
       <c r="L43">
         <v>6</v>
       </c>
@@ -3166,6 +3250,9 @@
       <c r="J47" t="s">
         <v>16</v>
       </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
       <c r="L47">
         <v>40</v>
       </c>
@@ -3248,6 +3335,9 @@
       <c r="J49" t="s">
         <v>16</v>
       </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
       <c r="L49">
         <v>19</v>
       </c>
@@ -3453,6 +3543,9 @@
       <c r="J54" t="s">
         <v>16</v>
       </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
       <c r="L54">
         <v>13</v>
       </c>
@@ -3520,6 +3613,9 @@
       <c r="J56" t="s">
         <v>16</v>
       </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
       <c r="L56">
         <v>35</v>
       </c>
@@ -3584,6 +3680,9 @@
       <c r="J58" t="s">
         <v>10</v>
       </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
       <c r="L58">
         <v>1</v>
       </c>
@@ -3622,6 +3721,9 @@
       <c r="J59" t="s">
         <v>10</v>
       </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
       <c r="L59">
         <v>10</v>
       </c>
@@ -3754,6 +3856,9 @@
       <c r="J62" t="s">
         <v>10</v>
       </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
       <c r="L62">
         <v>9</v>
       </c>
@@ -3798,6 +3903,9 @@
       <c r="J63" t="s">
         <v>16</v>
       </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
       <c r="L63">
         <v>28</v>
       </c>
@@ -3915,6 +4023,9 @@
       <c r="J66" t="s">
         <v>15</v>
       </c>
+      <c r="K66">
+        <v>1</v>
+      </c>
       <c r="L66">
         <v>1</v>
       </c>
@@ -4026,6 +4137,9 @@
       <c r="J69" t="s">
         <v>10</v>
       </c>
+      <c r="K69">
+        <v>1</v>
+      </c>
       <c r="L69">
         <v>16</v>
       </c>
@@ -4177,6 +4291,9 @@
       <c r="F74" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
       <c r="L74">
         <v>1</v>
       </c>
@@ -4794,6 +4911,9 @@
       <c r="J93" t="s">
         <v>16</v>
       </c>
+      <c r="K93">
+        <v>1</v>
+      </c>
       <c r="L93">
         <v>2</v>
       </c>
@@ -4965,7 +5085,7 @@
         <v>16</v>
       </c>
       <c r="K97">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L97">
         <v>35</v>
@@ -5037,6 +5157,9 @@
       <c r="J99" t="s">
         <v>16</v>
       </c>
+      <c r="K99">
+        <v>1</v>
+      </c>
       <c r="L99">
         <v>27</v>
       </c>
@@ -5195,6 +5318,9 @@
       <c r="J103" t="s">
         <v>10</v>
       </c>
+      <c r="K103">
+        <v>1</v>
+      </c>
       <c r="L103">
         <v>8</v>
       </c>
@@ -5321,6 +5447,9 @@
       <c r="J106" t="s">
         <v>10</v>
       </c>
+      <c r="K106">
+        <v>1</v>
+      </c>
       <c r="L106">
         <v>17</v>
       </c>
@@ -5397,6 +5526,9 @@
       <c r="J108" t="s">
         <v>16</v>
       </c>
+      <c r="K108">
+        <v>1</v>
+      </c>
       <c r="L108">
         <v>32</v>
       </c>
@@ -5441,6 +5573,9 @@
       <c r="J109" t="s">
         <v>16</v>
       </c>
+      <c r="K109">
+        <v>1</v>
+      </c>
       <c r="L109">
         <v>23</v>
       </c>
@@ -5995,6 +6130,9 @@
       <c r="J122" t="s">
         <v>16</v>
       </c>
+      <c r="K122">
+        <v>1</v>
+      </c>
       <c r="L122">
         <v>26</v>
       </c>
@@ -6036,6 +6174,9 @@
       <c r="J123" t="s">
         <v>15</v>
       </c>
+      <c r="K123">
+        <v>1</v>
+      </c>
       <c r="M123" t="s">
         <v>371</v>
       </c>
@@ -6077,6 +6218,9 @@
       <c r="J124" t="s">
         <v>16</v>
       </c>
+      <c r="K124">
+        <v>1</v>
+      </c>
       <c r="M124" t="s">
         <v>371</v>
       </c>
@@ -6147,6 +6291,9 @@
       <c r="J126" t="s">
         <v>16</v>
       </c>
+      <c r="K126">
+        <v>1</v>
+      </c>
       <c r="L126">
         <v>12</v>
       </c>
@@ -6184,6 +6331,9 @@
       </c>
       <c r="J127" t="s">
         <v>15</v>
+      </c>
+      <c r="K127">
+        <v>1</v>
       </c>
       <c r="L127">
         <v>2</v>
@@ -6670,6 +6820,9 @@
       <c r="J142" t="s">
         <v>16</v>
       </c>
+      <c r="K142">
+        <v>1</v>
+      </c>
       <c r="L142">
         <v>5</v>
       </c>
@@ -6819,6 +6972,9 @@
       <c r="H146">
         <v>90</v>
       </c>
+      <c r="K146">
+        <v>1</v>
+      </c>
       <c r="L146">
         <v>3</v>
       </c>
@@ -6921,6 +7077,9 @@
       <c r="J149" t="s">
         <v>10</v>
       </c>
+      <c r="K149">
+        <v>1</v>
+      </c>
       <c r="L149">
         <v>2</v>
       </c>
@@ -6956,6 +7115,9 @@
       <c r="F150" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="K150">
+        <v>1</v>
+      </c>
       <c r="L150">
         <v>2</v>
       </c>
@@ -6991,6 +7153,9 @@
       <c r="F151" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="K151">
+        <v>1</v>
+      </c>
       <c r="L151">
         <v>3</v>
       </c>
@@ -7023,6 +7188,9 @@
       <c r="F152" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="K152">
+        <v>1</v>
+      </c>
       <c r="L152">
         <v>3</v>
       </c>
@@ -7055,6 +7223,9 @@
       <c r="F153" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="K153">
+        <v>1</v>
+      </c>
       <c r="L153">
         <v>5</v>
       </c>
@@ -7122,6 +7293,9 @@
       <c r="H155">
         <v>90</v>
       </c>
+      <c r="K155">
+        <v>1</v>
+      </c>
       <c r="L155">
         <v>1</v>
       </c>
@@ -7186,6 +7360,9 @@
       <c r="H157">
         <v>270</v>
       </c>
+      <c r="K157">
+        <v>1</v>
+      </c>
       <c r="L157">
         <v>1</v>
       </c>
@@ -7335,6 +7512,9 @@
       <c r="J166" t="s">
         <v>10</v>
       </c>
+      <c r="K166">
+        <v>1</v>
+      </c>
       <c r="L166">
         <v>8</v>
       </c>
@@ -7493,6 +7673,9 @@
       <c r="J170" t="s">
         <v>10</v>
       </c>
+      <c r="K170">
+        <v>1</v>
+      </c>
       <c r="L170">
         <v>2</v>
       </c>
@@ -7534,6 +7717,9 @@
       <c r="J171" t="s">
         <v>10</v>
       </c>
+      <c r="K171">
+        <v>1</v>
+      </c>
       <c r="L171">
         <v>1</v>
       </c>
@@ -7654,6 +7840,9 @@
       <c r="J174" t="s">
         <v>10</v>
       </c>
+      <c r="K174">
+        <v>1</v>
+      </c>
       <c r="L174">
         <v>2</v>
       </c>
@@ -7698,6 +7887,9 @@
       <c r="J175" t="s">
         <v>10</v>
       </c>
+      <c r="K175">
+        <v>1</v>
+      </c>
       <c r="L175">
         <v>14</v>
       </c>
@@ -7742,6 +7934,9 @@
       <c r="J176" t="s">
         <v>10</v>
       </c>
+      <c r="K176">
+        <v>1</v>
+      </c>
       <c r="L176">
         <v>2</v>
       </c>
@@ -7783,6 +7978,9 @@
       <c r="J177" t="s">
         <v>10</v>
       </c>
+      <c r="K177">
+        <v>1</v>
+      </c>
       <c r="L177">
         <v>2</v>
       </c>
@@ -7827,6 +8025,9 @@
       <c r="J178" t="s">
         <v>10</v>
       </c>
+      <c r="K178">
+        <v>1</v>
+      </c>
       <c r="L178">
         <v>3</v>
       </c>
@@ -7871,6 +8072,9 @@
       <c r="J179" t="s">
         <v>10</v>
       </c>
+      <c r="K179">
+        <v>1</v>
+      </c>
       <c r="L179">
         <v>2</v>
       </c>
@@ -7916,7 +8120,7 @@
         <v>10</v>
       </c>
       <c r="K180">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L180">
         <v>20</v>
@@ -7962,6 +8166,9 @@
       <c r="J181" t="s">
         <v>10</v>
       </c>
+      <c r="K181">
+        <v>1</v>
+      </c>
       <c r="L181">
         <v>22</v>
       </c>
@@ -8041,6 +8248,9 @@
       <c r="J183" t="s">
         <v>10</v>
       </c>
+      <c r="K183">
+        <v>1</v>
+      </c>
       <c r="L183">
         <v>17</v>
       </c>
@@ -8085,6 +8295,9 @@
       <c r="J184" t="s">
         <v>10</v>
       </c>
+      <c r="K184">
+        <v>1</v>
+      </c>
       <c r="L184">
         <v>12</v>
       </c>
@@ -8222,6 +8435,9 @@
       <c r="J188" t="s">
         <v>10</v>
       </c>
+      <c r="K188">
+        <v>1</v>
+      </c>
       <c r="L188">
         <v>17</v>
       </c>
@@ -8307,6 +8523,9 @@
       <c r="J190" t="s">
         <v>10</v>
       </c>
+      <c r="K190">
+        <v>1</v>
+      </c>
       <c r="L190">
         <v>4</v>
       </c>
@@ -8392,6 +8611,9 @@
       <c r="J192" t="s">
         <v>10</v>
       </c>
+      <c r="K192">
+        <v>1</v>
+      </c>
       <c r="L192">
         <v>12</v>
       </c>
@@ -8433,6 +8655,9 @@
       <c r="H193">
         <v>270</v>
       </c>
+      <c r="K193">
+        <v>1</v>
+      </c>
       <c r="M193" t="s">
         <v>398</v>
       </c>
@@ -8474,6 +8699,9 @@
       <c r="J194" t="s">
         <v>16</v>
       </c>
+      <c r="K194">
+        <v>1</v>
+      </c>
       <c r="L194">
         <v>40</v>
       </c>
@@ -8518,6 +8746,9 @@
       <c r="J195" t="s">
         <v>16</v>
       </c>
+      <c r="K195">
+        <v>1</v>
+      </c>
       <c r="L195">
         <v>20</v>
       </c>
@@ -8597,6 +8828,9 @@
       <c r="J197" t="s">
         <v>16</v>
       </c>
+      <c r="K197">
+        <v>1</v>
+      </c>
       <c r="L197">
         <v>15</v>
       </c>
@@ -8641,6 +8875,9 @@
       <c r="J198" t="s">
         <v>15</v>
       </c>
+      <c r="K198">
+        <v>1</v>
+      </c>
       <c r="L198">
         <v>15</v>
       </c>
@@ -8790,6 +9027,9 @@
       <c r="J202" t="s">
         <v>10</v>
       </c>
+      <c r="K202">
+        <v>1</v>
+      </c>
       <c r="L202">
         <v>20</v>
       </c>
@@ -8875,6 +9115,9 @@
       <c r="J204" t="s">
         <v>10</v>
       </c>
+      <c r="K204">
+        <v>1</v>
+      </c>
       <c r="L204">
         <v>3</v>
       </c>
@@ -8913,6 +9156,9 @@
       <c r="J205" t="s">
         <v>10</v>
       </c>
+      <c r="K205">
+        <v>1</v>
+      </c>
       <c r="L205">
         <v>4</v>
       </c>
@@ -8957,6 +9203,9 @@
       <c r="J206" t="s">
         <v>16</v>
       </c>
+      <c r="K206">
+        <v>1</v>
+      </c>
       <c r="L206">
         <v>35</v>
       </c>
@@ -8995,6 +9244,9 @@
       <c r="J207" t="s">
         <v>10</v>
       </c>
+      <c r="K207">
+        <v>1</v>
+      </c>
       <c r="L207">
         <v>1</v>
       </c>
@@ -9106,6 +9358,9 @@
       <c r="F210" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="K210">
+        <v>1</v>
+      </c>
       <c r="L210">
         <v>4</v>
       </c>
@@ -9188,6 +9443,9 @@
       <c r="J212" t="s">
         <v>10</v>
       </c>
+      <c r="K212">
+        <v>1</v>
+      </c>
       <c r="L212">
         <v>3</v>
       </c>
@@ -9223,6 +9481,9 @@
       <c r="F213" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="K213">
+        <v>1</v>
+      </c>
       <c r="L213">
         <v>15</v>
       </c>
@@ -9305,6 +9566,9 @@
       <c r="J215" t="s">
         <v>15</v>
       </c>
+      <c r="K215">
+        <v>1</v>
+      </c>
       <c r="L215">
         <v>1</v>
       </c>
@@ -9372,6 +9636,9 @@
       <c r="F217" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="K217">
+        <v>1</v>
+      </c>
       <c r="L217">
         <v>6</v>
       </c>
@@ -9644,6 +9911,9 @@
       <c r="J237" t="s">
         <v>15</v>
       </c>
+      <c r="K237">
+        <v>1</v>
+      </c>
       <c r="L237">
         <v>1</v>
       </c>
@@ -9679,6 +9949,9 @@
       <c r="J238" t="s">
         <v>10</v>
       </c>
+      <c r="K238">
+        <v>1</v>
+      </c>
       <c r="L238">
         <v>1</v>
       </c>
@@ -9717,6 +9990,9 @@
       <c r="J239" t="s">
         <v>10</v>
       </c>
+      <c r="K239">
+        <v>1</v>
+      </c>
       <c r="L239">
         <v>1</v>
       </c>
@@ -9796,6 +10072,9 @@
       <c r="J241" t="s">
         <v>15</v>
       </c>
+      <c r="K241">
+        <v>1</v>
+      </c>
       <c r="L241">
         <v>20</v>
       </c>
@@ -10232,6 +10511,9 @@
       <c r="J252" t="s">
         <v>10</v>
       </c>
+      <c r="K252">
+        <v>1</v>
+      </c>
       <c r="L252">
         <v>2</v>
       </c>
@@ -10469,6 +10751,9 @@
       <c r="J258" t="s">
         <v>10</v>
       </c>
+      <c r="K258">
+        <v>1</v>
+      </c>
       <c r="L258">
         <v>2</v>
       </c>
@@ -10507,6 +10792,9 @@
       <c r="J259" t="s">
         <v>10</v>
       </c>
+      <c r="K259">
+        <v>1</v>
+      </c>
       <c r="L259">
         <v>2</v>
       </c>
@@ -10752,6 +11040,9 @@
       </c>
       <c r="J265" t="s">
         <v>10</v>
+      </c>
+      <c r="K265">
+        <v>1</v>
       </c>
       <c r="L265">
         <v>1</v>
@@ -10821,7 +11112,9 @@
       <c r="E279" s="2">
         <v>43217.268750000003</v>
       </c>
-      <c r="F279" s="2"/>
+      <c r="F279" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="N279" s="2"/>
       <c r="O279" s="2"/>
     </row>
@@ -10841,27 +11134,47 @@
       <c r="E280" s="2">
         <v>43217.288194444445</v>
       </c>
-      <c r="F280" s="2"/>
-      <c r="N280" s="2"/>
-      <c r="O280" s="2"/>
+      <c r="F280" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N280" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="O280" s="2" t="s">
+        <v>423</v>
+      </c>
     </row>
     <row r="281" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>125</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>67</v>
+        <v>122</v>
       </c>
       <c r="C281" s="3">
-        <v>6983032356674</v>
+        <v>6983090356519</v>
       </c>
       <c r="D281" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E281" s="2">
-        <v>43217.292361111111</v>
-      </c>
-      <c r="F281" s="2"/>
+        <v>43217.288194444445</v>
+      </c>
+      <c r="F281" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G281">
+        <v>210</v>
+      </c>
+      <c r="H281">
+        <v>125</v>
+      </c>
+      <c r="I281" t="s">
+        <v>156</v>
+      </c>
+      <c r="L281">
+        <v>1</v>
+      </c>
       <c r="N281" s="2"/>
       <c r="O281" s="2"/>
     </row>
@@ -10870,18 +11183,32 @@
         <v>125</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="C282" s="3">
-        <v>6982991356782</v>
+        <v>6983032356674</v>
       </c>
       <c r="D282" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E282" s="2">
-        <v>43217.294444444444</v>
-      </c>
-      <c r="F282" s="2"/>
+        <v>43217.292361111111</v>
+      </c>
+      <c r="F282" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G282">
+        <v>15</v>
+      </c>
+      <c r="H282">
+        <v>90</v>
+      </c>
+      <c r="J282" t="s">
+        <v>16</v>
+      </c>
+      <c r="L282">
+        <v>1</v>
+      </c>
       <c r="N282" s="2"/>
       <c r="O282" s="2"/>
     </row>
@@ -10890,18 +11217,32 @@
         <v>125</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C283" s="3">
-        <v>6982916356948</v>
+        <v>6983032356674</v>
       </c>
       <c r="D283" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="E283" s="2">
-        <v>43217.296527777777</v>
-      </c>
-      <c r="F283" s="2"/>
+        <v>43217.292361111111</v>
+      </c>
+      <c r="F283" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G283">
+        <v>198</v>
+      </c>
+      <c r="H283">
+        <v>15</v>
+      </c>
+      <c r="I283" t="s">
+        <v>156</v>
+      </c>
+      <c r="L283">
+        <v>1</v>
+      </c>
       <c r="N283" s="2"/>
       <c r="O283" s="2"/>
     </row>
@@ -10910,18 +11251,20 @@
         <v>125</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>29</v>
+        <v>116</v>
       </c>
       <c r="C284" s="3">
-        <v>6982928357079</v>
+        <v>6982991356782</v>
       </c>
       <c r="D284" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E284" s="2">
-        <v>43217.298611111109</v>
-      </c>
-      <c r="F284" s="2"/>
+        <v>43217.294444444444</v>
+      </c>
+      <c r="F284" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="N284" s="2"/>
       <c r="O284" s="2"/>
     </row>
@@ -10933,15 +11276,17 @@
         <v>51</v>
       </c>
       <c r="C285" s="3">
-        <v>6982958357172</v>
+        <v>6982916356948</v>
       </c>
       <c r="D285" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="E285" s="2">
-        <v>43217.3</v>
-      </c>
-      <c r="F285" s="2"/>
+        <v>43217.296527777777</v>
+      </c>
+      <c r="F285" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="N285" s="2"/>
       <c r="O285" s="2"/>
     </row>
@@ -10950,18 +11295,32 @@
         <v>125</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C286" s="3">
-        <v>6982732357448</v>
+        <v>6982928357079</v>
       </c>
       <c r="D286" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E286" s="2">
-        <v>43217.305555555555</v>
-      </c>
-      <c r="F286" s="2"/>
+        <v>43217.298611111109</v>
+      </c>
+      <c r="F286" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G286">
+        <v>27</v>
+      </c>
+      <c r="H286">
+        <v>280</v>
+      </c>
+      <c r="I286" t="s">
+        <v>154</v>
+      </c>
+      <c r="L286">
+        <v>1</v>
+      </c>
       <c r="N286" s="2"/>
       <c r="O286" s="2"/>
     </row>
@@ -10970,18 +11329,20 @@
         <v>125</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>116</v>
+        <v>51</v>
       </c>
       <c r="C287" s="3">
-        <v>6982630357699</v>
+        <v>6982958357172</v>
       </c>
       <c r="D287" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="E287" s="2">
-        <v>43217.30972222222</v>
-      </c>
-      <c r="F287" s="2"/>
+        <v>43217.3</v>
+      </c>
+      <c r="F287" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="N287" s="2"/>
       <c r="O287" s="2"/>
     </row>
@@ -10990,18 +11351,20 @@
         <v>125</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="C288" s="3">
-        <v>6982183358919</v>
+        <v>6982732357448</v>
       </c>
       <c r="D288" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E288" s="2">
-        <v>43217.379861111112</v>
-      </c>
-      <c r="F288" s="2"/>
+        <v>43217.305555555555</v>
+      </c>
+      <c r="F288" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="N288" s="2"/>
       <c r="O288" s="2"/>
     </row>
@@ -11010,38 +11373,59 @@
         <v>125</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>35</v>
+        <v>116</v>
       </c>
       <c r="C289" s="3">
-        <v>6982114359058</v>
+        <v>6982630357699</v>
       </c>
       <c r="D289" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="E289" s="2">
-        <v>43217.384027777778</v>
-      </c>
-      <c r="F289" s="2"/>
-      <c r="N289" s="2"/>
+        <v>43217.30972222222</v>
+      </c>
+      <c r="F289" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="N289" s="2" t="s">
+        <v>424</v>
+      </c>
       <c r="O289" s="2"/>
     </row>
     <row r="290" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>125</v>
+        <v>425</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C290" s="3">
-        <v>6982006359291</v>
+        <v>6982348358299</v>
       </c>
       <c r="D290" t="s">
-        <v>240</v>
+        <v>316</v>
       </c>
       <c r="E290" s="2">
-        <v>43217.388888888891</v>
-      </c>
-      <c r="F290" s="2"/>
+        <v>43217.333333333336</v>
+      </c>
+      <c r="F290" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G290">
+        <v>117</v>
+      </c>
+      <c r="H290">
+        <v>26</v>
+      </c>
+      <c r="I290" t="s">
+        <v>153</v>
+      </c>
+      <c r="J290" t="s">
+        <v>10</v>
+      </c>
+      <c r="L290">
+        <v>1</v>
+      </c>
       <c r="N290" s="2"/>
       <c r="O290" s="2"/>
     </row>
@@ -11050,18 +11434,35 @@
         <v>125</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C291" s="3">
-        <v>6981940359461</v>
+        <v>6982183358919</v>
       </c>
       <c r="D291" t="s">
-        <v>239</v>
+        <v>306</v>
       </c>
       <c r="E291" s="2">
-        <v>43217.392361111109</v>
-      </c>
-      <c r="F291" s="2"/>
+        <v>43217.379861111112</v>
+      </c>
+      <c r="F291" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G291">
+        <v>119</v>
+      </c>
+      <c r="H291">
+        <v>330</v>
+      </c>
+      <c r="I291" t="s">
+        <v>153</v>
+      </c>
+      <c r="J291" t="s">
+        <v>15</v>
+      </c>
+      <c r="L291">
+        <v>1</v>
+      </c>
       <c r="N291" s="2"/>
       <c r="O291" s="2"/>
     </row>
@@ -11070,19 +11471,35 @@
         <v>125</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="C292" s="3">
-        <v>6981870359749</v>
+        <v>6982183358919</v>
       </c>
       <c r="D292" t="s">
-        <v>255</v>
+        <v>306</v>
       </c>
       <c r="E292" s="2">
-        <v>43217.4</v>
-      </c>
-      <c r="F292" s="2"/>
-      <c r="N292" s="2"/>
+        <v>43217.379861111112</v>
+      </c>
+      <c r="F292" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G292">
+        <v>222</v>
+      </c>
+      <c r="H292">
+        <v>112</v>
+      </c>
+      <c r="I292" t="s">
+        <v>156</v>
+      </c>
+      <c r="L292">
+        <v>1</v>
+      </c>
+      <c r="N292" s="2" t="s">
+        <v>426</v>
+      </c>
       <c r="O292" s="2"/>
     </row>
     <row r="293" spans="1:16" x14ac:dyDescent="0.2">
@@ -11090,18 +11507,35 @@
         <v>125</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="C293" s="3">
-        <v>6981921360308</v>
+        <v>6982114359058</v>
       </c>
       <c r="D293" t="s">
-        <v>214</v>
+        <v>307</v>
       </c>
       <c r="E293" s="2">
-        <v>43217.407638888886</v>
-      </c>
-      <c r="F293" s="2"/>
+        <v>43217.384027777778</v>
+      </c>
+      <c r="F293" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G293">
+        <v>63</v>
+      </c>
+      <c r="H293">
+        <v>302</v>
+      </c>
+      <c r="I293" t="s">
+        <v>153</v>
+      </c>
+      <c r="J293" t="s">
+        <v>10</v>
+      </c>
+      <c r="L293">
+        <v>2</v>
+      </c>
       <c r="N293" s="2"/>
       <c r="O293" s="2"/>
     </row>
@@ -11110,18 +11544,35 @@
         <v>125</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C294" s="3">
-        <v>6983945359739</v>
+        <v>6982006359291</v>
       </c>
       <c r="D294" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="E294" s="2">
-        <v>43217.45208333333</v>
-      </c>
-      <c r="F294" s="2"/>
+        <v>43217.388888888891</v>
+      </c>
+      <c r="F294" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G294">
+        <v>257</v>
+      </c>
+      <c r="H294">
+        <v>326</v>
+      </c>
+      <c r="I294" t="s">
+        <v>153</v>
+      </c>
+      <c r="J294" t="s">
+        <v>16</v>
+      </c>
+      <c r="L294">
+        <v>3</v>
+      </c>
       <c r="N294" s="2"/>
       <c r="O294" s="2"/>
     </row>
@@ -11130,18 +11581,35 @@
         <v>125</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C295" s="3">
-        <v>6984478359678</v>
+        <v>6981940359461</v>
       </c>
       <c r="D295" t="s">
-        <v>199</v>
+        <v>239</v>
       </c>
       <c r="E295" s="2">
-        <v>43217.461805555555</v>
-      </c>
-      <c r="F295" s="2"/>
+        <v>43217.392361111109</v>
+      </c>
+      <c r="F295" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G295">
+        <v>132</v>
+      </c>
+      <c r="H295">
+        <v>86</v>
+      </c>
+      <c r="I295" t="s">
+        <v>153</v>
+      </c>
+      <c r="J295" t="s">
+        <v>10</v>
+      </c>
+      <c r="L295">
+        <v>1</v>
+      </c>
       <c r="N295" s="2"/>
       <c r="O295" s="2"/>
     </row>
@@ -11150,18 +11618,20 @@
         <v>125</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="C296" s="3">
-        <v>6984553359647</v>
+        <v>6981870359749</v>
       </c>
       <c r="D296" t="s">
-        <v>199</v>
+        <v>255</v>
       </c>
       <c r="E296" s="2">
-        <v>43217.465277777781</v>
-      </c>
-      <c r="F296" s="2"/>
+        <v>43217.4</v>
+      </c>
+      <c r="F296" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="N296" s="2"/>
       <c r="O296" s="2"/>
     </row>
@@ -11170,18 +11640,20 @@
         <v>125</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="C297" s="3">
-        <v>6985096359518</v>
+        <v>6981921360308</v>
       </c>
       <c r="D297" t="s">
-        <v>308</v>
+        <v>214</v>
       </c>
       <c r="E297" s="2">
-        <v>43217.475694444445</v>
-      </c>
-      <c r="F297" s="2"/>
+        <v>43217.407638888886</v>
+      </c>
+      <c r="F297" s="2" t="s">
+        <v>161</v>
+      </c>
       <c r="N297" s="2"/>
     </row>
     <row r="298" spans="1:16" x14ac:dyDescent="0.2">
@@ -11189,18 +11661,32 @@
         <v>125</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C298" s="3">
-        <v>6985863359293</v>
+        <v>6981921360308</v>
       </c>
       <c r="D298" t="s">
-        <v>309</v>
+        <v>214</v>
       </c>
       <c r="E298" s="2">
-        <v>43217.490972222222</v>
-      </c>
-      <c r="F298" s="2"/>
+        <v>43217.407638888886</v>
+      </c>
+      <c r="F298" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G298">
+        <v>234</v>
+      </c>
+      <c r="H298">
+        <v>76</v>
+      </c>
+      <c r="I298" t="s">
+        <v>156</v>
+      </c>
+      <c r="L298">
+        <v>1</v>
+      </c>
       <c r="N298" s="2"/>
     </row>
     <row r="299" spans="1:16" x14ac:dyDescent="0.2">
@@ -11208,37 +11694,73 @@
         <v>125</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="C299" s="3">
-        <v>6985409358759</v>
+        <v>6983945359739</v>
       </c>
       <c r="D299" t="s">
-        <v>266</v>
+        <v>221</v>
       </c>
       <c r="E299" s="2">
-        <v>43217.513194444444</v>
-      </c>
-      <c r="F299" s="2"/>
-      <c r="N299" s="2"/>
+        <v>43217.45208333333</v>
+      </c>
+      <c r="F299" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G299">
+        <v>16</v>
+      </c>
+      <c r="H299">
+        <v>274</v>
+      </c>
+      <c r="I299" t="s">
+        <v>153</v>
+      </c>
+      <c r="J299" t="s">
+        <v>10</v>
+      </c>
+      <c r="L299">
+        <v>1</v>
+      </c>
+      <c r="N299" s="2" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="300" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>125</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="C300" s="3">
-        <v>6985041358323</v>
+        <v>6984478359678</v>
       </c>
       <c r="D300" t="s">
-        <v>278</v>
+        <v>199</v>
       </c>
       <c r="E300" s="2">
-        <v>43217.520138888889</v>
-      </c>
-      <c r="F300" s="2"/>
+        <v>43217.461805555555</v>
+      </c>
+      <c r="F300" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G300">
+        <v>78</v>
+      </c>
+      <c r="H300">
+        <v>16</v>
+      </c>
+      <c r="I300" t="s">
+        <v>153</v>
+      </c>
+      <c r="J300" t="s">
+        <v>10</v>
+      </c>
+      <c r="L300">
+        <v>1</v>
+      </c>
       <c r="N300" s="2"/>
     </row>
     <row r="301" spans="1:16" x14ac:dyDescent="0.2">
@@ -11246,259 +11768,341 @@
         <v>125</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
       <c r="C301" s="3">
-        <v>6983184356513</v>
+        <v>6984553359647</v>
       </c>
       <c r="D301" t="s">
-        <v>310</v>
+        <v>199</v>
       </c>
       <c r="E301" s="2">
-        <v>43217.554166666669</v>
-      </c>
-      <c r="F301" s="2"/>
+        <v>43217.465277777781</v>
+      </c>
+      <c r="F301" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G301">
+        <v>71</v>
+      </c>
+      <c r="H301">
+        <v>20</v>
+      </c>
+      <c r="I301" t="s">
+        <v>153</v>
+      </c>
+      <c r="J301" t="s">
+        <v>10</v>
+      </c>
+      <c r="L301">
+        <v>3</v>
+      </c>
       <c r="P301" s="2"/>
     </row>
     <row r="302" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C302" s="3">
-        <v>7005963362616</v>
+        <v>6985096359518</v>
       </c>
       <c r="D302" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="E302" s="2">
-        <v>43220.375</v>
-      </c>
-      <c r="F302" s="2"/>
+        <v>43217.475694444445</v>
+      </c>
+      <c r="F302" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G302">
+        <v>303</v>
+      </c>
+      <c r="H302">
+        <v>96</v>
+      </c>
+      <c r="I302" t="s">
+        <v>154</v>
+      </c>
+      <c r="J302" t="s">
+        <v>10</v>
+      </c>
+      <c r="L302">
+        <v>1</v>
+      </c>
+      <c r="M302" t="s">
+        <v>428</v>
+      </c>
       <c r="P302" s="2"/>
     </row>
     <row r="303" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>67</v>
+        <v>120</v>
       </c>
       <c r="C303" s="3">
-        <v>7005930362243</v>
+        <v>6985096359518</v>
       </c>
       <c r="D303" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E303" s="2">
-        <v>43220.384027777778</v>
-      </c>
-      <c r="F303" s="2"/>
+        <v>43217.475694444445</v>
+      </c>
+      <c r="F303" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G303">
+        <v>282</v>
+      </c>
+      <c r="H303">
+        <v>118</v>
+      </c>
+      <c r="I303" t="s">
+        <v>154</v>
+      </c>
+      <c r="J303" t="s">
+        <v>10</v>
+      </c>
+      <c r="L303">
+        <v>1</v>
+      </c>
       <c r="P303" s="2"/>
     </row>
     <row r="304" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="C304" s="3">
-        <v>7005887361616</v>
+        <v>6985863359293</v>
       </c>
       <c r="D304" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E304" s="2">
-        <v>43220.38958333333</v>
-      </c>
-      <c r="F304" s="2"/>
+        <v>43217.490972222222</v>
+      </c>
+      <c r="F304" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M304" t="s">
+        <v>429</v>
+      </c>
+      <c r="N304" t="s">
+        <v>430</v>
+      </c>
       <c r="O304" s="2"/>
       <c r="P304" s="2"/>
     </row>
     <row r="305" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
       <c r="C305" s="3">
-        <v>7005948361408</v>
+        <v>6985409358759</v>
       </c>
       <c r="D305" t="s">
-        <v>313</v>
+        <v>266</v>
       </c>
       <c r="E305" s="2">
-        <v>43220.393055555556</v>
-      </c>
-      <c r="F305" s="2"/>
+        <v>43217.513194444444</v>
+      </c>
+      <c r="F305" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G305">
+        <v>84</v>
+      </c>
+      <c r="H305">
+        <v>32</v>
+      </c>
+      <c r="I305" t="s">
+        <v>153</v>
+      </c>
+      <c r="J305" t="s">
+        <v>15</v>
+      </c>
+      <c r="L305">
+        <v>2</v>
+      </c>
+      <c r="M305" t="s">
+        <v>431</v>
+      </c>
       <c r="O305" s="2"/>
       <c r="P305" s="2"/>
     </row>
     <row r="306" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C306" s="3">
-        <v>7006091360439</v>
+        <v>6985041358323</v>
       </c>
       <c r="D306" t="s">
-        <v>219</v>
+        <v>278</v>
       </c>
       <c r="E306" s="2">
-        <v>43220.415277777778</v>
-      </c>
-      <c r="F306" s="2"/>
+        <v>43217.520138888889</v>
+      </c>
+      <c r="F306" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G306">
+        <v>0.98</v>
+      </c>
+      <c r="H306">
+        <v>270</v>
+      </c>
+      <c r="J306" t="s">
+        <v>15</v>
+      </c>
+      <c r="K306">
+        <v>1</v>
+      </c>
+      <c r="L306">
+        <v>15</v>
+      </c>
       <c r="O306" s="2"/>
       <c r="P306" s="2"/>
     </row>
     <row r="307" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="C307" s="3">
-        <v>7006105360299</v>
+        <v>6985041358323</v>
       </c>
       <c r="D307" t="s">
-        <v>247</v>
+        <v>278</v>
       </c>
       <c r="E307" s="2">
-        <v>43220.418055555558</v>
-      </c>
-      <c r="F307" s="2"/>
+        <v>43217.520138888889</v>
+      </c>
+      <c r="F307" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G307">
+        <v>95</v>
+      </c>
+      <c r="H307">
+        <v>108</v>
+      </c>
+      <c r="I307" t="s">
+        <v>156</v>
+      </c>
+      <c r="L307">
+        <v>1</v>
+      </c>
       <c r="O307" s="2"/>
       <c r="P307" s="2"/>
     </row>
     <row r="308" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>72</v>
+        <v>433</v>
       </c>
       <c r="C308" s="3">
-        <v>7006130360148</v>
+        <v>6984145357456</v>
       </c>
       <c r="D308" t="s">
-        <v>253</v>
+        <v>434</v>
       </c>
       <c r="E308" s="2">
-        <v>43220.422222222223</v>
-      </c>
-      <c r="F308" s="2"/>
-      <c r="M308" s="3"/>
+        <v>43217.541666666664</v>
+      </c>
+      <c r="F308" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G308">
+        <v>17</v>
+      </c>
+      <c r="H308">
+        <v>20</v>
+      </c>
+      <c r="I308" t="s">
+        <v>154</v>
+      </c>
+      <c r="J308" t="s">
+        <v>10</v>
+      </c>
+      <c r="L308">
+        <v>2</v>
+      </c>
+      <c r="M308" s="3" t="s">
+        <v>435</v>
+      </c>
       <c r="O308" s="2"/>
       <c r="P308" s="2"/>
     </row>
     <row r="309" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="C309" s="3">
-        <v>7006133360128</v>
+        <v>6983184356513</v>
       </c>
       <c r="D309" t="s">
-        <v>253</v>
+        <v>310</v>
       </c>
       <c r="E309" s="2">
-        <v>43220.424305555556</v>
-      </c>
-      <c r="F309" s="2"/>
-      <c r="M309" s="3"/>
+        <v>43217.554166666669</v>
+      </c>
+      <c r="F309" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K309">
+        <v>1</v>
+      </c>
+      <c r="L309">
+        <v>4</v>
+      </c>
+      <c r="M309" s="3" t="s">
+        <v>432</v>
+      </c>
       <c r="O309" s="2"/>
       <c r="P309" s="2"/>
     </row>
     <row r="310" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A310" t="s">
-        <v>145</v>
-      </c>
-      <c r="B310" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C310" s="3">
-        <v>7006146360075</v>
-      </c>
-      <c r="D310" t="s">
-        <v>225</v>
-      </c>
-      <c r="E310" s="2">
-        <v>43220.425694444442</v>
-      </c>
       <c r="F310" s="2"/>
       <c r="M310" s="3"/>
       <c r="O310" s="2"/>
       <c r="P310" s="2"/>
     </row>
     <row r="311" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A311" t="s">
-        <v>145</v>
-      </c>
-      <c r="B311" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C311" s="3">
-        <v>7006171360032</v>
-      </c>
-      <c r="D311" t="s">
-        <v>294</v>
-      </c>
-      <c r="E311" s="2">
-        <v>43220.427777777775</v>
-      </c>
       <c r="F311" s="2"/>
       <c r="M311" s="3"/>
       <c r="O311" s="2"/>
       <c r="P311" s="2"/>
     </row>
     <row r="312" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A312" t="s">
-        <v>145</v>
-      </c>
-      <c r="B312" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C312" s="3">
-        <v>7006203359711</v>
-      </c>
-      <c r="D312" t="s">
-        <v>233</v>
-      </c>
-      <c r="E312" s="2">
-        <v>43220.432638888888</v>
-      </c>
       <c r="F312" s="2"/>
       <c r="M312" s="3"/>
       <c r="O312" s="2"/>
       <c r="P312" s="2"/>
     </row>
     <row r="313" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A313" t="s">
-        <v>145</v>
-      </c>
-      <c r="B313" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C313" s="3">
-        <v>7006211359605</v>
-      </c>
-      <c r="D313" t="s">
-        <v>217</v>
-      </c>
-      <c r="E313" s="2">
-        <v>43220.43472222222</v>
-      </c>
       <c r="F313" s="2"/>
       <c r="M313" s="3"/>
       <c r="O313" s="2"/>
@@ -11509,18 +12113,20 @@
         <v>145</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C314" s="3">
-        <v>7006143359330</v>
+        <v>7005963362616</v>
       </c>
       <c r="D314" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="E314" s="2">
-        <v>43220.4375</v>
-      </c>
-      <c r="F314" s="2"/>
+        <v>43220.375</v>
+      </c>
+      <c r="F314" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="M314" s="3"/>
       <c r="O314" s="2"/>
       <c r="P314" s="2"/>
@@ -11530,16 +12136,16 @@
         <v>145</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="C315" s="3">
-        <v>7006114359146</v>
+        <v>7005930362243</v>
       </c>
       <c r="D315" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E315" s="2">
-        <v>43220.441666666666</v>
+        <v>43220.384027777778</v>
       </c>
       <c r="F315" s="2"/>
       <c r="M315" s="3"/>
@@ -11551,16 +12157,16 @@
         <v>145</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="C316" s="3">
-        <v>7006105359105</v>
+        <v>7005887361616</v>
       </c>
       <c r="D316" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="E316" s="2">
-        <v>43220.443055555559</v>
+        <v>43220.38958333333</v>
       </c>
       <c r="F316" s="2"/>
       <c r="M316" s="3"/>
@@ -11572,16 +12178,16 @@
         <v>145</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="C317" s="3">
-        <v>7006097359055</v>
+        <v>7005948361408</v>
       </c>
       <c r="D317" t="s">
-        <v>273</v>
+        <v>313</v>
       </c>
       <c r="E317" s="2">
-        <v>43220.445138888892</v>
+        <v>43220.393055555556</v>
       </c>
       <c r="F317" s="2"/>
       <c r="M317" s="3"/>
@@ -11593,16 +12199,16 @@
         <v>145</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="C318" s="3">
-        <v>7006092358975</v>
+        <v>7006091360439</v>
       </c>
       <c r="D318" t="s">
-        <v>307</v>
+        <v>219</v>
       </c>
       <c r="E318" s="2">
-        <v>43220.448611111111</v>
+        <v>43220.415277777778</v>
       </c>
       <c r="F318" s="2"/>
       <c r="M318" s="3"/>
@@ -11614,16 +12220,16 @@
         <v>145</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="C319" s="3">
-        <v>7006069358719</v>
+        <v>7006105360299</v>
       </c>
       <c r="D319" t="s">
-        <v>315</v>
+        <v>247</v>
       </c>
       <c r="E319" s="2">
-        <v>43220.45208333333</v>
+        <v>43220.418055555558</v>
       </c>
       <c r="F319" s="2"/>
       <c r="M319" s="3"/>
@@ -11635,16 +12241,16 @@
         <v>145</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="C320" s="3">
-        <v>7006070358639</v>
+        <v>7006130360148</v>
       </c>
       <c r="D320" t="s">
-        <v>310</v>
+        <v>253</v>
       </c>
       <c r="E320" s="2">
-        <v>43220.45416666667</v>
+        <v>43220.422222222223</v>
       </c>
       <c r="F320" s="2"/>
       <c r="M320" s="3"/>
@@ -11656,16 +12262,16 @@
         <v>145</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C321" s="3">
-        <v>7006048358564</v>
+        <v>7006133360128</v>
       </c>
       <c r="D321" t="s">
-        <v>306</v>
+        <v>253</v>
       </c>
       <c r="E321" s="2">
-        <v>43220.455555555556</v>
+        <v>43220.424305555556</v>
       </c>
       <c r="F321" s="2"/>
       <c r="M321" s="3"/>
@@ -11677,16 +12283,16 @@
         <v>145</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>128</v>
+        <v>74</v>
       </c>
       <c r="C322" s="3">
-        <v>7005966358599</v>
+        <v>7006146360075</v>
       </c>
       <c r="D322" t="s">
-        <v>316</v>
+        <v>225</v>
       </c>
       <c r="E322" s="2">
-        <v>43220.482638888891</v>
+        <v>43220.425694444442</v>
       </c>
       <c r="F322" s="2"/>
       <c r="M322" s="3"/>
@@ -11698,16 +12304,16 @@
         <v>145</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="C323" s="3">
-        <v>7005754358715</v>
+        <v>7006171360032</v>
       </c>
       <c r="D323" t="s">
-        <v>317</v>
+        <v>294</v>
       </c>
       <c r="E323" s="2">
-        <v>43220.486805555556</v>
+        <v>43220.427777777775</v>
       </c>
       <c r="F323" s="2"/>
       <c r="M323" s="3"/>
@@ -11719,16 +12325,16 @@
         <v>145</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="C324" s="3">
-        <v>7005614358794</v>
+        <v>7006203359711</v>
       </c>
       <c r="D324" t="s">
-        <v>302</v>
+        <v>233</v>
       </c>
       <c r="E324" s="2">
-        <v>43220.488888888889</v>
+        <v>43220.432638888888</v>
       </c>
       <c r="F324" s="2"/>
       <c r="M324" s="3"/>
@@ -11740,16 +12346,16 @@
         <v>145</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="C325" s="3">
-        <v>7005555358825</v>
+        <v>7006211359605</v>
       </c>
       <c r="D325" t="s">
-        <v>318</v>
+        <v>217</v>
       </c>
       <c r="E325" s="2">
-        <v>43220.490277777775</v>
+        <v>43220.43472222222</v>
       </c>
       <c r="F325" s="2"/>
       <c r="M325" s="3"/>
@@ -11761,16 +12367,16 @@
         <v>145</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C326" s="3">
-        <v>7005172359049</v>
+        <v>7006143359330</v>
       </c>
       <c r="D326" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E326" s="2">
-        <v>43220.493055555555</v>
+        <v>43220.4375</v>
       </c>
       <c r="F326" s="2"/>
       <c r="M326" s="3"/>
@@ -11782,16 +12388,16 @@
         <v>145</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="C327" s="3">
-        <v>7004845359228</v>
+        <v>7006114359146</v>
       </c>
       <c r="D327" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="E327" s="2">
-        <v>43220.49722222222</v>
+        <v>43220.441666666666</v>
       </c>
       <c r="F327" s="2"/>
       <c r="M327" s="3"/>
@@ -11803,17 +12409,18 @@
         <v>145</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C328" s="3">
-        <v>7004594359342</v>
+        <v>7006105359105</v>
       </c>
       <c r="D328" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="E328" s="2">
-        <v>43220.503472222219</v>
-      </c>
+        <v>43220.443055555559</v>
+      </c>
+      <c r="F328" s="2"/>
       <c r="M328" s="3"/>
       <c r="O328" s="2"/>
       <c r="P328" s="2"/>
@@ -11823,16 +12430,16 @@
         <v>145</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="C329" s="3">
-        <v>7004462359409</v>
+        <v>7006097359055</v>
       </c>
       <c r="D329" t="s">
-        <v>322</v>
+        <v>273</v>
       </c>
       <c r="E329" s="2">
-        <v>43220.506249999999</v>
+        <v>43220.445138888892</v>
       </c>
       <c r="M329" s="3"/>
       <c r="O329" s="2"/>
@@ -11843,16 +12450,16 @@
         <v>145</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="C330" s="3">
-        <v>7004326359594</v>
+        <v>7006092358975</v>
       </c>
       <c r="D330" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="E330" s="2">
-        <v>43220.508333333331</v>
+        <v>43220.448611111111</v>
       </c>
       <c r="M330" s="3"/>
       <c r="O330" s="2"/>
@@ -11863,16 +12470,16 @@
         <v>145</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="C331" s="3">
-        <v>7004265359557</v>
+        <v>7006069358719</v>
       </c>
       <c r="D331" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="E331" s="2">
-        <v>43220.509722222225</v>
+        <v>43220.45208333333</v>
       </c>
       <c r="M331" s="3"/>
       <c r="O331" s="2"/>
@@ -11882,16 +12489,16 @@
         <v>145</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="C332" s="3">
-        <v>7004067359659</v>
+        <v>7006070358639</v>
       </c>
       <c r="D332" t="s">
-        <v>288</v>
+        <v>310</v>
       </c>
       <c r="E332" s="2">
-        <v>43220.513194444444</v>
+        <v>43220.45416666667</v>
       </c>
       <c r="M332" s="3"/>
       <c r="O332" s="2"/>
@@ -11901,16 +12508,16 @@
         <v>145</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>133</v>
+        <v>68</v>
       </c>
       <c r="C333" s="3">
-        <v>7004008359687</v>
+        <v>7006048358564</v>
       </c>
       <c r="D333" t="s">
-        <v>325</v>
+        <v>306</v>
       </c>
       <c r="E333" s="2">
-        <v>43220.515277777777</v>
+        <v>43220.455555555556</v>
       </c>
       <c r="M333" s="3"/>
       <c r="O333" s="2"/>
@@ -11920,16 +12527,16 @@
         <v>145</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C334" s="3">
-        <v>7003441360041</v>
+        <v>7005966358599</v>
       </c>
       <c r="D334" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="E334" s="2">
-        <v>43220.525694444441</v>
+        <v>43220.482638888891</v>
       </c>
       <c r="M334" s="3"/>
     </row>
@@ -11938,16 +12545,16 @@
         <v>145</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="C335" s="3">
-        <v>7003437360048</v>
+        <v>7005754358715</v>
       </c>
       <c r="D335" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="E335" s="2">
-        <v>43220.52847222222</v>
+        <v>43220.486805555556</v>
       </c>
       <c r="M335" s="3"/>
     </row>
@@ -11956,16 +12563,16 @@
         <v>145</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C336" s="3">
-        <v>7003383360066</v>
+        <v>7005614358794</v>
       </c>
       <c r="D336" t="s">
-        <v>327</v>
+        <v>302</v>
       </c>
       <c r="E336" s="2">
-        <v>43220.53125</v>
+        <v>43220.488888888889</v>
       </c>
       <c r="M336" s="3"/>
     </row>
@@ -11974,16 +12581,16 @@
         <v>145</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C337" s="3">
-        <v>7003064360213</v>
+        <v>7005555358825</v>
       </c>
       <c r="D337" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="E337" s="2">
-        <v>43220.536111111112</v>
+        <v>43220.490277777775</v>
       </c>
       <c r="M337" s="3"/>
     </row>
@@ -11992,16 +12599,16 @@
         <v>145</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C338" s="3">
-        <v>7002924360280</v>
+        <v>7005172359049</v>
       </c>
       <c r="D338" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="E338" s="2">
-        <v>43220.539583333331</v>
+        <v>43220.493055555555</v>
       </c>
     </row>
     <row r="339" spans="1:15" x14ac:dyDescent="0.2">
@@ -12009,16 +12616,16 @@
         <v>145</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="C339" s="3">
-        <v>7002846360330</v>
+        <v>7004845359228</v>
       </c>
       <c r="D339" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="E339" s="2">
-        <v>43220.542361111111</v>
+        <v>43220.49722222222</v>
       </c>
     </row>
     <row r="340" spans="1:15" x14ac:dyDescent="0.2">
@@ -12026,16 +12633,16 @@
         <v>145</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="C340" s="3">
-        <v>7002828360337</v>
+        <v>7004594359342</v>
       </c>
       <c r="D340" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="E340" s="2">
-        <v>43220.544444444444</v>
+        <v>43220.503472222219</v>
       </c>
       <c r="O340" s="2"/>
     </row>
@@ -12044,16 +12651,16 @@
         <v>145</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>138</v>
+        <v>51</v>
       </c>
       <c r="C341" s="3">
-        <v>7002573360565</v>
+        <v>7004462359409</v>
       </c>
       <c r="D341" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="E341" s="2">
-        <v>43220.55</v>
+        <v>43220.506249999999</v>
       </c>
       <c r="O341" s="2"/>
     </row>
@@ -12062,16 +12669,16 @@
         <v>145</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="C342" s="3">
-        <v>7002551360604</v>
+        <v>7004326359594</v>
       </c>
       <c r="D342" t="s">
-        <v>304</v>
+        <v>323</v>
       </c>
       <c r="E342" s="2">
-        <v>43220.552777777775</v>
+        <v>43220.508333333331</v>
       </c>
       <c r="O342" s="2"/>
     </row>
@@ -12080,16 +12687,16 @@
         <v>145</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>139</v>
+        <v>51</v>
       </c>
       <c r="C343" s="3">
-        <v>7002731360751</v>
+        <v>7004265359557</v>
       </c>
       <c r="D343" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="E343" s="2">
-        <v>43220.55972222222</v>
+        <v>43220.509722222225</v>
       </c>
       <c r="O343" s="2"/>
     </row>
@@ -12098,16 +12705,16 @@
         <v>145</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="C344" s="3">
-        <v>7003942361654</v>
+        <v>7004067359659</v>
       </c>
       <c r="D344" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="E344" s="2">
-        <v>43220.577777777777</v>
+        <v>43220.513194444444</v>
       </c>
       <c r="L344" s="3"/>
       <c r="N344" s="2"/>
@@ -12118,16 +12725,16 @@
         <v>145</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="C345" s="3">
-        <v>7004010361690</v>
+        <v>7004008359687</v>
       </c>
       <c r="D345" t="s">
-        <v>300</v>
+        <v>325</v>
       </c>
       <c r="E345" s="2">
-        <v>43220.580555555556</v>
+        <v>43220.515277777777</v>
       </c>
       <c r="L345" s="3"/>
       <c r="N345" s="2"/>
@@ -12138,16 +12745,16 @@
         <v>145</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="C346" s="3">
-        <v>7004478361995</v>
+        <v>7003441360041</v>
       </c>
       <c r="D346" t="s">
-        <v>300</v>
+        <v>326</v>
       </c>
       <c r="E346" s="2">
-        <v>43220.63958333333</v>
+        <v>43220.525694444441</v>
       </c>
       <c r="L346" s="3"/>
       <c r="N346" s="2"/>
@@ -12158,16 +12765,16 @@
         <v>145</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>140</v>
+        <v>49</v>
       </c>
       <c r="C347" s="3">
-        <v>7004518362018</v>
+        <v>7003437360048</v>
       </c>
       <c r="D347" t="s">
-        <v>300</v>
+        <v>326</v>
       </c>
       <c r="E347" s="2">
-        <v>43220.64166666667</v>
+        <v>43220.52847222222</v>
       </c>
       <c r="L347" s="3"/>
       <c r="N347" s="2"/>
@@ -12178,16 +12785,16 @@
         <v>145</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C348" s="3">
-        <v>7004641362075</v>
+        <v>7003383360066</v>
       </c>
       <c r="D348" t="s">
-        <v>292</v>
+        <v>327</v>
       </c>
       <c r="E348" s="2">
-        <v>43220.643750000003</v>
+        <v>43220.53125</v>
       </c>
       <c r="L348" s="3"/>
       <c r="N348" s="2"/>
@@ -12198,16 +12805,16 @@
         <v>145</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C349" s="3">
-        <v>7004976362244</v>
+        <v>7003064360213</v>
       </c>
       <c r="D349" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="E349" s="2">
-        <v>43220.648611111108</v>
+        <v>43220.536111111112</v>
       </c>
       <c r="L349" s="3"/>
       <c r="N349" s="2"/>
@@ -12218,16 +12825,16 @@
         <v>145</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C350" s="3">
-        <v>7005036362271</v>
+        <v>7002924360280</v>
       </c>
       <c r="D350" t="s">
-        <v>304</v>
+        <v>328</v>
       </c>
       <c r="E350" s="2">
-        <v>43220.650694444441</v>
+        <v>43220.539583333331</v>
       </c>
       <c r="L350" s="3"/>
       <c r="N350" s="2"/>
@@ -12238,16 +12845,16 @@
         <v>145</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>144</v>
+        <v>31</v>
       </c>
       <c r="C351" s="3">
-        <v>7005401362460</v>
+        <v>7002846360330</v>
       </c>
       <c r="D351" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E351" s="2">
-        <v>43220.654861111114</v>
+        <v>43220.542361111111</v>
       </c>
       <c r="L351" s="3"/>
       <c r="N351" s="2"/>
@@ -12255,19 +12862,19 @@
     </row>
     <row r="352" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>146</v>
+        <v>33</v>
       </c>
       <c r="C352" s="3">
-        <v>7004400359209</v>
+        <v>7002828360337</v>
       </c>
       <c r="D352" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="E352" s="2">
-        <v>43221.29583333333</v>
+        <v>43220.544444444444</v>
       </c>
       <c r="L352" s="3"/>
       <c r="N352" s="2"/>
@@ -12275,19 +12882,19 @@
     </row>
     <row r="353" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>30</v>
+        <v>138</v>
       </c>
       <c r="C353" s="3">
-        <v>7003918358291</v>
+        <v>7002573360565</v>
       </c>
       <c r="D353" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="E353" s="2">
-        <v>43221.315972222219</v>
+        <v>43220.55</v>
       </c>
       <c r="L353" s="3"/>
       <c r="N353" s="2"/>
@@ -12295,19 +12902,19 @@
     </row>
     <row r="354" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="C354" s="3">
-        <v>7003782358005</v>
+        <v>7002551360604</v>
       </c>
       <c r="D354" t="s">
-        <v>325</v>
+        <v>304</v>
       </c>
       <c r="E354" s="2">
-        <v>43221.322222222225</v>
+        <v>43220.552777777775</v>
       </c>
       <c r="L354" s="3"/>
       <c r="N354" s="2"/>
@@ -12315,19 +12922,19 @@
     </row>
     <row r="355" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="C355" s="3">
-        <v>7003733357829</v>
+        <v>7002731360751</v>
       </c>
       <c r="D355" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E355" s="2">
-        <v>43221.325694444444</v>
+        <v>43220.55972222222</v>
       </c>
       <c r="L355" s="3"/>
       <c r="N355" s="2"/>
@@ -12335,19 +12942,19 @@
     </row>
     <row r="356" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="C356" s="3">
-        <v>7003632357578</v>
+        <v>7003942361654</v>
       </c>
       <c r="D356" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="E356" s="2">
-        <v>43221.329861111109</v>
+        <v>43220.577777777777</v>
       </c>
       <c r="L356" s="3"/>
       <c r="N356" s="2"/>
@@ -12355,19 +12962,19 @@
     </row>
     <row r="357" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="C357" s="3">
-        <v>7002949356265</v>
+        <v>7004010361690</v>
       </c>
       <c r="D357" t="s">
-        <v>335</v>
+        <v>300</v>
       </c>
       <c r="E357" s="2">
-        <v>43221.34375</v>
+        <v>43220.580555555556</v>
       </c>
       <c r="L357" s="3"/>
       <c r="N357" s="2"/>
@@ -12375,19 +12982,19 @@
     </row>
     <row r="358" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="C358" s="3">
-        <v>7002812355949</v>
+        <v>7004478361995</v>
       </c>
       <c r="D358" t="s">
-        <v>336</v>
+        <v>300</v>
       </c>
       <c r="E358" s="2">
-        <v>43221.348611111112</v>
+        <v>43220.63958333333</v>
       </c>
       <c r="L358" s="3"/>
       <c r="N358" s="2"/>
@@ -12395,19 +13002,19 @@
     </row>
     <row r="359" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>84</v>
+        <v>140</v>
       </c>
       <c r="C359" s="3">
-        <v>7002785355789</v>
+        <v>7004518362018</v>
       </c>
       <c r="D359" t="s">
-        <v>337</v>
+        <v>300</v>
       </c>
       <c r="E359" s="2">
-        <v>43221.351388888892</v>
+        <v>43220.64166666667</v>
       </c>
       <c r="L359" s="3"/>
       <c r="N359" s="2"/>
@@ -12415,19 +13022,19 @@
     </row>
     <row r="360" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
       <c r="C360" s="3">
-        <v>7002775355736</v>
+        <v>7004641362075</v>
       </c>
       <c r="D360" t="s">
-        <v>338</v>
+        <v>292</v>
       </c>
       <c r="E360" s="2">
-        <v>43221.354166666664</v>
+        <v>43220.643750000003</v>
       </c>
       <c r="L360" s="3"/>
       <c r="N360" s="2"/>
@@ -12435,19 +13042,19 @@
     </row>
     <row r="361" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>68</v>
+        <v>142</v>
       </c>
       <c r="C361" s="3">
-        <v>7002767355630</v>
+        <v>7004976362244</v>
       </c>
       <c r="D361" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="E361" s="2">
-        <v>43221.375694444447</v>
+        <v>43220.648611111108</v>
       </c>
       <c r="L361" s="3"/>
       <c r="N361" s="2"/>
@@ -12455,19 +13062,19 @@
     </row>
     <row r="362" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>41</v>
+        <v>143</v>
       </c>
       <c r="C362" s="3">
-        <v>7003185355743</v>
+        <v>7005036362271</v>
       </c>
       <c r="D362" t="s">
-        <v>340</v>
+        <v>304</v>
       </c>
       <c r="E362" s="2">
-        <v>43221.38958333333</v>
+        <v>43220.650694444441</v>
       </c>
       <c r="L362" s="3"/>
       <c r="N362" s="2"/>
@@ -12475,19 +13082,19 @@
     </row>
     <row r="363" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>70</v>
+        <v>144</v>
       </c>
       <c r="C363" s="3">
-        <v>7003537355760</v>
+        <v>7005401362460</v>
       </c>
       <c r="D363" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="E363" s="2">
-        <v>43221.397916666669</v>
+        <v>43220.654861111114</v>
       </c>
       <c r="L363" s="3"/>
       <c r="N363" s="2"/>
@@ -12498,16 +13105,16 @@
         <v>149</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>42</v>
+        <v>146</v>
       </c>
       <c r="C364" s="3">
-        <v>7003563355747</v>
+        <v>7004400359209</v>
       </c>
       <c r="D364" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="E364" s="2">
-        <v>43221.4</v>
+        <v>43221.29583333333</v>
       </c>
       <c r="L364" s="3"/>
       <c r="N364" s="2"/>
@@ -12518,16 +13125,16 @@
         <v>149</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C365" s="3">
-        <v>7003632355750</v>
+        <v>7003918358291</v>
       </c>
       <c r="D365" t="s">
-        <v>343</v>
+        <v>321</v>
       </c>
       <c r="E365" s="2">
-        <v>43221.404166666667</v>
+        <v>43221.315972222219</v>
       </c>
       <c r="L365" s="3"/>
       <c r="N365" s="2"/>
@@ -12538,16 +13145,16 @@
         <v>149</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C366" s="3">
-        <v>7005429356236</v>
+        <v>7003782358005</v>
       </c>
       <c r="D366" t="s">
-        <v>344</v>
+        <v>325</v>
       </c>
       <c r="E366" s="2">
-        <v>43221.426388888889</v>
+        <v>43221.322222222225</v>
       </c>
       <c r="L366" s="3"/>
       <c r="N366" s="2"/>
@@ -12558,16 +13165,16 @@
         <v>149</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C367" s="3">
-        <v>7005578356227</v>
+        <v>7003733357829</v>
       </c>
       <c r="D367" t="s">
-        <v>322</v>
+        <v>334</v>
       </c>
       <c r="E367" s="2">
-        <v>43221.431944444441</v>
+        <v>43221.325694444444</v>
       </c>
       <c r="L367" s="3"/>
       <c r="N367" s="2"/>
@@ -12578,16 +13185,16 @@
         <v>149</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C368" s="3">
-        <v>7005615356234</v>
+        <v>7003632357578</v>
       </c>
       <c r="D368" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="E368" s="2">
-        <v>43221.433333333334</v>
+        <v>43221.329861111109</v>
       </c>
       <c r="L368" s="3"/>
       <c r="N368" s="2"/>
@@ -12598,16 +13205,16 @@
         <v>149</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C369" s="3">
-        <v>7005818356285</v>
+        <v>7002949356265</v>
       </c>
       <c r="D369" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="E369" s="2">
-        <v>43221.438888888886</v>
+        <v>43221.34375</v>
       </c>
       <c r="L369" s="3"/>
       <c r="N369" s="2"/>
@@ -12618,16 +13225,16 @@
         <v>149</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>147</v>
+        <v>36</v>
       </c>
       <c r="C370" s="3">
-        <v>7005889356297</v>
+        <v>7002812355949</v>
       </c>
       <c r="D370" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="E370" s="2">
-        <v>43221.440972222219</v>
+        <v>43221.348611111112</v>
       </c>
       <c r="L370" s="3"/>
       <c r="N370" s="2"/>
@@ -12638,16 +13245,16 @@
         <v>149</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="C371" s="3">
-        <v>7005982356291</v>
+        <v>7002785355789</v>
       </c>
       <c r="D371" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="E371" s="2">
-        <v>43221.445833333331</v>
+        <v>43221.351388888892</v>
       </c>
       <c r="L371" s="3"/>
       <c r="N371" s="2"/>
@@ -12658,16 +13265,16 @@
         <v>149</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="C372" s="3">
-        <v>7006067356287</v>
+        <v>7002775355736</v>
       </c>
       <c r="D372" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="E372" s="2">
-        <v>43221.448611111111</v>
+        <v>43221.354166666664</v>
       </c>
       <c r="L372" s="3"/>
       <c r="N372" s="2"/>
@@ -12678,16 +13285,16 @@
         <v>149</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C373" s="3">
-        <v>7006110356278</v>
+        <v>7002767355630</v>
       </c>
       <c r="D373" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="E373" s="2">
-        <v>43221.45208333333</v>
+        <v>43221.375694444447</v>
       </c>
       <c r="L373" s="3"/>
       <c r="N373" s="2"/>
@@ -12698,16 +13305,16 @@
         <v>149</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C374" s="3">
-        <v>7006178356268</v>
+        <v>7003185355743</v>
       </c>
       <c r="D374" t="s">
-        <v>241</v>
+        <v>340</v>
       </c>
       <c r="E374" s="2">
-        <v>43221.455555555556</v>
+        <v>43221.38958333333</v>
       </c>
       <c r="L374" s="3"/>
       <c r="N374" s="2"/>
@@ -12718,16 +13325,16 @@
         <v>149</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="C375" s="3">
-        <v>7006451356272</v>
+        <v>7003537355760</v>
       </c>
       <c r="D375" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="E375" s="2">
-        <v>43221.461111111108</v>
+        <v>43221.397916666669</v>
       </c>
       <c r="L375" s="3"/>
       <c r="N375" s="2"/>
@@ -12738,16 +13345,16 @@
         <v>149</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="C376" s="3">
-        <v>7006803356301</v>
+        <v>7003563355747</v>
       </c>
       <c r="D376" t="s">
-        <v>245</v>
+        <v>342</v>
       </c>
       <c r="E376" s="2">
-        <v>43221.468055555553</v>
+        <v>43221.4</v>
       </c>
       <c r="L376" s="3"/>
       <c r="N376" s="2"/>
@@ -12758,16 +13365,16 @@
         <v>149</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C377" s="3">
-        <v>7006600356476</v>
+        <v>7003632355750</v>
       </c>
       <c r="D377" t="s">
-        <v>290</v>
+        <v>343</v>
       </c>
       <c r="E377" s="2">
-        <v>43221.475694444445</v>
+        <v>43221.404166666667</v>
       </c>
       <c r="L377" s="3"/>
       <c r="N377" s="2"/>
@@ -12777,16 +13384,16 @@
         <v>149</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="C378" s="3">
-        <v>7005428357911</v>
+        <v>7005429356236</v>
       </c>
       <c r="D378" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E378" s="2">
-        <v>43221.529166666667</v>
+        <v>43221.426388888889</v>
       </c>
       <c r="L378" s="3"/>
       <c r="N378" s="2"/>
@@ -12796,16 +13403,16 @@
         <v>149</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C379" s="3">
-        <v>7005274358127</v>
+        <v>7005578356227</v>
       </c>
       <c r="D379" t="s">
-        <v>291</v>
+        <v>322</v>
       </c>
       <c r="E379" s="2">
-        <v>43221.532638888886</v>
+        <v>43221.431944444441</v>
       </c>
       <c r="L379" s="3"/>
       <c r="N379" s="2"/>
@@ -12815,16 +13422,16 @@
         <v>149</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C380" s="3">
-        <v>7005214358195</v>
+        <v>7005615356234</v>
       </c>
       <c r="D380" t="s">
-        <v>351</v>
+        <v>321</v>
       </c>
       <c r="E380" s="2">
-        <v>43221.535416666666</v>
+        <v>43221.433333333334</v>
       </c>
       <c r="L380" s="3"/>
       <c r="N380" s="2"/>
@@ -12834,220 +13441,220 @@
         <v>149</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>148</v>
+        <v>71</v>
       </c>
       <c r="C381" s="3">
-        <v>7004453359147</v>
+        <v>7005818356285</v>
       </c>
       <c r="D381" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="E381" s="2">
-        <v>43221.547222222223</v>
+        <v>43221.438888888886</v>
       </c>
     </row>
     <row r="382" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C382" s="3">
-        <v>7008546366649</v>
+        <v>7005889356297</v>
       </c>
       <c r="D382" t="s">
-        <v>208</v>
+        <v>346</v>
       </c>
       <c r="E382" s="2">
-        <v>43222.325694444444</v>
+        <v>43221.440972222219</v>
       </c>
     </row>
     <row r="383" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="C383" s="3">
-        <v>7008527366619</v>
+        <v>7005982356291</v>
       </c>
       <c r="D383" t="s">
-        <v>235</v>
+        <v>346</v>
       </c>
       <c r="E383" s="2">
-        <v>43222.329861111109</v>
+        <v>43221.445833333331</v>
       </c>
     </row>
     <row r="384" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="C384" s="3">
-        <v>7008489366555</v>
+        <v>7006067356287</v>
       </c>
       <c r="D384" t="s">
-        <v>196</v>
+        <v>347</v>
       </c>
       <c r="E384" s="2">
-        <v>43222.334027777775</v>
+        <v>43221.448611111111</v>
       </c>
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="C385" s="3">
-        <v>7008481366542</v>
+        <v>7006110356278</v>
       </c>
       <c r="D385" t="s">
-        <v>223</v>
+        <v>348</v>
       </c>
       <c r="E385" s="2">
-        <v>43222.335416666669</v>
+        <v>43221.45208333333</v>
       </c>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C386" s="3">
-        <v>7008469366500</v>
+        <v>7006178356268</v>
       </c>
       <c r="D386" t="s">
-        <v>213</v>
+        <v>241</v>
       </c>
       <c r="E386" s="2">
-        <v>43222.336805555555</v>
+        <v>43221.455555555556</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C387" s="3">
-        <v>7008230366123</v>
+        <v>7006451356272</v>
       </c>
       <c r="D387" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E387" s="2">
-        <v>43222.348611111112</v>
+        <v>43221.461111111108</v>
       </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="C388" s="3">
-        <v>7008184366055</v>
+        <v>7006803356301</v>
       </c>
       <c r="D388" t="s">
-        <v>354</v>
+        <v>245</v>
       </c>
       <c r="E388" s="2">
-        <v>43222.351388888892</v>
+        <v>43221.468055555553</v>
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C389" s="3">
-        <v>7007756365256</v>
+        <v>7006600356476</v>
       </c>
       <c r="D389" t="s">
-        <v>355</v>
+        <v>290</v>
       </c>
       <c r="E389" s="2">
-        <v>43222.363888888889</v>
+        <v>43221.475694444445</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="C390" s="3">
-        <v>7007701365129</v>
+        <v>7005428357911</v>
       </c>
       <c r="D390" t="s">
-        <v>188</v>
+        <v>350</v>
       </c>
       <c r="E390" s="2">
-        <v>43222.366666666669</v>
+        <v>43221.529166666667</v>
       </c>
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C391" s="3">
-        <v>7007599364865</v>
+        <v>7005274358127</v>
       </c>
       <c r="D391" t="s">
-        <v>356</v>
+        <v>291</v>
       </c>
       <c r="E391" s="2">
-        <v>43222.37222222222</v>
+        <v>43221.532638888886</v>
       </c>
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C392" s="3">
-        <v>7007353364176</v>
+        <v>7005214358195</v>
       </c>
       <c r="D392" t="s">
-        <v>273</v>
+        <v>351</v>
       </c>
       <c r="E392" s="2">
-        <v>43222.379166666666</v>
+        <v>43221.535416666666</v>
       </c>
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>45</v>
+        <v>148</v>
       </c>
       <c r="C393" s="3">
-        <v>7007224363897</v>
+        <v>7004453359147</v>
       </c>
       <c r="D393" t="s">
-        <v>303</v>
+        <v>352</v>
       </c>
       <c r="E393" s="2">
-        <v>43222.383333333331</v>
+        <v>43221.547222222223</v>
       </c>
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.2">
@@ -13055,16 +13662,16 @@
         <v>152</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>49</v>
+        <v>150</v>
       </c>
       <c r="C394" s="3">
-        <v>7006864363345</v>
+        <v>7008546366649</v>
       </c>
       <c r="D394" t="s">
-        <v>357</v>
+        <v>208</v>
       </c>
       <c r="E394" s="2">
-        <v>43222.400000000001</v>
+        <v>43222.325694444444</v>
       </c>
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.2">
@@ -13072,16 +13679,16 @@
         <v>152</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C395" s="3">
-        <v>7006855363327</v>
+        <v>7008527366619</v>
       </c>
       <c r="D395" t="s">
-        <v>319</v>
+        <v>235</v>
       </c>
       <c r="E395" s="2">
-        <v>43222.402083333334</v>
+        <v>43222.329861111109</v>
       </c>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.2">
@@ -13089,16 +13696,16 @@
         <v>152</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="C396" s="3">
-        <v>7006741363193</v>
+        <v>7008489366555</v>
       </c>
       <c r="D396" t="s">
-        <v>358</v>
+        <v>196</v>
       </c>
       <c r="E396" s="2">
-        <v>43222.40625</v>
+        <v>43222.334027777775</v>
       </c>
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.2">
@@ -13106,16 +13713,16 @@
         <v>152</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="C397" s="3">
-        <v>7006705363181</v>
+        <v>7008481366542</v>
       </c>
       <c r="D397" t="s">
-        <v>312</v>
+        <v>223</v>
       </c>
       <c r="E397" s="2">
-        <v>43222.408333333333</v>
+        <v>43222.335416666669</v>
       </c>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.2">
@@ -13123,16 +13730,16 @@
         <v>152</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="C398" s="3">
-        <v>7006635363106</v>
+        <v>7008469366500</v>
       </c>
       <c r="D398" t="s">
-        <v>358</v>
+        <v>213</v>
       </c>
       <c r="E398" s="2">
-        <v>43222.410416666666</v>
+        <v>43222.336805555555</v>
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.2">
@@ -13140,16 +13747,16 @@
         <v>152</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="C399" s="3">
-        <v>7006632363092</v>
+        <v>7008230366123</v>
       </c>
       <c r="D399" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="E399" s="2">
-        <v>43222.412499999999</v>
+        <v>43222.348611111112</v>
       </c>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.2">
@@ -13157,16 +13764,16 @@
         <v>152</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C400" s="3">
-        <v>7006656363084</v>
+        <v>7008184366055</v>
       </c>
       <c r="D400" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="E400" s="2">
-        <v>43222.425000000003</v>
+        <v>43222.351388888892</v>
       </c>
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.2">
@@ -13174,16 +13781,16 @@
         <v>152</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="C401" s="3">
-        <v>7006704363076</v>
+        <v>7007756365256</v>
       </c>
       <c r="D401" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E401" s="2">
-        <v>43222.431944444441</v>
+        <v>43222.363888888889</v>
       </c>
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.2">
@@ -13191,16 +13798,16 @@
         <v>152</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="C402" s="3">
-        <v>7006759363054</v>
+        <v>7007701365129</v>
       </c>
       <c r="D402" t="s">
-        <v>288</v>
+        <v>188</v>
       </c>
       <c r="E402" s="2">
-        <v>43222.435416666667</v>
+        <v>43222.366666666669</v>
       </c>
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.2">
@@ -13208,16 +13815,16 @@
         <v>152</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C403" s="3">
-        <v>7006796363052</v>
+        <v>7007599364865</v>
       </c>
       <c r="D403" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E403" s="2">
-        <v>43222.436805555553</v>
+        <v>43222.37222222222</v>
       </c>
     </row>
     <row r="404" spans="1:5" x14ac:dyDescent="0.2">
@@ -13225,16 +13832,16 @@
         <v>152</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="C404" s="3">
-        <v>7006864363034</v>
+        <v>7007353364176</v>
       </c>
       <c r="D404" t="s">
-        <v>313</v>
+        <v>273</v>
       </c>
       <c r="E404" s="2">
-        <v>43222.439583333333</v>
+        <v>43222.379166666666</v>
       </c>
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.2">
@@ -13242,16 +13849,16 @@
         <v>152</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C405" s="3">
-        <v>7006882363032</v>
+        <v>7007224363897</v>
       </c>
       <c r="D405" t="s">
-        <v>361</v>
+        <v>303</v>
       </c>
       <c r="E405" s="2">
-        <v>43222.44027777778</v>
+        <v>43222.383333333331</v>
       </c>
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.2">
@@ -13259,16 +13866,16 @@
         <v>152</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C406" s="3">
-        <v>7007268362982</v>
+        <v>7006864363345</v>
       </c>
       <c r="D406" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="E406" s="2">
-        <v>43222.448611111111</v>
+        <v>43222.400000000001</v>
       </c>
     </row>
     <row r="407" spans="1:5" x14ac:dyDescent="0.2">
@@ -13276,16 +13883,16 @@
         <v>152</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C407" s="3">
-        <v>7007286362985</v>
+        <v>7006855363327</v>
       </c>
       <c r="D407" t="s">
-        <v>282</v>
+        <v>319</v>
       </c>
       <c r="E407" s="2">
-        <v>43222.450694444444</v>
+        <v>43222.402083333334</v>
       </c>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.2">
@@ -13293,16 +13900,16 @@
         <v>152</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C408" s="3">
-        <v>7007299362986</v>
+        <v>7006741363193</v>
       </c>
       <c r="D408" t="s">
-        <v>281</v>
+        <v>358</v>
       </c>
       <c r="E408" s="2">
-        <v>43222.45208333333</v>
+        <v>43222.40625</v>
       </c>
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.2">
@@ -13310,16 +13917,16 @@
         <v>152</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C409" s="3">
-        <v>7007413362958</v>
+        <v>7006705363181</v>
       </c>
       <c r="D409" t="s">
-        <v>363</v>
+        <v>312</v>
       </c>
       <c r="E409" s="2">
-        <v>43222.455555555556</v>
+        <v>43222.408333333333</v>
       </c>
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.2">
@@ -13327,16 +13934,16 @@
         <v>152</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C410" s="3">
-        <v>7009681362779</v>
+        <v>7006635363106</v>
       </c>
       <c r="D410" t="s">
-        <v>243</v>
+        <v>358</v>
       </c>
       <c r="E410" s="2">
-        <v>43222.494444444441</v>
+        <v>43222.410416666666</v>
       </c>
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.2">
@@ -13344,16 +13951,16 @@
         <v>152</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C411" s="3">
-        <v>7010638362876</v>
+        <v>7006632363092</v>
       </c>
       <c r="D411" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="E411" s="2">
-        <v>43222.50277777778</v>
+        <v>43222.412499999999</v>
       </c>
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.2">
@@ -13361,16 +13968,16 @@
         <v>152</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C412" s="3">
-        <v>7010614362913</v>
+        <v>7006656363084</v>
       </c>
       <c r="D412" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="E412" s="2">
-        <v>43222.522222222222</v>
+        <v>43222.425000000003</v>
       </c>
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.2">
@@ -13378,16 +13985,16 @@
         <v>152</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C413" s="3">
-        <v>7010584362972</v>
+        <v>7006704363076</v>
       </c>
       <c r="D413" t="s">
-        <v>278</v>
+        <v>359</v>
       </c>
       <c r="E413" s="2">
-        <v>43222.524305555555</v>
+        <v>43222.431944444441</v>
       </c>
     </row>
     <row r="414" spans="1:5" x14ac:dyDescent="0.2">
@@ -13395,16 +14002,16 @@
         <v>152</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>151</v>
+        <v>73</v>
       </c>
       <c r="C414" s="3">
-        <v>7009698364284</v>
+        <v>7006759363054</v>
       </c>
       <c r="D414" t="s">
-        <v>365</v>
+        <v>288</v>
       </c>
       <c r="E414" s="2">
-        <v>43222.599305555559</v>
+        <v>43222.435416666667</v>
       </c>
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.2">
@@ -13412,16 +14019,16 @@
         <v>152</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C415" s="3">
-        <v>7009212365539</v>
+        <v>7006796363052</v>
       </c>
       <c r="D415" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="E415" s="2">
-        <v>43222.618055555555</v>
+        <v>43222.436805555553</v>
       </c>
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.2">
@@ -13429,16 +14036,16 @@
         <v>152</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="C416" s="3">
-        <v>7009208365577</v>
+        <v>7006864363034</v>
       </c>
       <c r="D416" t="s">
-        <v>366</v>
+        <v>313</v>
       </c>
       <c r="E416" s="2">
-        <v>43222.620138888888</v>
+        <v>43222.439583333333</v>
       </c>
     </row>
     <row r="417" spans="1:5" x14ac:dyDescent="0.2">
@@ -13446,16 +14053,16 @@
         <v>152</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="C417" s="3">
-        <v>7009208365588</v>
+        <v>7006882363032</v>
       </c>
       <c r="D417" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="E417" s="2">
-        <v>43222.621527777781</v>
+        <v>43222.44027777778</v>
       </c>
     </row>
     <row r="418" spans="1:5" x14ac:dyDescent="0.2">
@@ -13463,16 +14070,16 @@
         <v>152</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="C418" s="3">
-        <v>7009199365638</v>
+        <v>7007268362982</v>
       </c>
       <c r="D418" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="E418" s="2">
-        <v>43222.623611111114</v>
+        <v>43222.448611111111</v>
       </c>
     </row>
     <row r="419" spans="1:5" x14ac:dyDescent="0.2">
@@ -13480,16 +14087,16 @@
         <v>152</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C419" s="3">
-        <v>7009186365662</v>
+        <v>7007286362985</v>
       </c>
       <c r="D419" t="s">
-        <v>369</v>
+        <v>282</v>
       </c>
       <c r="E419" s="2">
-        <v>43222.625694444447</v>
+        <v>43222.450694444444</v>
       </c>
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.2">
@@ -13497,16 +14104,16 @@
         <v>152</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="C420" s="3">
-        <v>7008623366228</v>
+        <v>7007299362986</v>
       </c>
       <c r="D420" t="s">
-        <v>184</v>
+        <v>281</v>
       </c>
       <c r="E420" s="2">
-        <v>43222.638888888891</v>
+        <v>43222.45208333333</v>
       </c>
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.2">
@@ -13514,13 +14121,16 @@
         <v>152</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="C421" s="3">
-        <v>7009183365670</v>
+        <v>7007413362958</v>
+      </c>
+      <c r="D421" t="s">
+        <v>363</v>
       </c>
       <c r="E421" s="2">
-        <v>43222.640277777777</v>
+        <v>43222.455555555556</v>
       </c>
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.2">
@@ -13528,19 +14138,220 @@
         <v>152</v>
       </c>
       <c r="B422" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C422" s="3">
+        <v>7009681362779</v>
+      </c>
+      <c r="D422" t="s">
+        <v>243</v>
+      </c>
+      <c r="E422" s="2">
+        <v>43222.494444444441</v>
+      </c>
+    </row>
+    <row r="423" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A423" t="s">
+        <v>152</v>
+      </c>
+      <c r="B423" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C423" s="3">
+        <v>7010638362876</v>
+      </c>
+      <c r="D423" t="s">
+        <v>364</v>
+      </c>
+      <c r="E423" s="2">
+        <v>43222.50277777778</v>
+      </c>
+    </row>
+    <row r="424" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A424" t="s">
+        <v>152</v>
+      </c>
+      <c r="B424" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C424" s="3">
+        <v>7010614362913</v>
+      </c>
+      <c r="D424" t="s">
+        <v>364</v>
+      </c>
+      <c r="E424" s="2">
+        <v>43222.522222222222</v>
+      </c>
+    </row>
+    <row r="425" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A425" t="s">
+        <v>152</v>
+      </c>
+      <c r="B425" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C425" s="3">
+        <v>7010584362972</v>
+      </c>
+      <c r="D425" t="s">
+        <v>278</v>
+      </c>
+      <c r="E425" s="2">
+        <v>43222.524305555555</v>
+      </c>
+    </row>
+    <row r="426" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A426" t="s">
+        <v>152</v>
+      </c>
+      <c r="B426" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C426" s="3">
+        <v>7009698364284</v>
+      </c>
+      <c r="D426" t="s">
+        <v>365</v>
+      </c>
+      <c r="E426" s="2">
+        <v>43222.599305555559</v>
+      </c>
+    </row>
+    <row r="427" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A427" t="s">
+        <v>152</v>
+      </c>
+      <c r="B427" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C427" s="3">
+        <v>7009212365539</v>
+      </c>
+      <c r="D427" t="s">
+        <v>354</v>
+      </c>
+      <c r="E427" s="2">
+        <v>43222.618055555555</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A428" t="s">
+        <v>152</v>
+      </c>
+      <c r="B428" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C428" s="3">
+        <v>7009208365577</v>
+      </c>
+      <c r="D428" t="s">
+        <v>366</v>
+      </c>
+      <c r="E428" s="2">
+        <v>43222.620138888888</v>
+      </c>
+    </row>
+    <row r="429" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A429" t="s">
+        <v>152</v>
+      </c>
+      <c r="B429" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C429" s="3">
+        <v>7009208365588</v>
+      </c>
+      <c r="D429" t="s">
+        <v>367</v>
+      </c>
+      <c r="E429" s="2">
+        <v>43222.621527777781</v>
+      </c>
+    </row>
+    <row r="430" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A430" t="s">
+        <v>152</v>
+      </c>
+      <c r="B430" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C430" s="3">
+        <v>7009199365638</v>
+      </c>
+      <c r="D430" t="s">
+        <v>368</v>
+      </c>
+      <c r="E430" s="2">
+        <v>43222.623611111114</v>
+      </c>
+    </row>
+    <row r="431" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A431" t="s">
+        <v>152</v>
+      </c>
+      <c r="B431" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C431" s="3">
+        <v>7009186365662</v>
+      </c>
+      <c r="D431" t="s">
+        <v>369</v>
+      </c>
+      <c r="E431" s="2">
+        <v>43222.625694444447</v>
+      </c>
+    </row>
+    <row r="432" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A432" t="s">
+        <v>152</v>
+      </c>
+      <c r="B432" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C432" s="3">
+        <v>7008623366228</v>
+      </c>
+      <c r="D432" t="s">
+        <v>184</v>
+      </c>
+      <c r="E432" s="2">
+        <v>43222.638888888891</v>
+      </c>
+    </row>
+    <row r="433" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A433" t="s">
+        <v>152</v>
+      </c>
+      <c r="B433" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C433" s="3">
+        <v>7009183365670</v>
+      </c>
+      <c r="E433" s="2">
+        <v>43222.640277777777</v>
+      </c>
+    </row>
+    <row r="434" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A434" t="s">
+        <v>152</v>
+      </c>
+      <c r="B434" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C422" s="3">
+      <c r="C434" s="3">
         <v>7008631366281</v>
       </c>
-      <c r="D422" t="s">
+      <c r="D434" t="s">
         <v>370</v>
       </c>
-      <c r="E422" s="2">
+      <c r="E434" s="2">
         <v>43222.640972222223</v>
       </c>
     </row>
-    <row r="438" spans="12:15" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:15" x14ac:dyDescent="0.2">
       <c r="L438" s="3"/>
       <c r="N438" s="2"/>
       <c r="O438" s="2"/>

</xml_diff>

<commit_message>
fixade vädret på 076
</commit_message>
<xml_diff>
--- a/Rawdata/riptransekter helags 2018.xlsx
+++ b/Rawdata/riptransekter helags 2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9680" yWindow="460" windowWidth="25600" windowHeight="14120" xr2:uid="{731D7839-4CAB-374B-BEA5-3406519CB6C1}"/>
+    <workbookView xWindow="1260" yWindow="460" windowWidth="25600" windowHeight="14120" xr2:uid="{731D7839-4CAB-374B-BEA5-3406519CB6C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2588" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2640" uniqueCount="457">
   <si>
     <t>vinkel</t>
   </si>
@@ -1751,9 +1751,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B9831C9-A413-654D-876F-A809696709AE}">
   <dimension ref="A1:Z445"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A299" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C403" sqref="C403"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A367" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O372" sqref="O372:O401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14080,8 +14080,12 @@
       <c r="M373" t="s">
         <v>393</v>
       </c>
-      <c r="N373" s="2"/>
-      <c r="O373" s="2"/>
+      <c r="N373" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="O373" s="2" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="374" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
@@ -14114,8 +14118,12 @@
       <c r="M374" t="s">
         <v>419</v>
       </c>
-      <c r="N374" s="2"/>
-      <c r="O374" s="2"/>
+      <c r="N374" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="O374" s="2" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="375" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
@@ -14142,8 +14150,12 @@
       <c r="L375" s="3">
         <v>1</v>
       </c>
-      <c r="N375" s="2"/>
-      <c r="O375" s="2"/>
+      <c r="N375" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="O375" s="2" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="376" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
@@ -14173,8 +14185,12 @@
       <c r="L376" s="3">
         <v>1</v>
       </c>
-      <c r="N376" s="2"/>
-      <c r="O376" s="2"/>
+      <c r="N376" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="O376" s="2" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="377" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
@@ -14201,7 +14217,12 @@
       <c r="L377" s="3">
         <v>1</v>
       </c>
-      <c r="N377" s="2"/>
+      <c r="N377" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="O377" s="2" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="378" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
@@ -14234,6 +14255,9 @@
       <c r="N378" s="2" t="s">
         <v>445</v>
       </c>
+      <c r="O378" s="2" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="379" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
@@ -14272,7 +14296,12 @@
       <c r="M379" t="s">
         <v>446</v>
       </c>
-      <c r="N379" s="2"/>
+      <c r="N379" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="O379" s="2" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="380" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
@@ -14308,7 +14337,12 @@
       <c r="L380" s="3">
         <v>1</v>
       </c>
-      <c r="N380" s="2"/>
+      <c r="N380" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="O380" s="2" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="381" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
@@ -14332,6 +14366,9 @@
       <c r="N381" t="s">
         <v>447</v>
       </c>
+      <c r="O381" s="2" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="382" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
@@ -14364,6 +14401,12 @@
       <c r="M382" t="s">
         <v>419</v>
       </c>
+      <c r="N382" t="s">
+        <v>447</v>
+      </c>
+      <c r="O382" s="2" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="383" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
@@ -14390,6 +14433,12 @@
       <c r="M383" t="s">
         <v>448</v>
       </c>
+      <c r="N383" t="s">
+        <v>447</v>
+      </c>
+      <c r="O383" s="2" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="384" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
@@ -14425,8 +14474,11 @@
       <c r="N384" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="385" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O384" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="385" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>149</v>
       </c>
@@ -14457,8 +14509,14 @@
       <c r="L385" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="386" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N385" t="s">
+        <v>450</v>
+      </c>
+      <c r="O385" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="386" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>149</v>
       </c>
@@ -14492,8 +14550,14 @@
       <c r="L386" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="387" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N386" t="s">
+        <v>450</v>
+      </c>
+      <c r="O386" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="387" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>149</v>
       </c>
@@ -14527,8 +14591,14 @@
       <c r="L387" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="388" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N387" t="s">
+        <v>450</v>
+      </c>
+      <c r="O387" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="388" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>149</v>
       </c>
@@ -14556,8 +14626,14 @@
       <c r="L388" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="389" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N388" t="s">
+        <v>450</v>
+      </c>
+      <c r="O388" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="389" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>149</v>
       </c>
@@ -14588,8 +14664,14 @@
       <c r="M389" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="390" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N389" t="s">
+        <v>450</v>
+      </c>
+      <c r="O389" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="390" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>149</v>
       </c>
@@ -14614,8 +14696,14 @@
       <c r="L390" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="391" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N390" t="s">
+        <v>450</v>
+      </c>
+      <c r="O390" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="391" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>149</v>
       </c>
@@ -14649,8 +14737,14 @@
       <c r="L391" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="392" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N391" t="s">
+        <v>450</v>
+      </c>
+      <c r="O391" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="392" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>149</v>
       </c>
@@ -14675,8 +14769,14 @@
       <c r="L392" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="393" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N392" t="s">
+        <v>450</v>
+      </c>
+      <c r="O392" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="393" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>149</v>
       </c>
@@ -14704,8 +14804,14 @@
       <c r="M393" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="394" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N393" t="s">
+        <v>450</v>
+      </c>
+      <c r="O393" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="394" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>149</v>
       </c>
@@ -14730,8 +14836,14 @@
       <c r="L394" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="395" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N394" t="s">
+        <v>450</v>
+      </c>
+      <c r="O394" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="395" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
         <v>149</v>
       </c>
@@ -14759,8 +14871,14 @@
       <c r="L395" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="396" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N395" t="s">
+        <v>450</v>
+      </c>
+      <c r="O395" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="396" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>149</v>
       </c>
@@ -14791,8 +14909,14 @@
       <c r="L396" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="397" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N396" t="s">
+        <v>450</v>
+      </c>
+      <c r="O396" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="397" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>149</v>
       </c>
@@ -14814,8 +14938,11 @@
       <c r="N397" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="398" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O397" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="398" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>149</v>
       </c>
@@ -14846,8 +14973,11 @@
       <c r="N398" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="399" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O398" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="399" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>149</v>
       </c>
@@ -14884,8 +15014,11 @@
       <c r="N399" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="400" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O399" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="400" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>149</v>
       </c>
@@ -14913,8 +15046,14 @@
       <c r="M400" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="401" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N400" t="s">
+        <v>455</v>
+      </c>
+      <c r="O400" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="401" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>149</v>
       </c>
@@ -14942,8 +15081,14 @@
       <c r="M401" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="402" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N401" t="s">
+        <v>455</v>
+      </c>
+      <c r="O401" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="402" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>152</v>
       </c>
@@ -14963,7 +15108,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="406" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>152</v>
       </c>
@@ -14980,7 +15125,7 @@
         <v>43222.325694444444</v>
       </c>
     </row>
-    <row r="407" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>152</v>
       </c>
@@ -14997,7 +15142,7 @@
         <v>43222.329861111109</v>
       </c>
     </row>
-    <row r="408" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>152</v>
       </c>
@@ -15014,7 +15159,7 @@
         <v>43222.334027777775</v>
       </c>
     </row>
-    <row r="409" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>152</v>
       </c>
@@ -15031,7 +15176,7 @@
         <v>43222.335416666669</v>
       </c>
     </row>
-    <row r="410" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>152</v>
       </c>
@@ -15048,7 +15193,7 @@
         <v>43222.336805555555</v>
       </c>
     </row>
-    <row r="411" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>152</v>
       </c>
@@ -15065,7 +15210,7 @@
         <v>43222.348611111112</v>
       </c>
     </row>
-    <row r="412" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>152</v>
       </c>
@@ -15082,7 +15227,7 @@
         <v>43222.351388888892</v>
       </c>
     </row>
-    <row r="413" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>152</v>
       </c>
@@ -15099,7 +15244,7 @@
         <v>43222.363888888889</v>
       </c>
     </row>
-    <row r="414" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>152</v>
       </c>
@@ -15116,7 +15261,7 @@
         <v>43222.366666666669</v>
       </c>
     </row>
-    <row r="415" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>152</v>
       </c>
@@ -15133,7 +15278,7 @@
         <v>43222.37222222222</v>
       </c>
     </row>
-    <row r="416" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>152</v>
       </c>

</xml_diff>

<commit_message>
hittade 3 värden som sakanades för antal fjällripor. La till dem i rådataexcelfilen.
</commit_message>
<xml_diff>
--- a/Rawdata/riptransekter helags 2018.xlsx
+++ b/Rawdata/riptransekter helags 2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="660" windowWidth="25600" windowHeight="14120" xr2:uid="{731D7839-4CAB-374B-BEA5-3406519CB6C1}"/>
+    <workbookView xWindow="4180" yWindow="1080" windowWidth="25600" windowHeight="14120" xr2:uid="{731D7839-4CAB-374B-BEA5-3406519CB6C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -1800,8 +1800,8 @@
   <dimension ref="A1:Z397"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A366" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G371" sqref="G371"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2167,6 +2167,9 @@
       <c r="J10" t="s">
         <v>15</v>
       </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
       <c r="N10" t="s">
         <v>59</v>
       </c>
@@ -3068,6 +3071,9 @@
       <c r="I36" t="s">
         <v>156</v>
       </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
       <c r="N36" t="s">
         <v>158</v>
       </c>
@@ -3105,6 +3111,9 @@
       </c>
       <c r="I37" t="s">
         <v>156</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
       </c>
       <c r="N37" t="s">
         <v>158</v>

</xml_diff>

<commit_message>
En rad på lya 096 med fel namn som åtgärdats. Lagt till lite i skriptet.
</commit_message>
<xml_diff>
--- a/Rawdata/riptransekter helags 2018.xlsx
+++ b/Rawdata/riptransekter helags 2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="1080" windowWidth="25600" windowHeight="14120" xr2:uid="{731D7839-4CAB-374B-BEA5-3406519CB6C1}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14120" xr2:uid="{731D7839-4CAB-374B-BEA5-3406519CB6C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2875" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2875" uniqueCount="472">
   <si>
     <t>vinkel</t>
   </si>
@@ -1296,9 +1296,6 @@
   </si>
   <si>
     <t>snö, lätt vind</t>
-  </si>
-  <si>
-    <t>saknar</t>
   </si>
   <si>
     <t>sol, lite snöfall</t>
@@ -1800,8 +1797,8 @@
   <dimension ref="A1:Z397"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L38" sqref="L38"/>
+      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A247" sqref="A247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11148,7 +11145,7 @@
         <v>422</v>
       </c>
       <c r="O239" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="240" spans="1:26" x14ac:dyDescent="0.2">
@@ -11186,7 +11183,7 @@
         <v>422</v>
       </c>
       <c r="O240" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="241" spans="1:15" x14ac:dyDescent="0.2">
@@ -11224,7 +11221,7 @@
         <v>422</v>
       </c>
       <c r="O241" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="242" spans="1:15" x14ac:dyDescent="0.2">
@@ -11262,7 +11259,7 @@
         <v>422</v>
       </c>
       <c r="O242" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="243" spans="1:15" x14ac:dyDescent="0.2">
@@ -11288,7 +11285,7 @@
         <v>422</v>
       </c>
       <c r="O243" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="244" spans="1:15" x14ac:dyDescent="0.2">
@@ -11314,7 +11311,7 @@
         <v>422</v>
       </c>
       <c r="O244" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="245" spans="1:15" x14ac:dyDescent="0.2">
@@ -11352,7 +11349,7 @@
         <v>422</v>
       </c>
       <c r="O245" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="246" spans="1:15" x14ac:dyDescent="0.2">
@@ -11378,7 +11375,7 @@
         <v>422</v>
       </c>
       <c r="O246" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="247" spans="1:15" x14ac:dyDescent="0.2">
@@ -11404,7 +11401,7 @@
         <v>422</v>
       </c>
       <c r="O247" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="248" spans="1:15" x14ac:dyDescent="0.2">
@@ -11430,12 +11427,12 @@
         <v>423</v>
       </c>
       <c r="O248" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="249" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>424</v>
+        <v>125</v>
       </c>
       <c r="B249" s="1" t="s">
         <v>66</v>
@@ -11471,7 +11468,7 @@
         <v>423</v>
       </c>
       <c r="O249" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="250" spans="1:15" x14ac:dyDescent="0.2">
@@ -11512,7 +11509,7 @@
         <v>423</v>
       </c>
       <c r="O250" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="251" spans="1:15" x14ac:dyDescent="0.2">
@@ -11547,10 +11544,10 @@
         <v>1</v>
       </c>
       <c r="N251" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="O251" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="252" spans="1:15" x14ac:dyDescent="0.2">
@@ -11588,10 +11585,10 @@
         <v>2</v>
       </c>
       <c r="N252" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="O252" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="253" spans="1:15" x14ac:dyDescent="0.2">
@@ -11629,10 +11626,10 @@
         <v>3</v>
       </c>
       <c r="N253" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="O253" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="254" spans="1:15" x14ac:dyDescent="0.2">
@@ -11670,10 +11667,10 @@
         <v>1</v>
       </c>
       <c r="N254" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="O254" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="255" spans="1:15" x14ac:dyDescent="0.2">
@@ -11696,10 +11693,10 @@
         <v>51</v>
       </c>
       <c r="N255" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="O255" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="256" spans="1:15" x14ac:dyDescent="0.2">
@@ -11722,10 +11719,10 @@
         <v>161</v>
       </c>
       <c r="N256" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="O256" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="257" spans="1:16" x14ac:dyDescent="0.2">
@@ -11760,10 +11757,10 @@
         <v>1</v>
       </c>
       <c r="N257" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="O257" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="258" spans="1:16" x14ac:dyDescent="0.2">
@@ -11801,10 +11798,10 @@
         <v>1</v>
       </c>
       <c r="N258" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="O258" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="259" spans="1:16" x14ac:dyDescent="0.2">
@@ -11842,10 +11839,10 @@
         <v>1</v>
       </c>
       <c r="N259" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="O259" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="260" spans="1:16" x14ac:dyDescent="0.2">
@@ -11883,10 +11880,10 @@
         <v>3</v>
       </c>
       <c r="N260" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="O260" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="P260" s="2"/>
     </row>
@@ -11925,13 +11922,13 @@
         <v>1</v>
       </c>
       <c r="M261" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="N261" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="O261" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="P261" s="2"/>
     </row>
@@ -11970,10 +11967,10 @@
         <v>1</v>
       </c>
       <c r="N262" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="O262" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="P262" s="2"/>
     </row>
@@ -11997,13 +11994,13 @@
         <v>161</v>
       </c>
       <c r="M263" t="s">
+        <v>427</v>
+      </c>
+      <c r="N263" t="s">
         <v>428</v>
       </c>
-      <c r="N263" t="s">
-        <v>429</v>
-      </c>
       <c r="O263" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="P263" s="2"/>
     </row>
@@ -12042,13 +12039,13 @@
         <v>2</v>
       </c>
       <c r="M264" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="N264" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="O264" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="P264" s="2"/>
     </row>
@@ -12087,10 +12084,10 @@
         <v>15</v>
       </c>
       <c r="N265" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="O265" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="P265" s="2"/>
     </row>
@@ -12126,10 +12123,10 @@
         <v>1</v>
       </c>
       <c r="N266" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="O266" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="P266" s="2"/>
     </row>
@@ -12138,13 +12135,13 @@
         <v>125</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C267" s="3">
         <v>6984145357456</v>
       </c>
       <c r="D267" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E267" s="2">
         <v>43217.541666666664</v>
@@ -12168,13 +12165,13 @@
         <v>2</v>
       </c>
       <c r="M267" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="N267" t="s">
         <v>434</v>
       </c>
-      <c r="N267" t="s">
+      <c r="O267" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="O267" s="2" t="s">
-        <v>436</v>
       </c>
       <c r="P267" s="2"/>
     </row>
@@ -12204,13 +12201,13 @@
         <v>4</v>
       </c>
       <c r="M268" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="N268" t="s">
+        <v>434</v>
+      </c>
+      <c r="O268" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="O268" s="2" t="s">
-        <v>436</v>
       </c>
       <c r="P268" s="2"/>
     </row>
@@ -12235,10 +12232,10 @@
       </c>
       <c r="M269" s="3"/>
       <c r="N269" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="O269" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="P269" s="2"/>
     </row>
@@ -12269,10 +12266,10 @@
       </c>
       <c r="M270" s="3"/>
       <c r="N270" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="O270" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="P270" s="2"/>
     </row>
@@ -12297,10 +12294,10 @@
       </c>
       <c r="M271" s="3"/>
       <c r="N271" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="O271" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="P271" s="2"/>
     </row>
@@ -12331,10 +12328,10 @@
       </c>
       <c r="M272" s="3"/>
       <c r="N272" t="s">
+        <v>441</v>
+      </c>
+      <c r="O272" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O272" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="P272" s="2"/>
     </row>
@@ -12365,10 +12362,10 @@
       </c>
       <c r="M273" s="3"/>
       <c r="N273" t="s">
+        <v>441</v>
+      </c>
+      <c r="O273" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O273" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="P273" s="2"/>
     </row>
@@ -12405,10 +12402,10 @@
       </c>
       <c r="M274" s="3"/>
       <c r="N274" t="s">
+        <v>441</v>
+      </c>
+      <c r="O274" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O274" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="P274" s="2"/>
     </row>
@@ -12439,10 +12436,10 @@
       </c>
       <c r="M275" s="3"/>
       <c r="N275" t="s">
+        <v>441</v>
+      </c>
+      <c r="O275" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O275" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="P275" s="2"/>
     </row>
@@ -12473,10 +12470,10 @@
       </c>
       <c r="M276" s="3"/>
       <c r="N276" t="s">
+        <v>441</v>
+      </c>
+      <c r="O276" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O276" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="P276" s="2"/>
     </row>
@@ -12507,10 +12504,10 @@
       </c>
       <c r="M277" s="3"/>
       <c r="N277" t="s">
+        <v>441</v>
+      </c>
+      <c r="O277" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O277" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="P277" s="2"/>
     </row>
@@ -12541,10 +12538,10 @@
       </c>
       <c r="M278" s="3"/>
       <c r="N278" t="s">
+        <v>441</v>
+      </c>
+      <c r="O278" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O278" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="P278" s="2"/>
     </row>
@@ -12583,13 +12580,13 @@
         <v>1</v>
       </c>
       <c r="M279" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N279" t="s">
+        <v>441</v>
+      </c>
+      <c r="O279" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O279" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="P279" s="2"/>
     </row>
@@ -12620,10 +12617,10 @@
       </c>
       <c r="M280" s="3"/>
       <c r="N280" t="s">
+        <v>441</v>
+      </c>
+      <c r="O280" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O280" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="P280" s="2"/>
     </row>
@@ -12654,10 +12651,10 @@
       </c>
       <c r="M281" s="3"/>
       <c r="N281" t="s">
+        <v>441</v>
+      </c>
+      <c r="O281" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O281" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="P281" s="2"/>
     </row>
@@ -12697,10 +12694,10 @@
       </c>
       <c r="M282" s="3"/>
       <c r="N282" t="s">
+        <v>441</v>
+      </c>
+      <c r="O282" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O282" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="P282" s="2"/>
     </row>
@@ -12737,10 +12734,10 @@
       </c>
       <c r="M283" s="3"/>
       <c r="N283" t="s">
+        <v>441</v>
+      </c>
+      <c r="O283" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O283" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="P283" s="2"/>
     </row>
@@ -12777,10 +12774,10 @@
       </c>
       <c r="M284" s="3"/>
       <c r="N284" t="s">
+        <v>441</v>
+      </c>
+      <c r="O284" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O284" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="P284" s="2"/>
     </row>
@@ -12811,10 +12808,10 @@
       </c>
       <c r="M285" s="3"/>
       <c r="N285" t="s">
+        <v>441</v>
+      </c>
+      <c r="O285" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O285" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="P285" s="2"/>
     </row>
@@ -12845,10 +12842,10 @@
       </c>
       <c r="M286" s="3"/>
       <c r="N286" t="s">
+        <v>441</v>
+      </c>
+      <c r="O286" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O286" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="287" spans="1:16" x14ac:dyDescent="0.2">
@@ -12878,10 +12875,10 @@
       </c>
       <c r="M287" s="3"/>
       <c r="N287" t="s">
+        <v>441</v>
+      </c>
+      <c r="O287" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O287" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="288" spans="1:16" x14ac:dyDescent="0.2">
@@ -12905,10 +12902,10 @@
       </c>
       <c r="M288" s="3"/>
       <c r="N288" t="s">
+        <v>441</v>
+      </c>
+      <c r="O288" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O288" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="289" spans="1:15" x14ac:dyDescent="0.2">
@@ -12938,10 +12935,10 @@
       </c>
       <c r="M289" s="3"/>
       <c r="N289" t="s">
+        <v>441</v>
+      </c>
+      <c r="O289" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O289" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="290" spans="1:15" x14ac:dyDescent="0.2">
@@ -12970,13 +12967,13 @@
         <v>2</v>
       </c>
       <c r="M290" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="N290" t="s">
+        <v>441</v>
+      </c>
+      <c r="O290" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O290" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="291" spans="1:15" x14ac:dyDescent="0.2">
@@ -13006,10 +13003,10 @@
       </c>
       <c r="M291" s="3"/>
       <c r="N291" t="s">
+        <v>441</v>
+      </c>
+      <c r="O291" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O291" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="292" spans="1:15" x14ac:dyDescent="0.2">
@@ -13039,10 +13036,10 @@
       </c>
       <c r="M292" s="3"/>
       <c r="N292" t="s">
+        <v>441</v>
+      </c>
+      <c r="O292" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O292" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="293" spans="1:15" x14ac:dyDescent="0.2">
@@ -13071,13 +13068,13 @@
         <v>1</v>
       </c>
       <c r="M293" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="N293" t="s">
+        <v>441</v>
+      </c>
+      <c r="O293" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O293" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="294" spans="1:15" x14ac:dyDescent="0.2">
@@ -13106,10 +13103,10 @@
         <v>1</v>
       </c>
       <c r="N294" t="s">
+        <v>441</v>
+      </c>
+      <c r="O294" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O294" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="295" spans="1:15" x14ac:dyDescent="0.2">
@@ -13138,10 +13135,10 @@
         <v>1</v>
       </c>
       <c r="N295" t="s">
+        <v>441</v>
+      </c>
+      <c r="O295" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O295" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="296" spans="1:15" x14ac:dyDescent="0.2">
@@ -13164,10 +13161,10 @@
         <v>51</v>
       </c>
       <c r="N296" t="s">
+        <v>441</v>
+      </c>
+      <c r="O296" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O296" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="297" spans="1:15" x14ac:dyDescent="0.2">
@@ -13190,10 +13187,10 @@
         <v>51</v>
       </c>
       <c r="N297" t="s">
+        <v>441</v>
+      </c>
+      <c r="O297" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O297" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="298" spans="1:15" x14ac:dyDescent="0.2">
@@ -13216,10 +13213,10 @@
         <v>51</v>
       </c>
       <c r="N298" t="s">
+        <v>441</v>
+      </c>
+      <c r="O298" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O298" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="299" spans="1:15" x14ac:dyDescent="0.2">
@@ -13248,10 +13245,10 @@
         <v>2</v>
       </c>
       <c r="N299" t="s">
+        <v>441</v>
+      </c>
+      <c r="O299" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O299" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="300" spans="1:15" x14ac:dyDescent="0.2">
@@ -13280,10 +13277,10 @@
         <v>2</v>
       </c>
       <c r="N300" t="s">
+        <v>441</v>
+      </c>
+      <c r="O300" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O300" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="301" spans="1:15" x14ac:dyDescent="0.2">
@@ -13312,13 +13309,13 @@
         <v>2</v>
       </c>
       <c r="M301" t="s">
+        <v>440</v>
+      </c>
+      <c r="N301" t="s">
         <v>441</v>
       </c>
-      <c r="N301" t="s">
+      <c r="O301" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O301" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="302" spans="1:15" x14ac:dyDescent="0.2">
@@ -13356,10 +13353,10 @@
         <v>2</v>
       </c>
       <c r="N302" t="s">
+        <v>441</v>
+      </c>
+      <c r="O302" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O302" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="303" spans="1:15" x14ac:dyDescent="0.2">
@@ -13388,13 +13385,13 @@
         <v>3</v>
       </c>
       <c r="M303" t="s">
+        <v>440</v>
+      </c>
+      <c r="N303" t="s">
         <v>441</v>
       </c>
-      <c r="N303" t="s">
+      <c r="O303" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O303" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="304" spans="1:15" x14ac:dyDescent="0.2">
@@ -13426,10 +13423,10 @@
         <v>1</v>
       </c>
       <c r="N304" t="s">
+        <v>441</v>
+      </c>
+      <c r="O304" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O304" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="305" spans="1:15" x14ac:dyDescent="0.2">
@@ -13458,10 +13455,10 @@
         <v>1</v>
       </c>
       <c r="N305" t="s">
+        <v>441</v>
+      </c>
+      <c r="O305" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O305" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="306" spans="1:15" x14ac:dyDescent="0.2">
@@ -13496,10 +13493,10 @@
         <v>23</v>
       </c>
       <c r="N306" t="s">
+        <v>441</v>
+      </c>
+      <c r="O306" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O306" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="307" spans="1:15" x14ac:dyDescent="0.2">
@@ -13534,10 +13531,10 @@
         <v>23</v>
       </c>
       <c r="N307" t="s">
+        <v>441</v>
+      </c>
+      <c r="O307" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O307" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="308" spans="1:15" x14ac:dyDescent="0.2">
@@ -13572,10 +13569,10 @@
         <v>1</v>
       </c>
       <c r="N308" t="s">
+        <v>441</v>
+      </c>
+      <c r="O308" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O308" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="309" spans="1:15" x14ac:dyDescent="0.2">
@@ -13599,10 +13596,10 @@
       </c>
       <c r="L309" s="3"/>
       <c r="N309" t="s">
+        <v>441</v>
+      </c>
+      <c r="O309" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O309" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="310" spans="1:15" x14ac:dyDescent="0.2">
@@ -13631,10 +13628,10 @@
         <v>2</v>
       </c>
       <c r="N310" t="s">
+        <v>441</v>
+      </c>
+      <c r="O310" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O310" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="311" spans="1:15" x14ac:dyDescent="0.2">
@@ -13672,10 +13669,10 @@
         <v>1</v>
       </c>
       <c r="N311" t="s">
+        <v>441</v>
+      </c>
+      <c r="O311" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O311" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="312" spans="1:15" x14ac:dyDescent="0.2">
@@ -13704,10 +13701,10 @@
         <v>4</v>
       </c>
       <c r="N312" t="s">
+        <v>441</v>
+      </c>
+      <c r="O312" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O312" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="313" spans="1:15" x14ac:dyDescent="0.2">
@@ -13736,10 +13733,10 @@
         <v>2</v>
       </c>
       <c r="N313" t="s">
+        <v>441</v>
+      </c>
+      <c r="O313" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O313" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="314" spans="1:15" x14ac:dyDescent="0.2">
@@ -13768,10 +13765,10 @@
         <v>2</v>
       </c>
       <c r="N314" t="s">
+        <v>441</v>
+      </c>
+      <c r="O314" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O314" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="315" spans="1:15" x14ac:dyDescent="0.2">
@@ -13800,10 +13797,10 @@
         <v>2</v>
       </c>
       <c r="N315" t="s">
+        <v>441</v>
+      </c>
+      <c r="O315" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O315" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="316" spans="1:15" x14ac:dyDescent="0.2">
@@ -13832,10 +13829,10 @@
         <v>1</v>
       </c>
       <c r="N316" t="s">
+        <v>441</v>
+      </c>
+      <c r="O316" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O316" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="317" spans="1:15" x14ac:dyDescent="0.2">
@@ -13864,10 +13861,10 @@
         <v>5</v>
       </c>
       <c r="N317" t="s">
+        <v>441</v>
+      </c>
+      <c r="O317" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O317" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="318" spans="1:15" x14ac:dyDescent="0.2">
@@ -13896,10 +13893,10 @@
         <v>1</v>
       </c>
       <c r="N318" t="s">
+        <v>441</v>
+      </c>
+      <c r="O318" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="O318" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="319" spans="1:15" x14ac:dyDescent="0.2">
@@ -13923,10 +13920,10 @@
       </c>
       <c r="L319" s="3"/>
       <c r="N319" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="O319" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="O319" s="2" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="320" spans="1:15" x14ac:dyDescent="0.2">
@@ -13961,10 +13958,10 @@
         <v>394</v>
       </c>
       <c r="N320" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="O320" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="O320" s="2" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="321" spans="1:15" x14ac:dyDescent="0.2">
@@ -13999,10 +13996,10 @@
         <v>420</v>
       </c>
       <c r="N321" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="O321" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="O321" s="2" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="322" spans="1:15" x14ac:dyDescent="0.2">
@@ -14031,10 +14028,10 @@
         <v>1</v>
       </c>
       <c r="N322" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="O322" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="O322" s="2" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="323" spans="1:15" x14ac:dyDescent="0.2">
@@ -14066,10 +14063,10 @@
         <v>1</v>
       </c>
       <c r="N323" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="O323" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="O323" s="2" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="324" spans="1:15" x14ac:dyDescent="0.2">
@@ -14098,10 +14095,10 @@
         <v>1</v>
       </c>
       <c r="N324" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="O324" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="O324" s="2" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="325" spans="1:15" x14ac:dyDescent="0.2">
@@ -14133,10 +14130,10 @@
         <v>30</v>
       </c>
       <c r="N325" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="O325" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="326" spans="1:15" x14ac:dyDescent="0.2">
@@ -14174,13 +14171,13 @@
         <v>2</v>
       </c>
       <c r="M326" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="N326" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="O326" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="327" spans="1:15" x14ac:dyDescent="0.2">
@@ -14218,10 +14215,10 @@
         <v>1</v>
       </c>
       <c r="N327" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="O327" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="328" spans="1:15" x14ac:dyDescent="0.2">
@@ -14244,10 +14241,10 @@
         <v>161</v>
       </c>
       <c r="N328" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="O328" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="329" spans="1:15" x14ac:dyDescent="0.2">
@@ -14282,10 +14279,10 @@
         <v>420</v>
       </c>
       <c r="N329" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="O329" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="330" spans="1:15" x14ac:dyDescent="0.2">
@@ -14311,13 +14308,13 @@
         <v>1</v>
       </c>
       <c r="M330" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="N330" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="O330" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="331" spans="1:15" x14ac:dyDescent="0.2">
@@ -14349,13 +14346,13 @@
         <v>2</v>
       </c>
       <c r="M331" t="s">
+        <v>449</v>
+      </c>
+      <c r="N331" t="s">
         <v>450</v>
       </c>
-      <c r="N331" t="s">
-        <v>451</v>
-      </c>
       <c r="O331" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="332" spans="1:15" x14ac:dyDescent="0.2">
@@ -14390,10 +14387,10 @@
         <v>1</v>
       </c>
       <c r="N332" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O332" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="333" spans="1:15" x14ac:dyDescent="0.2">
@@ -14431,10 +14428,10 @@
         <v>2</v>
       </c>
       <c r="N333" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O333" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="334" spans="1:15" x14ac:dyDescent="0.2">
@@ -14472,10 +14469,10 @@
         <v>2</v>
       </c>
       <c r="N334" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O334" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="335" spans="1:15" x14ac:dyDescent="0.2">
@@ -14507,10 +14504,10 @@
         <v>2</v>
       </c>
       <c r="N335" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O335" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="336" spans="1:15" x14ac:dyDescent="0.2">
@@ -14545,10 +14542,10 @@
         <v>394</v>
       </c>
       <c r="N336" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O336" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="337" spans="1:15" x14ac:dyDescent="0.2">
@@ -14577,10 +14574,10 @@
         <v>1</v>
       </c>
       <c r="N337" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O337" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="338" spans="1:15" x14ac:dyDescent="0.2">
@@ -14618,10 +14615,10 @@
         <v>1</v>
       </c>
       <c r="N338" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O338" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="339" spans="1:15" x14ac:dyDescent="0.2">
@@ -14650,10 +14647,10 @@
         <v>1</v>
       </c>
       <c r="N339" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O339" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="340" spans="1:15" x14ac:dyDescent="0.2">
@@ -14682,13 +14679,13 @@
         <v>5</v>
       </c>
       <c r="M340" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="N340" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O340" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="341" spans="1:15" x14ac:dyDescent="0.2">
@@ -14717,10 +14714,10 @@
         <v>1</v>
       </c>
       <c r="N341" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O341" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="342" spans="1:15" x14ac:dyDescent="0.2">
@@ -14752,10 +14749,10 @@
         <v>1</v>
       </c>
       <c r="N342" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O342" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="343" spans="1:15" x14ac:dyDescent="0.2">
@@ -14790,10 +14787,10 @@
         <v>2</v>
       </c>
       <c r="N343" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O343" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="344" spans="1:15" x14ac:dyDescent="0.2">
@@ -14816,10 +14813,10 @@
         <v>161</v>
       </c>
       <c r="N344" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="O344" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="345" spans="1:15" x14ac:dyDescent="0.2">
@@ -14848,13 +14845,13 @@
         <v>15</v>
       </c>
       <c r="M345" t="s">
+        <v>453</v>
+      </c>
+      <c r="N345" t="s">
         <v>454</v>
       </c>
-      <c r="N345" t="s">
-        <v>455</v>
-      </c>
       <c r="O345" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="346" spans="1:15" x14ac:dyDescent="0.2">
@@ -14892,10 +14889,10 @@
         <v>2</v>
       </c>
       <c r="N346" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="O346" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="347" spans="1:15" x14ac:dyDescent="0.2">
@@ -14927,10 +14924,10 @@
         <v>393</v>
       </c>
       <c r="N347" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="O347" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="348" spans="1:15" x14ac:dyDescent="0.2">
@@ -14959,13 +14956,13 @@
         <v>20</v>
       </c>
       <c r="M348" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="N348" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="O348" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="349" spans="1:15" x14ac:dyDescent="0.2">
@@ -15040,10 +15037,10 @@
         <v>1</v>
       </c>
       <c r="N351" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O351" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="352" spans="1:15" x14ac:dyDescent="0.2">
@@ -15075,13 +15072,13 @@
         <v>3</v>
       </c>
       <c r="M352" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="N352" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O352" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="353" spans="1:15" x14ac:dyDescent="0.2">
@@ -15116,10 +15113,10 @@
         <v>23</v>
       </c>
       <c r="N353" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O353" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="354" spans="1:15" x14ac:dyDescent="0.2">
@@ -15154,10 +15151,10 @@
         <v>23</v>
       </c>
       <c r="N354" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O354" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="355" spans="1:15" x14ac:dyDescent="0.2">
@@ -15192,10 +15189,10 @@
         <v>23</v>
       </c>
       <c r="N355" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O355" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="356" spans="1:15" x14ac:dyDescent="0.2">
@@ -15230,10 +15227,10 @@
         <v>23</v>
       </c>
       <c r="N356" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O356" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="357" spans="1:15" x14ac:dyDescent="0.2">
@@ -15268,10 +15265,10 @@
         <v>392</v>
       </c>
       <c r="N357" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O357" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="358" spans="1:15" x14ac:dyDescent="0.2">
@@ -15306,10 +15303,10 @@
         <v>23</v>
       </c>
       <c r="N358" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O358" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="359" spans="1:15" x14ac:dyDescent="0.2">
@@ -15347,10 +15344,10 @@
         <v>1</v>
       </c>
       <c r="N359" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O359" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="360" spans="1:15" x14ac:dyDescent="0.2">
@@ -15385,10 +15382,10 @@
         <v>1</v>
       </c>
       <c r="N360" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O360" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="361" spans="1:15" x14ac:dyDescent="0.2">
@@ -15423,10 +15420,10 @@
         <v>1</v>
       </c>
       <c r="N361" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O361" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="362" spans="1:15" x14ac:dyDescent="0.2">
@@ -15464,10 +15461,10 @@
         <v>2</v>
       </c>
       <c r="N362" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O362" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="363" spans="1:15" x14ac:dyDescent="0.2">
@@ -15502,10 +15499,10 @@
         <v>1</v>
       </c>
       <c r="N363" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O363" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="364" spans="1:15" x14ac:dyDescent="0.2">
@@ -15534,13 +15531,13 @@
         <v>6</v>
       </c>
       <c r="M364" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="N364" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O364" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="365" spans="1:15" x14ac:dyDescent="0.2">
@@ -15575,10 +15572,10 @@
         <v>1</v>
       </c>
       <c r="N365" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O365" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="366" spans="1:15" x14ac:dyDescent="0.2">
@@ -15610,13 +15607,13 @@
         <v>20</v>
       </c>
       <c r="M366" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="N366" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O366" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="367" spans="1:15" x14ac:dyDescent="0.2">
@@ -15645,13 +15642,13 @@
         <v>1</v>
       </c>
       <c r="M367" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="N367" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O367" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="368" spans="1:15" x14ac:dyDescent="0.2">
@@ -15680,10 +15677,10 @@
         <v>1</v>
       </c>
       <c r="N368" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O368" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="369" spans="1:15" x14ac:dyDescent="0.2">
@@ -15712,10 +15709,10 @@
         <v>3</v>
       </c>
       <c r="N369" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O369" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="370" spans="1:15" x14ac:dyDescent="0.2">
@@ -15738,10 +15735,10 @@
         <v>161</v>
       </c>
       <c r="N370" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O370" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="371" spans="1:15" x14ac:dyDescent="0.2">
@@ -15779,10 +15776,10 @@
         <v>1</v>
       </c>
       <c r="N371" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O371" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="372" spans="1:15" x14ac:dyDescent="0.2">
@@ -15814,13 +15811,13 @@
         <v>30</v>
       </c>
       <c r="M372" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N372" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O372" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="373" spans="1:15" x14ac:dyDescent="0.2">
@@ -15849,13 +15846,13 @@
         <v>8</v>
       </c>
       <c r="M373" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="N373" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O373" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="374" spans="1:15" x14ac:dyDescent="0.2">
@@ -15884,13 +15881,13 @@
         <v>3</v>
       </c>
       <c r="M374" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="N374" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O374" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="375" spans="1:15" x14ac:dyDescent="0.2">
@@ -15919,13 +15916,13 @@
         <v>4</v>
       </c>
       <c r="M375" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="N375" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O375" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="376" spans="1:15" x14ac:dyDescent="0.2">
@@ -15954,13 +15951,13 @@
         <v>1</v>
       </c>
       <c r="M376" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="N376" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O376" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="377" spans="1:15" x14ac:dyDescent="0.2">
@@ -15992,13 +15989,13 @@
         <v>4</v>
       </c>
       <c r="M377" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="N377" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O377" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="378" spans="1:15" x14ac:dyDescent="0.2">
@@ -16030,13 +16027,13 @@
         <v>20</v>
       </c>
       <c r="M378" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="N378" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O378" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="379" spans="1:15" x14ac:dyDescent="0.2">
@@ -16071,10 +16068,10 @@
         <v>23</v>
       </c>
       <c r="N379" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O379" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="380" spans="1:15" x14ac:dyDescent="0.2">
@@ -16106,13 +16103,13 @@
         <v>10</v>
       </c>
       <c r="M380" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="N380" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O380" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="381" spans="1:15" x14ac:dyDescent="0.2">
@@ -16147,10 +16144,10 @@
         <v>392</v>
       </c>
       <c r="N381" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O381" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="382" spans="1:15" x14ac:dyDescent="0.2">
@@ -16188,10 +16185,10 @@
         <v>2</v>
       </c>
       <c r="N382" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O382" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="383" spans="1:15" x14ac:dyDescent="0.2">
@@ -16226,10 +16223,10 @@
         <v>1</v>
       </c>
       <c r="N383" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O383" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="384" spans="1:15" x14ac:dyDescent="0.2">
@@ -16252,10 +16249,10 @@
         <v>161</v>
       </c>
       <c r="N384" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O384" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="385" spans="1:15" x14ac:dyDescent="0.2">
@@ -16293,10 +16290,10 @@
         <v>1</v>
       </c>
       <c r="N385" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O385" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="386" spans="1:15" x14ac:dyDescent="0.2">
@@ -16331,10 +16328,10 @@
         <v>23</v>
       </c>
       <c r="N386" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="O386" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="387" spans="1:15" x14ac:dyDescent="0.2">
@@ -16357,10 +16354,10 @@
         <v>151</v>
       </c>
       <c r="N387" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="O387" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="388" spans="1:15" x14ac:dyDescent="0.2">
@@ -16392,13 +16389,13 @@
         <v>5</v>
       </c>
       <c r="M388" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="N388" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="O388" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="389" spans="1:15" x14ac:dyDescent="0.2">
@@ -16430,13 +16427,13 @@
         <v>2</v>
       </c>
       <c r="M389" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="N389" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="O389" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="390" spans="1:15" x14ac:dyDescent="0.2">
@@ -16468,13 +16465,13 @@
         <v>40</v>
       </c>
       <c r="M390" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="N390" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="O390" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="391" spans="1:15" x14ac:dyDescent="0.2">
@@ -16506,13 +16503,13 @@
         <v>20</v>
       </c>
       <c r="M391" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N391" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="O391" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="392" spans="1:15" x14ac:dyDescent="0.2">
@@ -16544,13 +16541,13 @@
         <v>20</v>
       </c>
       <c r="M392" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="N392" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="O392" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="393" spans="1:15" x14ac:dyDescent="0.2">
@@ -16585,10 +16582,10 @@
         <v>1</v>
       </c>
       <c r="N393" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="O393" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="394" spans="1:15" x14ac:dyDescent="0.2">
@@ -16623,10 +16620,10 @@
         <v>1</v>
       </c>
       <c r="N394" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="O394" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="395" spans="1:15" x14ac:dyDescent="0.2">
@@ -16661,10 +16658,10 @@
         <v>23</v>
       </c>
       <c r="N395" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="O395" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="396" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>